<commit_message>
US01 - Date verification
Created date validation module and completed US01. Updated file verification to check label level. Updated team report
</commit_message>
<xml_diff>
--- a/TeamDReport copy.xlsx
+++ b/TeamDReport copy.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10123"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sasto\Desktop\SchoolWork\555\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/JP/OneDrive/Jonathan's Folder!/Stevens/CS_555_Aglie_Methods_for_SW_Development/Project_Documents/SSW555-DriverlessCar/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B7A87BE5-4776-4F20-B5F6-9DC40B14728A}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD83C6C1-7AAF-5B40-9CEC-D5ADA090C246}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17985" windowHeight="5693" tabRatio="500" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="14400" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Team" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="366" uniqueCount="212">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="370" uniqueCount="213">
   <si>
     <t>Date</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -707,6 +707,9 @@
   </si>
   <si>
     <t xml:space="preserve">We were a little confused at how the roles needed to be split up for each sprint. Once we got help from the professor it was clear. </t>
+  </si>
+  <si>
+    <t>in progress</t>
   </si>
 </sst>
 </file>
@@ -1022,7 +1025,7 @@
             <c:numRef>
               <c:f>'Burndown README'!$B$15:$B$20</c:f>
               <c:numCache>
-                <c:formatCode>m/d/yyyy</c:formatCode>
+                <c:formatCode>m/d/yy</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
                   <c:v>41065</c:v>
@@ -1093,7 +1096,7 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:numFmt formatCode="m/d/yyyy" sourceLinked="1"/>
+        <c:numFmt formatCode="m/d/yy" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -2080,15 +2083,15 @@
       <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.8203125" defaultRowHeight="12.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="7.8203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.64453125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.46875" customWidth="1"/>
-    <col min="4" max="5" width="20.46875" customWidth="1"/>
+    <col min="1" max="1" width="7.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.5" customWidth="1"/>
+    <col min="4" max="5" width="20.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A1" s="4" t="s">
         <v>19</v>
       </c>
@@ -2105,7 +2108,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="2" spans="1:5" s="17" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" s="17" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A2" s="17" t="s">
         <v>183</v>
       </c>
@@ -2122,7 +2125,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
         <v>182</v>
       </c>
@@ -2139,7 +2142,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A4" s="17" t="s">
         <v>187</v>
       </c>
@@ -2156,7 +2159,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A5" s="17" t="s">
         <v>195</v>
       </c>
@@ -2173,7 +2176,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.15">
       <c r="D10" s="4" t="s">
         <v>31</v>
       </c>
@@ -2182,7 +2185,7 @@
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A4:D6">
+  <sortState ref="A4:D6">
     <sortCondition ref="C4:C6"/>
   </sortState>
   <phoneticPr fontId="2" type="noConversion"/>
@@ -2202,21 +2205,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E33"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScale="150" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6:B7"/>
+    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.8203125" defaultRowHeight="12.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="6.8203125" style="20" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="29.17578125" style="20" customWidth="1"/>
-    <col min="3" max="3" width="34.46875" style="20" customWidth="1"/>
-    <col min="4" max="4" width="6.64453125" style="20" customWidth="1"/>
-    <col min="5" max="5" width="7.64453125" style="20" customWidth="1"/>
-    <col min="6" max="16384" width="10.8203125" style="20"/>
+    <col min="1" max="1" width="6.83203125" style="20" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="29.1640625" style="20" customWidth="1"/>
+    <col min="3" max="3" width="34.5" style="20" customWidth="1"/>
+    <col min="4" max="4" width="6.6640625" style="20" customWidth="1"/>
+    <col min="5" max="5" width="10.33203125" style="20" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="10.83203125" style="20"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="19" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" s="19" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A1" s="19" t="s">
         <v>29</v>
       </c>
@@ -2233,7 +2236,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="30" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" ht="34" x14ac:dyDescent="0.15">
       <c r="A2" s="20" t="s">
         <v>109</v>
       </c>
@@ -2246,8 +2249,11 @@
       <c r="D2" s="20" t="s">
         <v>195</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" ht="30" x14ac:dyDescent="0.3">
+      <c r="E2" s="20" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="34" x14ac:dyDescent="0.15">
       <c r="A3" s="20" t="s">
         <v>110</v>
       </c>
@@ -2260,8 +2266,11 @@
       <c r="D3" s="20" t="s">
         <v>195</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" ht="30" x14ac:dyDescent="0.3">
+      <c r="E3" s="20" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="34" x14ac:dyDescent="0.15">
       <c r="A4" s="20" t="s">
         <v>111</v>
       </c>
@@ -2275,7 +2284,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="45" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" ht="51" x14ac:dyDescent="0.15">
       <c r="A5" s="20" t="s">
         <v>112</v>
       </c>
@@ -2289,7 +2298,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="30" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" ht="34" x14ac:dyDescent="0.15">
       <c r="A6" s="20" t="s">
         <v>113</v>
       </c>
@@ -2299,8 +2308,11 @@
       <c r="C6" s="21" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" ht="30" x14ac:dyDescent="0.3">
+      <c r="D6" s="20" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="34" x14ac:dyDescent="0.15">
       <c r="A7" s="20" t="s">
         <v>114</v>
       </c>
@@ -2310,8 +2322,11 @@
       <c r="C7" s="21" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" ht="60" x14ac:dyDescent="0.3">
+      <c r="D7" s="20" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="68" x14ac:dyDescent="0.15">
       <c r="A8" s="20" t="s">
         <v>115</v>
       </c>
@@ -2322,7 +2337,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="45" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" ht="51" x14ac:dyDescent="0.15">
       <c r="A9" s="20" t="s">
         <v>116</v>
       </c>
@@ -2333,7 +2348,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="45" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" ht="51" x14ac:dyDescent="0.15">
       <c r="A10" s="20" t="s">
         <v>117</v>
       </c>
@@ -2344,7 +2359,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="45" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" ht="51" x14ac:dyDescent="0.15">
       <c r="A11" s="20" t="s">
         <v>118</v>
       </c>
@@ -2358,7 +2373,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="30" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" ht="34" x14ac:dyDescent="0.15">
       <c r="A12" s="20" t="s">
         <v>119</v>
       </c>
@@ -2372,7 +2387,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="60" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" ht="68" x14ac:dyDescent="0.15">
       <c r="A13" s="20" t="s">
         <v>120</v>
       </c>
@@ -2383,7 +2398,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="75" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" ht="85" x14ac:dyDescent="0.15">
       <c r="A14" s="20" t="s">
         <v>121</v>
       </c>
@@ -2394,7 +2409,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="30" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" ht="34" x14ac:dyDescent="0.15">
       <c r="A15" s="20" t="s">
         <v>122</v>
       </c>
@@ -2405,7 +2420,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="30" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" ht="34" x14ac:dyDescent="0.15">
       <c r="A16" s="20" t="s">
         <v>123</v>
       </c>
@@ -2416,7 +2431,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" ht="34" x14ac:dyDescent="0.15">
       <c r="A17" s="20" t="s">
         <v>124</v>
       </c>
@@ -2427,7 +2442,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3" ht="34" x14ac:dyDescent="0.15">
       <c r="A18" s="20" t="s">
         <v>125</v>
       </c>
@@ -2438,7 +2453,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="15" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:3" ht="17" x14ac:dyDescent="0.15">
       <c r="A19" s="20" t="s">
         <v>126</v>
       </c>
@@ -2449,7 +2464,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:3" ht="34" x14ac:dyDescent="0.15">
       <c r="A20" s="20" t="s">
         <v>127</v>
       </c>
@@ -2460,7 +2475,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:3" ht="34" x14ac:dyDescent="0.15">
       <c r="A21" s="20" t="s">
         <v>128</v>
       </c>
@@ -2471,7 +2486,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:3" ht="34" x14ac:dyDescent="0.15">
       <c r="A22" s="20" t="s">
         <v>130</v>
       </c>
@@ -2482,7 +2497,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="45" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:3" ht="51" x14ac:dyDescent="0.15">
       <c r="A23" s="20" t="s">
         <v>131</v>
       </c>
@@ -2493,7 +2508,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="45" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:3" ht="68" x14ac:dyDescent="0.15">
       <c r="A24" s="20" t="s">
         <v>132</v>
       </c>
@@ -2504,7 +2519,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="45" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:3" ht="51" x14ac:dyDescent="0.15">
       <c r="A25" s="20" t="s">
         <v>133</v>
       </c>
@@ -2515,7 +2530,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:3" ht="34" x14ac:dyDescent="0.15">
       <c r="A26" t="s">
         <v>135</v>
       </c>
@@ -2526,7 +2541,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:3" ht="51" x14ac:dyDescent="0.15">
       <c r="A27" t="s">
         <v>136</v>
       </c>
@@ -2537,7 +2552,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:3" ht="34" x14ac:dyDescent="0.15">
       <c r="A28" t="s">
         <v>137</v>
       </c>
@@ -2548,7 +2563,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:3" ht="34" x14ac:dyDescent="0.15">
       <c r="A29" t="s">
         <v>138</v>
       </c>
@@ -2559,7 +2574,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="30" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:3" ht="51" x14ac:dyDescent="0.15">
       <c r="A30" t="s">
         <v>139</v>
       </c>
@@ -2570,7 +2585,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="31" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:3" ht="34" x14ac:dyDescent="0.15">
       <c r="A31" t="s">
         <v>140</v>
       </c>
@@ -2581,7 +2596,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:3" ht="34" x14ac:dyDescent="0.15">
       <c r="A32" s="20" t="s">
         <v>149</v>
       </c>
@@ -2592,7 +2607,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="33" spans="1:3" ht="45" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:3" ht="51" x14ac:dyDescent="0.15">
       <c r="A33" s="20" t="s">
         <v>150</v>
       </c>
@@ -2618,47 +2633,47 @@
       <selection activeCell="B15" sqref="B15:B19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.8203125" defaultRowHeight="12.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="10.8203125" style="2"/>
-    <col min="2" max="2" width="9.46875" customWidth="1"/>
-    <col min="3" max="3" width="15.8203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.3515625" customWidth="1"/>
-    <col min="5" max="5" width="6.8203125" customWidth="1"/>
-    <col min="6" max="6" width="12.46875" style="7" customWidth="1"/>
+    <col min="1" max="1" width="10.83203125" style="2"/>
+    <col min="2" max="2" width="9.5" customWidth="1"/>
+    <col min="3" max="3" width="15.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.33203125" customWidth="1"/>
+    <col min="5" max="5" width="6.83203125" customWidth="1"/>
+    <col min="6" max="6" width="12.5" style="7" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A1" s="2" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A2" s="2" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A3" s="2" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A5" s="2" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A6" s="2" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A8" s="2" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="14" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A14" s="4" t="s">
         <v>156</v>
       </c>
@@ -2681,7 +2696,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A15" t="s">
         <v>157</v>
       </c>
@@ -2697,7 +2712,7 @@
       <c r="F15" s="12"/>
       <c r="G15" s="7"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A16" t="s">
         <v>158</v>
       </c>
@@ -2722,7 +2737,7 @@
         <v>125.00000000000001</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A17" s="2" t="s">
         <v>159</v>
       </c>
@@ -2747,7 +2762,7 @@
         <v>102.22222222222223</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A18" s="2" t="s">
         <v>160</v>
       </c>
@@ -2772,7 +2787,7 @@
         <v>97.5</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A19" s="2" t="s">
         <v>161</v>
       </c>
@@ -2812,17 +2827,17 @@
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.8203125" defaultRowHeight="12.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="10.8203125" style="2"/>
-    <col min="2" max="2" width="16.64453125" customWidth="1"/>
-    <col min="3" max="3" width="14.46875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.17578125" customWidth="1"/>
-    <col min="5" max="5" width="6.8203125" customWidth="1"/>
-    <col min="6" max="6" width="12.46875" style="7" customWidth="1"/>
+    <col min="1" max="1" width="10.83203125" style="2"/>
+    <col min="2" max="2" width="16.6640625" customWidth="1"/>
+    <col min="3" max="3" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.1640625" customWidth="1"/>
+    <col min="5" max="5" width="6.83203125" customWidth="1"/>
+    <col min="6" max="6" width="12.5" style="7" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -2842,7 +2857,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A2" s="2">
         <v>42044</v>
       </c>
@@ -2850,22 +2865,22 @@
         <v>32</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A3" s="2">
         <v>42058</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A4" s="2">
         <v>42072</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A5" s="2">
         <v>42093</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A6" s="2">
         <v>42107</v>
       </c>
@@ -2882,31 +2897,31 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:Q24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="150" workbookViewId="0">
+    <sheetView zoomScale="150" workbookViewId="0">
       <selection activeCell="B15" sqref="B15:B24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.8203125" defaultRowHeight="12.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="9" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="24.46875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="7.3515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.5" style="1" customWidth="1"/>
+    <col min="3" max="3" width="7.33203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="7" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.46875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.3515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.46875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.3515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.33203125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="11" style="2" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.46875" style="15" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="19.17578125" style="15" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.5" style="15" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="19.1640625" style="15" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="13" style="15" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="1.8203125" style="15" customWidth="1"/>
-    <col min="15" max="15" width="10.17578125" style="15" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="16.46875" style="15" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="10.17578125" style="15" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="1.83203125" style="15" customWidth="1"/>
+    <col min="15" max="15" width="10.1640625" style="15" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="16.5" style="15" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="10.1640625" style="15" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:17" ht="14" x14ac:dyDescent="0.15">
       <c r="A1" s="4" t="s">
         <v>9</v>
       </c>
@@ -2953,7 +2968,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
         <v>109</v>
       </c>
@@ -2976,7 +2991,7 @@
       <c r="P2" s="16"/>
       <c r="Q2" s="16"/>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
         <v>110</v>
       </c>
@@ -2993,7 +3008,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
         <v>111</v>
       </c>
@@ -3010,7 +3025,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
         <v>112</v>
       </c>
@@ -3027,7 +3042,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
         <v>113</v>
       </c>
@@ -3044,7 +3059,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A7" t="s">
         <v>114</v>
       </c>
@@ -3061,7 +3076,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A8" t="s">
         <v>200</v>
       </c>
@@ -3078,7 +3093,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A9" t="s">
         <v>119</v>
       </c>
@@ -3095,7 +3110,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:17" ht="14" x14ac:dyDescent="0.15">
       <c r="A10" t="s">
         <v>201</v>
       </c>
@@ -3109,7 +3124,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:17" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:17" ht="14" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="20" t="s">
         <v>203</v>
       </c>
@@ -3126,7 +3141,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.15">
       <c r="K12" s="16"/>
       <c r="L12" s="16"/>
       <c r="M12" s="16"/>
@@ -3134,43 +3149,43 @@
       <c r="P12" s="16"/>
       <c r="Q12" s="16"/>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:17" ht="14" x14ac:dyDescent="0.15">
       <c r="B15" s="5" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.15">
       <c r="B16" s="23"/>
     </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:2" ht="14" x14ac:dyDescent="0.15">
       <c r="B17" s="24" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="18" spans="2:2" ht="39.4" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:2" ht="48" x14ac:dyDescent="0.15">
       <c r="B18" s="25" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="19" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:2" x14ac:dyDescent="0.15">
       <c r="B19" s="5"/>
     </row>
-    <row r="20" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:2" ht="14" x14ac:dyDescent="0.15">
       <c r="B20" s="24" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="21" spans="2:2" ht="39.4" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:2" ht="48" x14ac:dyDescent="0.15">
       <c r="B21" s="25" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="23" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:2" ht="14" x14ac:dyDescent="0.15">
       <c r="B23" s="24" t="s">
         <v>210</v>
       </c>
     </row>
-    <row r="24" spans="2:2" ht="39.4" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:2" ht="48" x14ac:dyDescent="0.15">
       <c r="B24" s="25" t="s">
         <v>211</v>
       </c>
@@ -3190,9 +3205,9 @@
       <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.8203125" defaultRowHeight="12.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <sheetData>
-    <row r="1" spans="1:9" ht="24.75" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" ht="28" x14ac:dyDescent="0.15">
       <c r="A1" s="4" t="s">
         <v>9</v>
       </c>
@@ -3236,9 +3251,9 @@
       <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.8203125" defaultRowHeight="12.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <sheetData>
-    <row r="1" spans="1:9" ht="24.75" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" ht="28" x14ac:dyDescent="0.15">
       <c r="A1" s="4" t="s">
         <v>3</v>
       </c>
@@ -3281,9 +3296,9 @@
       <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.8203125" defaultRowHeight="12.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <sheetData>
-    <row r="1" spans="1:9" ht="24.75" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" ht="28" x14ac:dyDescent="0.15">
       <c r="A1" s="4" t="s">
         <v>3</v>
       </c>
@@ -3326,13 +3341,13 @@
       <selection activeCell="A21" sqref="A21:C21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.8203125" defaultRowHeight="12.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="2" max="2" width="28.17578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="49.46875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="28.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="49.5" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" s="4" customFormat="1" ht="14" x14ac:dyDescent="0.15">
       <c r="A1" s="4" t="s">
         <v>108</v>
       </c>
@@ -3343,7 +3358,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" ht="34" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
         <v>109</v>
       </c>
@@ -3354,7 +3369,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="15" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" ht="17" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
         <v>110</v>
       </c>
@@ -3365,7 +3380,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="15" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" ht="17" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
         <v>111</v>
       </c>
@@ -3376,7 +3391,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" ht="34" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
         <v>112</v>
       </c>
@@ -3387,7 +3402,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="15" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" ht="17" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
         <v>113</v>
       </c>
@@ -3398,7 +3413,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="15" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" ht="17" x14ac:dyDescent="0.15">
       <c r="A7" t="s">
         <v>114</v>
       </c>
@@ -3409,7 +3424,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="45" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" ht="51" x14ac:dyDescent="0.15">
       <c r="A8" t="s">
         <v>115</v>
       </c>
@@ -3420,7 +3435,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" ht="34" x14ac:dyDescent="0.15">
       <c r="A9" t="s">
         <v>116</v>
       </c>
@@ -3431,7 +3446,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" ht="34" x14ac:dyDescent="0.15">
       <c r="A10" t="s">
         <v>117</v>
       </c>
@@ -3442,7 +3457,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" ht="34" x14ac:dyDescent="0.15">
       <c r="A11" t="s">
         <v>118</v>
       </c>
@@ -3453,7 +3468,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" ht="34" x14ac:dyDescent="0.15">
       <c r="A12" t="s">
         <v>119</v>
       </c>
@@ -3464,7 +3479,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="45" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" ht="51" x14ac:dyDescent="0.15">
       <c r="A13" t="s">
         <v>120</v>
       </c>
@@ -3475,7 +3490,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="60" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" ht="68" x14ac:dyDescent="0.15">
       <c r="A14" t="s">
         <v>121</v>
       </c>
@@ -3486,7 +3501,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" ht="34" x14ac:dyDescent="0.15">
       <c r="A15" t="s">
         <v>122</v>
       </c>
@@ -3497,7 +3512,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="15" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" ht="17" x14ac:dyDescent="0.15">
       <c r="A16" t="s">
         <v>123</v>
       </c>
@@ -3508,7 +3523,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" ht="34" x14ac:dyDescent="0.15">
       <c r="A17" t="s">
         <v>124</v>
       </c>
@@ -3519,7 +3534,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="15" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3" ht="17" x14ac:dyDescent="0.15">
       <c r="A18" t="s">
         <v>125</v>
       </c>
@@ -3530,7 +3545,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="15" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:3" ht="17" x14ac:dyDescent="0.15">
       <c r="A19" t="s">
         <v>126</v>
       </c>
@@ -3541,7 +3556,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="15" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:3" ht="17" x14ac:dyDescent="0.15">
       <c r="A20" t="s">
         <v>127</v>
       </c>
@@ -3552,7 +3567,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:3" ht="34" x14ac:dyDescent="0.15">
       <c r="A21" t="s">
         <v>128</v>
       </c>
@@ -3563,7 +3578,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:3" ht="34" x14ac:dyDescent="0.15">
       <c r="A22" t="s">
         <v>129</v>
       </c>
@@ -3574,7 +3589,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:3" ht="34" x14ac:dyDescent="0.15">
       <c r="A23" t="s">
         <v>130</v>
       </c>
@@ -3585,7 +3600,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:3" ht="34" x14ac:dyDescent="0.15">
       <c r="A24" t="s">
         <v>131</v>
       </c>
@@ -3596,7 +3611,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="45" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:3" ht="51" x14ac:dyDescent="0.15">
       <c r="A25" t="s">
         <v>132</v>
       </c>
@@ -3607,7 +3622,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:3" ht="34" x14ac:dyDescent="0.15">
       <c r="A26" t="s">
         <v>133</v>
       </c>
@@ -3618,7 +3633,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="105" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:3" ht="136" x14ac:dyDescent="0.15">
       <c r="A27" t="s">
         <v>134</v>
       </c>
@@ -3629,7 +3644,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="15" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:3" ht="17" x14ac:dyDescent="0.15">
       <c r="A28" t="s">
         <v>135</v>
       </c>
@@ -3640,7 +3655,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:3" ht="34" x14ac:dyDescent="0.15">
       <c r="A29" t="s">
         <v>136</v>
       </c>
@@ -3651,7 +3666,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="30" spans="1:3" ht="15" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:3" ht="17" x14ac:dyDescent="0.15">
       <c r="A30" t="s">
         <v>137</v>
       </c>
@@ -3662,7 +3677,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="31" spans="1:3" ht="15" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:3" ht="17" x14ac:dyDescent="0.15">
       <c r="A31" t="s">
         <v>138</v>
       </c>
@@ -3673,7 +3688,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:3" ht="34" x14ac:dyDescent="0.15">
       <c r="A32" t="s">
         <v>139</v>
       </c>
@@ -3684,7 +3699,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="33" spans="1:3" ht="15" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:3" ht="17" x14ac:dyDescent="0.15">
       <c r="A33" t="s">
         <v>140</v>
       </c>
@@ -3695,7 +3710,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="34" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:3" ht="34" x14ac:dyDescent="0.15">
       <c r="A34" t="s">
         <v>141</v>
       </c>
@@ -3706,7 +3721,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="35" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:3" ht="51" x14ac:dyDescent="0.15">
       <c r="A35" t="s">
         <v>142</v>
       </c>
@@ -3717,7 +3732,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="36" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:3" ht="34" x14ac:dyDescent="0.15">
       <c r="A36" t="s">
         <v>143</v>
       </c>
@@ -3728,7 +3743,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="37" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:3" ht="34" x14ac:dyDescent="0.15">
       <c r="A37" t="s">
         <v>144</v>
       </c>
@@ -3739,7 +3754,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="38" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:3" ht="34" x14ac:dyDescent="0.15">
       <c r="A38" t="s">
         <v>145</v>
       </c>
@@ -3750,7 +3765,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="39" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:3" ht="34" x14ac:dyDescent="0.15">
       <c r="A39" t="s">
         <v>146</v>
       </c>
@@ -3761,7 +3776,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="40" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:3" ht="34" x14ac:dyDescent="0.15">
       <c r="A40" t="s">
         <v>147</v>
       </c>
@@ -3772,7 +3787,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="41" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:3" ht="34" x14ac:dyDescent="0.15">
       <c r="A41" t="s">
         <v>148</v>
       </c>
@@ -3783,7 +3798,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="42" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:3" ht="34" x14ac:dyDescent="0.15">
       <c r="A42" t="s">
         <v>149</v>
       </c>
@@ -3794,7 +3809,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="43" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:3" ht="34" x14ac:dyDescent="0.15">
       <c r="A43" t="s">
         <v>150</v>
       </c>

</xml_diff>

<commit_message>
update the US03 and US04's detail in TeamDReport
</commit_message>
<xml_diff>
--- a/TeamDReport copy.xlsx
+++ b/TeamDReport copy.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10123"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/JP/OneDrive/Jonathan's Folder!/Stevens/CS_555_Agile_Methods_for_SW_Development/Project_Documents/SSW555-DriverlessCar/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/franklin/SSW555/SSW555-DriverlessCar/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7D52371-C8EA-014D-A9B7-6D5F9023C8B8}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88F2F48E-A0EE-0E47-A6FF-6ADA6DE137E8}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="14400" tabRatio="500" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="23040" windowHeight="14400" tabRatio="500" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Team" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="378" uniqueCount="220">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="386" uniqueCount="224">
   <si>
     <t>Date</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -731,6 +731,18 @@
   </si>
   <si>
     <t>test_validateMarraigeDate</t>
+  </si>
+  <si>
+    <t>validate_birth_before_death</t>
+  </si>
+  <si>
+    <t>validate_marraige_before_divorce</t>
+  </si>
+  <si>
+    <t>test_validate_birth_before_death_XXX</t>
+  </si>
+  <si>
+    <t>test_validate_marraige_before_divorce_XXX</t>
   </si>
 </sst>
 </file>
@@ -880,7 +892,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -936,6 +948,12 @@
     </xf>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="66">
@@ -2918,8 +2936,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:Q24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="150" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="150" workbookViewId="0">
+      <selection activeCell="O12" sqref="O12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -3077,7 +3095,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:17" ht="28" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
         <v>111</v>
       </c>
@@ -3093,8 +3111,32 @@
       <c r="F4">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.15">
+      <c r="G4">
+        <v>15</v>
+      </c>
+      <c r="I4" s="2">
+        <v>42047</v>
+      </c>
+      <c r="K4" s="16" t="s">
+        <v>214</v>
+      </c>
+      <c r="L4" s="26" t="s">
+        <v>220</v>
+      </c>
+      <c r="M4" s="15">
+        <v>15</v>
+      </c>
+      <c r="O4" s="16" t="s">
+        <v>217</v>
+      </c>
+      <c r="P4" s="26" t="s">
+        <v>222</v>
+      </c>
+      <c r="Q4" s="15">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" ht="28" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
         <v>112</v>
       </c>
@@ -3109,6 +3151,30 @@
       </c>
       <c r="F5">
         <v>1</v>
+      </c>
+      <c r="G5">
+        <v>14</v>
+      </c>
+      <c r="I5" s="2">
+        <v>42047</v>
+      </c>
+      <c r="K5" s="16" t="s">
+        <v>214</v>
+      </c>
+      <c r="L5" s="27" t="s">
+        <v>221</v>
+      </c>
+      <c r="M5" s="15">
+        <v>14</v>
+      </c>
+      <c r="O5" s="16" t="s">
+        <v>217</v>
+      </c>
+      <c r="P5" s="26" t="s">
+        <v>223</v>
+      </c>
+      <c r="Q5" s="15">
+        <v>20</v>
       </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.15">

</xml_diff>

<commit_message>
US 12 & US 09 with tests
</commit_message>
<xml_diff>
--- a/TeamDReport copy.xlsx
+++ b/TeamDReport copy.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10709"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21425"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/michaelramos/SSW555-DriverlessCar/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sasto\Documents\GitHub\SSW555-DriverlessCar\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA7A9759-E8C7-0D46-9E52-DA9435E942CC}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{D9318E2F-C1F2-44CC-B778-2FBB8F252DD5}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="23040" windowHeight="14400" tabRatio="500" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1380" yWindow="1380" windowWidth="18000" windowHeight="9398" tabRatio="500" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Team" sheetId="1" r:id="rId1"/>
@@ -23,20 +23,23 @@
     <sheet name="Sprint4" sheetId="6" r:id="rId8"/>
     <sheet name="Stories" sheetId="11" r:id="rId9"/>
   </sheets>
-  <calcPr calcId="179021"/>
+  <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="330"/>
     </ext>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="476" uniqueCount="245">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="486" uniqueCount="253">
   <si>
     <t>Date</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -804,6 +807,30 @@
   </si>
   <si>
     <t>test_valid_sibling_spacing_XXX</t>
+  </si>
+  <si>
+    <t>ParentsNotTooOld.py</t>
+  </si>
+  <si>
+    <t>parents_too_old</t>
+  </si>
+  <si>
+    <t>BirthBeforeDEath.py</t>
+  </si>
+  <si>
+    <t>birth_before_death</t>
+  </si>
+  <si>
+    <t>TestBirthBeforeDeath.py</t>
+  </si>
+  <si>
+    <t>TestParentsTooOld.py</t>
+  </si>
+  <si>
+    <t>test_parents_not_too_old</t>
+  </si>
+  <si>
+    <t>test_birth_before_death</t>
   </si>
 </sst>
 </file>
@@ -1161,7 +1188,7 @@
             <c:numRef>
               <c:f>'Burndown README'!$B$15:$B$20</c:f>
               <c:numCache>
-                <c:formatCode>m/d/yy</c:formatCode>
+                <c:formatCode>m/d/yyyy</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
                   <c:v>41065</c:v>
@@ -1232,7 +1259,7 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:numFmt formatCode="m/d/yy" sourceLinked="1"/>
+        <c:numFmt formatCode="m/d/yyyy" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -2222,15 +2249,15 @@
       <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="10.8203125" defaultRowHeight="12.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="7.83203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.5" customWidth="1"/>
-    <col min="4" max="5" width="20.5" customWidth="1"/>
+    <col min="1" max="1" width="7.8203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.64453125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.46875" customWidth="1"/>
+    <col min="4" max="5" width="20.46875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>19</v>
       </c>
@@ -2247,7 +2274,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="2" spans="1:5" s="13" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:5" s="13" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="13" t="s">
         <v>183</v>
       </c>
@@ -2264,7 +2291,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>182</v>
       </c>
@@ -2281,7 +2308,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="13" t="s">
         <v>187</v>
       </c>
@@ -2298,7 +2325,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="13" t="s">
         <v>195</v>
       </c>
@@ -2315,7 +2342,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="D10" s="4" t="s">
         <v>31</v>
       </c>
@@ -2344,21 +2371,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E33"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+    <sheetView topLeftCell="A9" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="10.8203125" defaultRowHeight="12.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="6.83203125" style="16" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="29.1640625" style="16" customWidth="1"/>
-    <col min="3" max="3" width="34.5" style="16" customWidth="1"/>
-    <col min="4" max="4" width="6.6640625" style="16" customWidth="1"/>
-    <col min="5" max="5" width="10.33203125" style="16" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="10.83203125" style="16"/>
+    <col min="1" max="1" width="6.8203125" style="16" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="29.17578125" style="16" customWidth="1"/>
+    <col min="3" max="3" width="34.46875" style="16" customWidth="1"/>
+    <col min="4" max="4" width="6.64453125" style="16" customWidth="1"/>
+    <col min="5" max="5" width="10.3515625" style="16" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="10.8203125" style="16"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="15" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:5" s="15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="15" t="s">
         <v>29</v>
       </c>
@@ -2375,7 +2402,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="32" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:5" ht="30" x14ac:dyDescent="0.3">
       <c r="A2" s="16" t="s">
         <v>109</v>
       </c>
@@ -2392,7 +2419,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="32" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:5" ht="30" x14ac:dyDescent="0.3">
       <c r="A3" s="16" t="s">
         <v>110</v>
       </c>
@@ -2409,7 +2436,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="32" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:5" ht="30" x14ac:dyDescent="0.3">
       <c r="A4" s="16" t="s">
         <v>111</v>
       </c>
@@ -2426,7 +2453,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="48" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:5" ht="45" x14ac:dyDescent="0.3">
       <c r="A5" s="16" t="s">
         <v>112</v>
       </c>
@@ -2443,7 +2470,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="32" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:5" ht="30" x14ac:dyDescent="0.3">
       <c r="A6" s="16" t="s">
         <v>113</v>
       </c>
@@ -2460,7 +2487,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="32" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:5" ht="30" x14ac:dyDescent="0.3">
       <c r="A7" s="16" t="s">
         <v>114</v>
       </c>
@@ -2477,7 +2504,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="64" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:5" ht="60" x14ac:dyDescent="0.3">
       <c r="A8" s="16" t="s">
         <v>115</v>
       </c>
@@ -2494,7 +2521,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="48" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:5" ht="45" x14ac:dyDescent="0.3">
       <c r="A9" s="16" t="s">
         <v>116</v>
       </c>
@@ -2511,7 +2538,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="48" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:5" ht="45" x14ac:dyDescent="0.3">
       <c r="A10" s="16" t="s">
         <v>117</v>
       </c>
@@ -2525,10 +2552,10 @@
         <v>187</v>
       </c>
       <c r="E10" s="16" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" ht="48" x14ac:dyDescent="0.15">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="45" x14ac:dyDescent="0.3">
       <c r="A11" s="16" t="s">
         <v>118</v>
       </c>
@@ -2545,7 +2572,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="32" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:5" ht="30" x14ac:dyDescent="0.3">
       <c r="A12" s="16" t="s">
         <v>119</v>
       </c>
@@ -2562,7 +2589,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="64" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:5" ht="60" x14ac:dyDescent="0.3">
       <c r="A13" s="16" t="s">
         <v>120</v>
       </c>
@@ -2576,10 +2603,10 @@
         <v>187</v>
       </c>
       <c r="E13" s="16" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" ht="80" x14ac:dyDescent="0.15">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="75" x14ac:dyDescent="0.3">
       <c r="A14" s="16" t="s">
         <v>121</v>
       </c>
@@ -2596,7 +2623,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="32" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:5" ht="30" x14ac:dyDescent="0.3">
       <c r="A15" s="16" t="s">
         <v>122</v>
       </c>
@@ -2613,7 +2640,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="32" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:5" ht="30" x14ac:dyDescent="0.3">
       <c r="A16" s="16" t="s">
         <v>123</v>
       </c>
@@ -2624,7 +2651,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="32" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:5" ht="30" x14ac:dyDescent="0.3">
       <c r="A17" s="16" t="s">
         <v>124</v>
       </c>
@@ -2635,7 +2662,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="32" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:5" ht="30" x14ac:dyDescent="0.3">
       <c r="A18" s="16" t="s">
         <v>125</v>
       </c>
@@ -2646,7 +2673,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="32" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:5" ht="15" x14ac:dyDescent="0.3">
       <c r="A19" s="16" t="s">
         <v>126</v>
       </c>
@@ -2657,7 +2684,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="32" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:5" ht="30" x14ac:dyDescent="0.3">
       <c r="A20" s="16" t="s">
         <v>127</v>
       </c>
@@ -2668,7 +2695,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="32" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:5" ht="30" x14ac:dyDescent="0.3">
       <c r="A21" s="16" t="s">
         <v>128</v>
       </c>
@@ -2679,7 +2706,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="22" spans="1:5" ht="32" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:5" ht="30" x14ac:dyDescent="0.3">
       <c r="A22" s="16" t="s">
         <v>130</v>
       </c>
@@ -2690,7 +2717,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="23" spans="1:5" ht="48" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:5" ht="45" x14ac:dyDescent="0.3">
       <c r="A23" s="16" t="s">
         <v>131</v>
       </c>
@@ -2701,7 +2728,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="24" spans="1:5" ht="64" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:5" ht="45" x14ac:dyDescent="0.3">
       <c r="A24" s="16" t="s">
         <v>132</v>
       </c>
@@ -2712,7 +2739,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="25" spans="1:5" ht="48" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:5" ht="45" x14ac:dyDescent="0.3">
       <c r="A25" s="16" t="s">
         <v>133</v>
       </c>
@@ -2723,7 +2750,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="26" spans="1:5" ht="32" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:5" ht="30" x14ac:dyDescent="0.3">
       <c r="A26" s="16" t="s">
         <v>135</v>
       </c>
@@ -2734,7 +2761,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="27" spans="1:5" ht="32" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:5" ht="30" x14ac:dyDescent="0.3">
       <c r="A27" s="16" t="s">
         <v>136</v>
       </c>
@@ -2745,7 +2772,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="28" spans="1:5" ht="32" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:5" ht="30" x14ac:dyDescent="0.3">
       <c r="A28" s="16" t="s">
         <v>137</v>
       </c>
@@ -2756,7 +2783,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="29" spans="1:5" ht="32" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:5" ht="30" x14ac:dyDescent="0.3">
       <c r="A29" s="16" t="s">
         <v>138</v>
       </c>
@@ -2767,7 +2794,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="30" spans="1:5" ht="32" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:5" ht="30" x14ac:dyDescent="0.3">
       <c r="A30" s="16" t="s">
         <v>139</v>
       </c>
@@ -2778,7 +2805,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="31" spans="1:5" ht="32" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:5" ht="15" x14ac:dyDescent="0.3">
       <c r="A31" s="16" t="s">
         <v>140</v>
       </c>
@@ -2789,7 +2816,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="32" spans="1:5" ht="32" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:5" ht="30" x14ac:dyDescent="0.3">
       <c r="A32" s="16" t="s">
         <v>149</v>
       </c>
@@ -2806,7 +2833,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="33" spans="1:5" ht="48" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:5" ht="45" x14ac:dyDescent="0.3">
       <c r="A33" s="16" t="s">
         <v>150</v>
       </c>
@@ -2838,47 +2865,47 @@
       <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="10.8203125" defaultRowHeight="12.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.83203125" style="2"/>
-    <col min="2" max="2" width="9.5" customWidth="1"/>
-    <col min="3" max="3" width="15.83203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.33203125" customWidth="1"/>
-    <col min="5" max="5" width="6.83203125" customWidth="1"/>
-    <col min="6" max="6" width="12.5" style="7" customWidth="1"/>
+    <col min="1" max="1" width="10.8203125" style="2"/>
+    <col min="2" max="2" width="9.46875" customWidth="1"/>
+    <col min="3" max="3" width="15.8203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.3515625" customWidth="1"/>
+    <col min="5" max="5" width="6.8203125" customWidth="1"/>
+    <col min="6" max="6" width="12.46875" style="7" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="14" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A14" s="4" t="s">
         <v>156</v>
       </c>
@@ -2901,7 +2928,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>157</v>
       </c>
@@ -2917,7 +2944,7 @@
       <c r="F15" s="11"/>
       <c r="G15" s="7"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>158</v>
       </c>
@@ -2942,7 +2969,7 @@
         <v>125.00000000000001</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
         <v>159</v>
       </c>
@@ -2967,7 +2994,7 @@
         <v>102.22222222222223</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
         <v>160</v>
       </c>
@@ -2992,7 +3019,7 @@
         <v>97.5</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
         <v>161</v>
       </c>
@@ -3032,17 +3059,17 @@
       <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="10.8203125" defaultRowHeight="12.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.83203125" style="2"/>
-    <col min="2" max="2" width="16.6640625" customWidth="1"/>
-    <col min="3" max="3" width="14.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.1640625" customWidth="1"/>
-    <col min="5" max="5" width="6.83203125" customWidth="1"/>
-    <col min="6" max="6" width="12.5" style="7" customWidth="1"/>
+    <col min="1" max="1" width="10.8203125" style="2"/>
+    <col min="2" max="2" width="16.64453125" customWidth="1"/>
+    <col min="3" max="3" width="14.46875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.17578125" customWidth="1"/>
+    <col min="5" max="5" width="6.8203125" customWidth="1"/>
+    <col min="6" max="6" width="12.46875" style="7" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -3062,7 +3089,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="2">
         <v>42044</v>
       </c>
@@ -3073,7 +3100,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
         <v>42058</v>
       </c>
@@ -3095,17 +3122,17 @@
         <v>0.73643410852713176</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="2">
         <v>42072</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="2">
         <v>42093</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="2">
         <v>42107</v>
       </c>
@@ -3126,28 +3153,28 @@
       <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="10.8203125" defaultRowHeight="12.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="9" style="16" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="24.5" style="18" customWidth="1"/>
-    <col min="3" max="3" width="7.33203125" style="16" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.6640625" style="16" customWidth="1"/>
-    <col min="5" max="5" width="8.5" style="16" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.33203125" style="16" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.6640625" style="16" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.33203125" style="16" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.46875" style="18" customWidth="1"/>
+    <col min="3" max="3" width="7.3515625" style="16" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.64453125" style="16" customWidth="1"/>
+    <col min="5" max="5" width="8.46875" style="16" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.3515625" style="16" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.64453125" style="16" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.3515625" style="16" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="11" style="26" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="20.83203125" style="29" customWidth="1"/>
-    <col min="11" max="11" width="17.83203125" style="29" customWidth="1"/>
+    <col min="10" max="10" width="20.8203125" style="29" customWidth="1"/>
+    <col min="11" max="11" width="17.8203125" style="29" customWidth="1"/>
     <col min="12" max="12" width="13" style="24" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="1.83203125" style="24" customWidth="1"/>
-    <col min="14" max="14" width="16.83203125" style="29" customWidth="1"/>
-    <col min="15" max="15" width="22.83203125" style="29" customWidth="1"/>
-    <col min="16" max="16" width="10.1640625" style="24" bestFit="1" customWidth="1"/>
-    <col min="17" max="16384" width="10.83203125" style="16"/>
+    <col min="13" max="13" width="1.8203125" style="24" customWidth="1"/>
+    <col min="14" max="14" width="16.8203125" style="29" customWidth="1"/>
+    <col min="15" max="15" width="22.8203125" style="29" customWidth="1"/>
+    <col min="16" max="16" width="10.17578125" style="24" bestFit="1" customWidth="1"/>
+    <col min="17" max="16384" width="10.8203125" style="16"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A1" s="15" t="s">
         <v>9</v>
       </c>
@@ -3194,7 +3221,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="2" spans="1:16" ht="26" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:16" ht="24.75" x14ac:dyDescent="0.3">
       <c r="A2" s="16" t="s">
         <v>109</v>
       </c>
@@ -3241,7 +3268,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:16" ht="26" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:16" ht="24.75" x14ac:dyDescent="0.3">
       <c r="A3" s="16" t="s">
         <v>110</v>
       </c>
@@ -3288,7 +3315,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:16" ht="26" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:16" ht="24.75" x14ac:dyDescent="0.3">
       <c r="A4" s="16" t="s">
         <v>111</v>
       </c>
@@ -3335,7 +3362,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="5" spans="1:16" ht="26" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:16" ht="24.75" x14ac:dyDescent="0.3">
       <c r="A5" s="16" t="s">
         <v>112</v>
       </c>
@@ -3382,7 +3409,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="6" spans="1:16" ht="26" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:16" ht="24.75" x14ac:dyDescent="0.3">
       <c r="A6" s="16" t="s">
         <v>113</v>
       </c>
@@ -3429,7 +3456,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:16" ht="26" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:16" ht="24.75" x14ac:dyDescent="0.3">
       <c r="A7" s="16" t="s">
         <v>114</v>
       </c>
@@ -3476,7 +3503,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:16" ht="39" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:16" ht="37.15" x14ac:dyDescent="0.3">
       <c r="A8" s="16" t="s">
         <v>118</v>
       </c>
@@ -3523,7 +3550,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="9" spans="1:16" ht="26" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:16" ht="24.75" x14ac:dyDescent="0.3">
       <c r="A9" s="16" t="s">
         <v>119</v>
       </c>
@@ -3570,7 +3597,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
       <c r="J10" s="28"/>
       <c r="K10" s="28"/>
       <c r="L10" s="27"/>
@@ -3578,43 +3605,43 @@
       <c r="O10" s="28"/>
       <c r="P10" s="27"/>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B13" s="20" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B14" s="30"/>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B15" s="31" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="16" spans="1:16" ht="22" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:16" ht="19.5" x14ac:dyDescent="0.3">
       <c r="B16" s="32" t="s">
         <v>230</v>
       </c>
     </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.15">
+    <row r="17" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B17" s="20"/>
     </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.15">
+    <row r="18" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B18" s="31" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="19" spans="2:2" ht="66" x14ac:dyDescent="0.15">
+    <row r="19" spans="2:2" ht="58.5" x14ac:dyDescent="0.3">
       <c r="B19" s="32" t="s">
         <v>229</v>
       </c>
     </row>
-    <row r="21" spans="2:2" x14ac:dyDescent="0.15">
+    <row r="21" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B21" s="31" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="22" spans="2:2" x14ac:dyDescent="0.15">
+    <row r="22" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B22" s="32" t="s">
         <v>231</v>
       </c>
@@ -3631,24 +3658,24 @@
   <dimension ref="A1:P20"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
-      <selection activeCell="P7" sqref="P7"/>
+      <selection activeCell="P5" sqref="P5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="10.8203125" defaultRowHeight="12.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.83203125" style="33"/>
+    <col min="1" max="1" width="10.8203125" style="33"/>
     <col min="2" max="2" width="22" style="33" bestFit="1" customWidth="1"/>
-    <col min="3" max="9" width="10.83203125" style="33"/>
-    <col min="10" max="10" width="13.83203125" style="33" customWidth="1"/>
+    <col min="3" max="9" width="10.8203125" style="33"/>
+    <col min="10" max="10" width="13.8203125" style="33" customWidth="1"/>
     <col min="11" max="11" width="16" style="33" customWidth="1"/>
-    <col min="12" max="12" width="15.83203125" style="33" customWidth="1"/>
-    <col min="13" max="13" width="4.1640625" style="33" customWidth="1"/>
-    <col min="14" max="14" width="10.83203125" style="33" customWidth="1"/>
-    <col min="15" max="15" width="15.33203125" style="33" customWidth="1"/>
-    <col min="16" max="16384" width="10.83203125" style="33"/>
+    <col min="12" max="12" width="15.8203125" style="33" customWidth="1"/>
+    <col min="13" max="13" width="4.17578125" style="33" customWidth="1"/>
+    <col min="14" max="14" width="10.8203125" style="33" customWidth="1"/>
+    <col min="15" max="15" width="15.3515625" style="33" customWidth="1"/>
+    <col min="16" max="16384" width="10.8203125" style="33"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="34" t="s">
         <v>9</v>
       </c>
@@ -3696,7 +3723,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="2" spans="1:16" s="37" customFormat="1" ht="39" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:16" s="37" customFormat="1" ht="37.15" x14ac:dyDescent="0.3">
       <c r="A2" s="37" t="s">
         <v>115</v>
       </c>
@@ -3716,7 +3743,7 @@
       <c r="H2" s="36"/>
       <c r="I2" s="36"/>
     </row>
-    <row r="3" spans="1:16" s="37" customFormat="1" ht="39" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:16" s="37" customFormat="1" ht="37.15" x14ac:dyDescent="0.3">
       <c r="A3" s="37" t="s">
         <v>116</v>
       </c>
@@ -3736,7 +3763,7 @@
       <c r="H3" s="36"/>
       <c r="I3" s="36"/>
     </row>
-    <row r="4" spans="1:16" s="37" customFormat="1" ht="26" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:16" s="37" customFormat="1" ht="24.75" x14ac:dyDescent="0.3">
       <c r="A4" s="37" t="s">
         <v>117</v>
       </c>
@@ -3746,17 +3773,44 @@
       <c r="C4" s="37" t="s">
         <v>187</v>
       </c>
+      <c r="D4" s="37" t="s">
+        <v>228</v>
+      </c>
       <c r="E4" s="37">
         <v>25</v>
       </c>
       <c r="F4" s="37">
         <v>1</v>
       </c>
-      <c r="G4" s="36"/>
-      <c r="H4" s="36"/>
-      <c r="I4" s="36"/>
-    </row>
-    <row r="5" spans="1:16" s="37" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="G4" s="36">
+        <v>40</v>
+      </c>
+      <c r="H4" s="36">
+        <v>2</v>
+      </c>
+      <c r="I4" s="39">
+        <v>42078</v>
+      </c>
+      <c r="J4" s="37" t="s">
+        <v>247</v>
+      </c>
+      <c r="K4" s="37" t="s">
+        <v>248</v>
+      </c>
+      <c r="L4" s="37">
+        <v>31</v>
+      </c>
+      <c r="N4" s="37" t="s">
+        <v>249</v>
+      </c>
+      <c r="O4" s="37" t="s">
+        <v>252</v>
+      </c>
+      <c r="P4" s="37">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" s="37" customFormat="1" ht="24.75" x14ac:dyDescent="0.3">
       <c r="A5" s="37" t="s">
         <v>120</v>
       </c>
@@ -3766,17 +3820,44 @@
       <c r="C5" s="37" t="s">
         <v>187</v>
       </c>
+      <c r="D5" s="37" t="s">
+        <v>228</v>
+      </c>
       <c r="E5" s="37">
         <v>25</v>
       </c>
       <c r="F5" s="37">
         <v>1</v>
       </c>
-      <c r="G5" s="36"/>
-      <c r="H5" s="36"/>
-      <c r="I5" s="36"/>
-    </row>
-    <row r="6" spans="1:16" s="37" customFormat="1" ht="26" x14ac:dyDescent="0.15">
+      <c r="G5" s="36">
+        <v>30</v>
+      </c>
+      <c r="H5" s="36">
+        <v>1</v>
+      </c>
+      <c r="I5" s="39">
+        <v>42078</v>
+      </c>
+      <c r="J5" s="37" t="s">
+        <v>245</v>
+      </c>
+      <c r="K5" s="37" t="s">
+        <v>246</v>
+      </c>
+      <c r="L5" s="37">
+        <v>26</v>
+      </c>
+      <c r="N5" s="37" t="s">
+        <v>250</v>
+      </c>
+      <c r="O5" s="37" t="s">
+        <v>251</v>
+      </c>
+      <c r="P5" s="37">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" s="37" customFormat="1" ht="24.75" x14ac:dyDescent="0.3">
       <c r="A6" s="37" t="s">
         <v>121</v>
       </c>
@@ -3823,7 +3904,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:16" s="37" customFormat="1" ht="39" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:16" s="37" customFormat="1" ht="24.75" x14ac:dyDescent="0.3">
       <c r="A7" s="37" t="s">
         <v>122</v>
       </c>
@@ -3870,7 +3951,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="8" spans="1:16" s="37" customFormat="1" ht="26" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:16" s="37" customFormat="1" ht="24.75" x14ac:dyDescent="0.3">
       <c r="A8" s="37" t="s">
         <v>149</v>
       </c>
@@ -3917,7 +3998,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:16" s="37" customFormat="1" ht="26" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:16" s="37" customFormat="1" ht="24.75" x14ac:dyDescent="0.3">
       <c r="A9" s="37" t="s">
         <v>150</v>
       </c>
@@ -3964,17 +4045,17 @@
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:16" s="37" customFormat="1" x14ac:dyDescent="0.15"/>
-    <row r="11" spans="1:16" s="37" customFormat="1" x14ac:dyDescent="0.15"/>
-    <row r="12" spans="1:16" s="37" customFormat="1" x14ac:dyDescent="0.15"/>
-    <row r="13" spans="1:16" s="37" customFormat="1" x14ac:dyDescent="0.15"/>
-    <row r="14" spans="1:16" s="37" customFormat="1" x14ac:dyDescent="0.15"/>
-    <row r="15" spans="1:16" s="37" customFormat="1" x14ac:dyDescent="0.15"/>
-    <row r="16" spans="1:16" s="37" customFormat="1" x14ac:dyDescent="0.15"/>
-    <row r="17" s="37" customFormat="1" x14ac:dyDescent="0.15"/>
-    <row r="18" s="37" customFormat="1" x14ac:dyDescent="0.15"/>
-    <row r="19" s="37" customFormat="1" x14ac:dyDescent="0.15"/>
-    <row r="20" s="37" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="10" spans="1:16" s="37" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="11" spans="1:16" s="37" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="12" spans="1:16" s="37" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="13" spans="1:16" s="37" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="14" spans="1:16" s="37" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="15" spans="1:16" s="37" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="16" spans="1:16" s="37" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="17" s="37" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="18" s="37" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="19" s="37" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="20" s="37" customFormat="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -3990,9 +4071,9 @@
       <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="10.8203125" defaultRowHeight="12.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:9" ht="26" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:9" ht="24.75" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>3</v>
       </c>
@@ -4035,9 +4116,9 @@
       <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="10.8203125" defaultRowHeight="12.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:9" ht="26" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:9" ht="24.75" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>3</v>
       </c>
@@ -4080,13 +4161,13 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="10.8203125" defaultRowHeight="12.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="28.1640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="49.5" style="1" customWidth="1"/>
+    <col min="2" max="2" width="28.17578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="49.46875" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>108</v>
       </c>
@@ -4097,7 +4178,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="32" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:3" ht="30" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>109</v>
       </c>
@@ -4108,7 +4189,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="16" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:3" ht="15" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>110</v>
       </c>
@@ -4119,7 +4200,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="16" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:3" ht="15" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>111</v>
       </c>
@@ -4130,7 +4211,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="32" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:3" ht="30" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>112</v>
       </c>
@@ -4141,7 +4222,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="16" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:3" ht="15" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>113</v>
       </c>
@@ -4152,7 +4233,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="16" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:3" ht="15" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>114</v>
       </c>
@@ -4163,7 +4244,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="48" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:3" ht="45" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>115</v>
       </c>
@@ -4174,7 +4255,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="32" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:3" ht="30" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>116</v>
       </c>
@@ -4185,7 +4266,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="32" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:3" ht="30" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>117</v>
       </c>
@@ -4196,7 +4277,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="32" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:3" ht="30" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>118</v>
       </c>
@@ -4207,7 +4288,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="32" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:3" ht="30" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>119</v>
       </c>
@@ -4218,7 +4299,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="48" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:3" ht="45" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>120</v>
       </c>
@@ -4229,7 +4310,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="64" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:3" ht="60" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>121</v>
       </c>
@@ -4240,7 +4321,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="32" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:3" ht="30" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>122</v>
       </c>
@@ -4251,7 +4332,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="16" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:3" ht="15" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>123</v>
       </c>
@@ -4262,7 +4343,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="32" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:3" ht="30" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>124</v>
       </c>
@@ -4273,7 +4354,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="16" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:3" ht="15" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>125</v>
       </c>
@@ -4284,7 +4365,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="16" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:3" ht="15" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>126</v>
       </c>
@@ -4295,7 +4376,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="16" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:3" ht="15" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>127</v>
       </c>
@@ -4306,7 +4387,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="32" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:3" ht="30" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>128</v>
       </c>
@@ -4317,7 +4398,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="32" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:3" ht="30" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>129</v>
       </c>
@@ -4328,7 +4409,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="32" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:3" ht="30" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>130</v>
       </c>
@@ -4339,7 +4420,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="32" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:3" ht="30" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>131</v>
       </c>
@@ -4350,7 +4431,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="48" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:3" ht="45" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>132</v>
       </c>
@@ -4361,7 +4442,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="32" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:3" ht="30" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>133</v>
       </c>
@@ -4372,7 +4453,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="128" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:3" ht="105" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>134</v>
       </c>
@@ -4383,7 +4464,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="16" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:3" ht="15" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>135</v>
       </c>
@@ -4394,7 +4475,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="32" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:3" ht="30" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>136</v>
       </c>
@@ -4405,7 +4486,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="30" spans="1:3" ht="16" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:3" ht="15" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>137</v>
       </c>
@@ -4416,7 +4497,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="31" spans="1:3" ht="16" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:3" ht="15" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>138</v>
       </c>
@@ -4427,7 +4508,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="32" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:3" ht="30" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>139</v>
       </c>
@@ -4438,7 +4519,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="33" spans="1:3" ht="16" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:3" ht="15" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>140</v>
       </c>
@@ -4449,7 +4530,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="34" spans="1:3" ht="32" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:3" ht="30" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>141</v>
       </c>
@@ -4460,7 +4541,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="35" spans="1:3" ht="48" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:3" ht="30" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>142</v>
       </c>
@@ -4471,7 +4552,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="36" spans="1:3" ht="32" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:3" ht="30" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>143</v>
       </c>
@@ -4482,7 +4563,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="37" spans="1:3" ht="32" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:3" ht="30" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>144</v>
       </c>
@@ -4493,7 +4574,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="38" spans="1:3" ht="32" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:3" ht="30" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>145</v>
       </c>
@@ -4504,7 +4585,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="39" spans="1:3" ht="32" x14ac:dyDescent="0.15">
+    <row r="39" spans="1:3" ht="30" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>146</v>
       </c>
@@ -4515,7 +4596,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="40" spans="1:3" ht="32" x14ac:dyDescent="0.15">
+    <row r="40" spans="1:3" ht="30" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>147</v>
       </c>
@@ -4526,7 +4607,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="41" spans="1:3" ht="32" x14ac:dyDescent="0.15">
+    <row r="41" spans="1:3" ht="30" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>148</v>
       </c>
@@ -4537,7 +4618,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="42" spans="1:3" ht="32" x14ac:dyDescent="0.15">
+    <row r="42" spans="1:3" ht="30" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>149</v>
       </c>
@@ -4548,7 +4629,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="43" spans="1:3" ht="32" x14ac:dyDescent="0.15">
+    <row r="43" spans="1:3" ht="30" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>150</v>
       </c>

</xml_diff>

<commit_message>
added data for US 9 & 12
</commit_message>
<xml_diff>
--- a/TeamDReport copy.xlsx
+++ b/TeamDReport copy.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10709"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sasto\Documents\GitHub\SSW555-DriverlessCar\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/michaelramos/SSW555-DriverlessCar/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A5C89F89-F847-4A3D-8965-414D0628248C}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6A501C0-8A75-B544-AA89-103F1126CA54}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="24196" windowHeight="13096" tabRatio="500" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="24200" windowHeight="13100" tabRatio="500" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Team" sheetId="1" r:id="rId1"/>
@@ -23,15 +23,10 @@
     <sheet name="Sprint4" sheetId="6" r:id="rId8"/>
     <sheet name="Stories" sheetId="11" r:id="rId9"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="179021"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="330"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-      </xcalcf:calcFeatures>
     </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -41,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="494" uniqueCount="261">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="496" uniqueCount="261">
   <si>
     <t>Date</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -1214,7 +1209,7 @@
             <c:numRef>
               <c:f>'Burndown README'!$B$15:$B$20</c:f>
               <c:numCache>
-                <c:formatCode>m/d/yyyy</c:formatCode>
+                <c:formatCode>m/d/yy</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
                   <c:v>41065</c:v>
@@ -1285,7 +1280,7 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:numFmt formatCode="m/d/yyyy" sourceLinked="1"/>
+        <c:numFmt formatCode="m/d/yy" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -2275,15 +2270,15 @@
       <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.8203125" defaultRowHeight="12.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="7.8203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.64453125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.46875" customWidth="1"/>
-    <col min="4" max="5" width="20.46875" customWidth="1"/>
+    <col min="1" max="1" width="7.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.5" customWidth="1"/>
+    <col min="4" max="5" width="20.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A1" s="4" t="s">
         <v>19</v>
       </c>
@@ -2300,7 +2295,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="2" spans="1:5" s="13" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" s="13" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A2" s="13" t="s">
         <v>183</v>
       </c>
@@ -2317,7 +2312,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
         <v>182</v>
       </c>
@@ -2334,7 +2329,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A4" s="13" t="s">
         <v>187</v>
       </c>
@@ -2351,7 +2346,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A5" s="13" t="s">
         <v>195</v>
       </c>
@@ -2368,7 +2363,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.15">
       <c r="D10" s="4" t="s">
         <v>31</v>
       </c>
@@ -2401,17 +2396,17 @@
       <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.8203125" defaultRowHeight="12.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="6.8203125" style="16" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="29.17578125" style="16" customWidth="1"/>
-    <col min="3" max="3" width="34.46875" style="16" customWidth="1"/>
-    <col min="4" max="4" width="6.64453125" style="16" customWidth="1"/>
-    <col min="5" max="5" width="10.3515625" style="16" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="10.8203125" style="16"/>
+    <col min="1" max="1" width="6.83203125" style="16" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="29.1640625" style="16" customWidth="1"/>
+    <col min="3" max="3" width="34.5" style="16" customWidth="1"/>
+    <col min="4" max="4" width="6.6640625" style="16" customWidth="1"/>
+    <col min="5" max="5" width="10.33203125" style="16" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="10.83203125" style="16"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="15" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" s="15" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A1" s="15" t="s">
         <v>29</v>
       </c>
@@ -2428,7 +2423,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="30" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" ht="32" x14ac:dyDescent="0.15">
       <c r="A2" s="16" t="s">
         <v>109</v>
       </c>
@@ -2445,7 +2440,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="30" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" ht="32" x14ac:dyDescent="0.15">
       <c r="A3" s="16" t="s">
         <v>110</v>
       </c>
@@ -2462,7 +2457,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="30" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" ht="32" x14ac:dyDescent="0.15">
       <c r="A4" s="16" t="s">
         <v>111</v>
       </c>
@@ -2479,7 +2474,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="45" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" ht="48" x14ac:dyDescent="0.15">
       <c r="A5" s="16" t="s">
         <v>112</v>
       </c>
@@ -2496,7 +2491,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="30" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" ht="32" x14ac:dyDescent="0.15">
       <c r="A6" s="16" t="s">
         <v>113</v>
       </c>
@@ -2513,7 +2508,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="30" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" ht="32" x14ac:dyDescent="0.15">
       <c r="A7" s="16" t="s">
         <v>114</v>
       </c>
@@ -2530,7 +2525,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="60" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" ht="64" x14ac:dyDescent="0.15">
       <c r="A8" s="16" t="s">
         <v>115</v>
       </c>
@@ -2547,7 +2542,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="45" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" ht="48" x14ac:dyDescent="0.15">
       <c r="A9" s="16" t="s">
         <v>116</v>
       </c>
@@ -2564,7 +2559,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="45" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" ht="48" x14ac:dyDescent="0.15">
       <c r="A10" s="16" t="s">
         <v>117</v>
       </c>
@@ -2581,7 +2576,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="45" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" ht="48" x14ac:dyDescent="0.15">
       <c r="A11" s="16" t="s">
         <v>118</v>
       </c>
@@ -2598,7 +2593,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="30" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" ht="32" x14ac:dyDescent="0.15">
       <c r="A12" s="16" t="s">
         <v>119</v>
       </c>
@@ -2615,7 +2610,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="60" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" ht="64" x14ac:dyDescent="0.15">
       <c r="A13" s="16" t="s">
         <v>120</v>
       </c>
@@ -2632,7 +2627,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="75" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" ht="80" x14ac:dyDescent="0.15">
       <c r="A14" s="16" t="s">
         <v>121</v>
       </c>
@@ -2649,7 +2644,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="30" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" ht="32" x14ac:dyDescent="0.15">
       <c r="A15" s="16" t="s">
         <v>122</v>
       </c>
@@ -2666,7 +2661,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="30" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" ht="32" x14ac:dyDescent="0.15">
       <c r="A16" s="16" t="s">
         <v>123</v>
       </c>
@@ -2677,7 +2672,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="30" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" ht="32" x14ac:dyDescent="0.15">
       <c r="A17" s="16" t="s">
         <v>124</v>
       </c>
@@ -2688,7 +2683,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="30" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" ht="32" x14ac:dyDescent="0.15">
       <c r="A18" s="16" t="s">
         <v>125</v>
       </c>
@@ -2699,7 +2694,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="15" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" ht="16" x14ac:dyDescent="0.15">
       <c r="A19" s="16" t="s">
         <v>126</v>
       </c>
@@ -2710,7 +2705,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="30" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:5" ht="32" x14ac:dyDescent="0.15">
       <c r="A20" s="16" t="s">
         <v>127</v>
       </c>
@@ -2721,7 +2716,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="30" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:5" ht="32" x14ac:dyDescent="0.15">
       <c r="A21" s="16" t="s">
         <v>128</v>
       </c>
@@ -2732,7 +2727,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="22" spans="1:5" ht="30" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:5" ht="32" x14ac:dyDescent="0.15">
       <c r="A22" s="16" t="s">
         <v>130</v>
       </c>
@@ -2743,7 +2738,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="23" spans="1:5" ht="45" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:5" ht="48" x14ac:dyDescent="0.15">
       <c r="A23" s="16" t="s">
         <v>131</v>
       </c>
@@ -2754,7 +2749,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="24" spans="1:5" ht="45" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:5" ht="64" x14ac:dyDescent="0.15">
       <c r="A24" s="16" t="s">
         <v>132</v>
       </c>
@@ -2765,7 +2760,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="25" spans="1:5" ht="45" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:5" ht="48" x14ac:dyDescent="0.15">
       <c r="A25" s="16" t="s">
         <v>133</v>
       </c>
@@ -2776,7 +2771,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="26" spans="1:5" ht="30" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:5" ht="32" x14ac:dyDescent="0.15">
       <c r="A26" s="16" t="s">
         <v>135</v>
       </c>
@@ -2787,7 +2782,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="27" spans="1:5" ht="30" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:5" ht="32" x14ac:dyDescent="0.15">
       <c r="A27" s="16" t="s">
         <v>136</v>
       </c>
@@ -2798,7 +2793,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="28" spans="1:5" ht="30" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:5" ht="32" x14ac:dyDescent="0.15">
       <c r="A28" s="16" t="s">
         <v>137</v>
       </c>
@@ -2809,7 +2804,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="29" spans="1:5" ht="30" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:5" ht="32" x14ac:dyDescent="0.15">
       <c r="A29" s="16" t="s">
         <v>138</v>
       </c>
@@ -2820,7 +2815,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="30" spans="1:5" ht="30" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:5" ht="32" x14ac:dyDescent="0.15">
       <c r="A30" s="16" t="s">
         <v>139</v>
       </c>
@@ -2831,7 +2826,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="31" spans="1:5" ht="15" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:5" ht="32" x14ac:dyDescent="0.15">
       <c r="A31" s="16" t="s">
         <v>140</v>
       </c>
@@ -2842,7 +2837,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="32" spans="1:5" ht="30" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:5" ht="32" x14ac:dyDescent="0.15">
       <c r="A32" s="16" t="s">
         <v>149</v>
       </c>
@@ -2859,7 +2854,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="33" spans="1:5" ht="45" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:5" ht="48" x14ac:dyDescent="0.15">
       <c r="A33" s="16" t="s">
         <v>150</v>
       </c>
@@ -2891,47 +2886,47 @@
       <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.8203125" defaultRowHeight="12.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="10.8203125" style="2"/>
-    <col min="2" max="2" width="9.46875" customWidth="1"/>
-    <col min="3" max="3" width="15.8203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.3515625" customWidth="1"/>
-    <col min="5" max="5" width="6.8203125" customWidth="1"/>
-    <col min="6" max="6" width="12.46875" style="7" customWidth="1"/>
+    <col min="1" max="1" width="10.83203125" style="2"/>
+    <col min="2" max="2" width="9.5" customWidth="1"/>
+    <col min="3" max="3" width="15.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.33203125" customWidth="1"/>
+    <col min="5" max="5" width="6.83203125" customWidth="1"/>
+    <col min="6" max="6" width="12.5" style="7" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A1" s="2" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A2" s="2" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A3" s="2" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A5" s="2" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A6" s="2" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A8" s="2" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="14" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A14" s="4" t="s">
         <v>156</v>
       </c>
@@ -2954,7 +2949,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A15" t="s">
         <v>157</v>
       </c>
@@ -2970,7 +2965,7 @@
       <c r="F15" s="11"/>
       <c r="G15" s="7"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A16" t="s">
         <v>158</v>
       </c>
@@ -2995,7 +2990,7 @@
         <v>125.00000000000001</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A17" s="2" t="s">
         <v>159</v>
       </c>
@@ -3020,7 +3015,7 @@
         <v>102.22222222222223</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A18" s="2" t="s">
         <v>160</v>
       </c>
@@ -3045,7 +3040,7 @@
         <v>97.5</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A19" s="2" t="s">
         <v>161</v>
       </c>
@@ -3085,17 +3080,17 @@
       <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.8203125" defaultRowHeight="12.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="10.8203125" style="2"/>
-    <col min="2" max="2" width="16.64453125" customWidth="1"/>
-    <col min="3" max="3" width="14.46875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.17578125" customWidth="1"/>
-    <col min="5" max="5" width="6.8203125" customWidth="1"/>
-    <col min="6" max="6" width="12.46875" style="7" customWidth="1"/>
+    <col min="1" max="1" width="10.83203125" style="2"/>
+    <col min="2" max="2" width="16.6640625" customWidth="1"/>
+    <col min="3" max="3" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.1640625" customWidth="1"/>
+    <col min="5" max="5" width="6.83203125" customWidth="1"/>
+    <col min="6" max="6" width="12.5" style="7" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -3115,7 +3110,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A2" s="2">
         <v>42044</v>
       </c>
@@ -3126,7 +3121,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A3" s="2">
         <v>42058</v>
       </c>
@@ -3148,17 +3143,17 @@
         <v>0.73643410852713176</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A4" s="2">
         <v>42072</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A5" s="2">
         <v>42093</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A6" s="2">
         <v>42107</v>
       </c>
@@ -3179,28 +3174,28 @@
       <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.8203125" defaultRowHeight="12.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="9" style="16" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="24.46875" style="18" customWidth="1"/>
-    <col min="3" max="3" width="7.3515625" style="16" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.64453125" style="16" customWidth="1"/>
-    <col min="5" max="5" width="8.46875" style="16" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.3515625" style="16" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.64453125" style="16" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.3515625" style="16" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.5" style="18" customWidth="1"/>
+    <col min="3" max="3" width="7.33203125" style="16" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.6640625" style="16" customWidth="1"/>
+    <col min="5" max="5" width="8.5" style="16" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.33203125" style="16" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.6640625" style="16" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.33203125" style="16" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="11" style="26" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="20.8203125" style="29" customWidth="1"/>
-    <col min="11" max="11" width="17.8203125" style="29" customWidth="1"/>
+    <col min="10" max="10" width="20.83203125" style="29" customWidth="1"/>
+    <col min="11" max="11" width="17.83203125" style="29" customWidth="1"/>
     <col min="12" max="12" width="13" style="24" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="1.8203125" style="24" customWidth="1"/>
-    <col min="14" max="14" width="16.8203125" style="29" customWidth="1"/>
-    <col min="15" max="15" width="22.8203125" style="29" customWidth="1"/>
-    <col min="16" max="16" width="10.17578125" style="24" bestFit="1" customWidth="1"/>
-    <col min="17" max="16384" width="10.8203125" style="16"/>
+    <col min="13" max="13" width="1.83203125" style="24" customWidth="1"/>
+    <col min="14" max="14" width="16.83203125" style="29" customWidth="1"/>
+    <col min="15" max="15" width="22.83203125" style="29" customWidth="1"/>
+    <col min="16" max="16" width="10.1640625" style="24" bestFit="1" customWidth="1"/>
+    <col min="17" max="16384" width="10.83203125" style="16"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A1" s="15" t="s">
         <v>9</v>
       </c>
@@ -3247,7 +3242,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="2" spans="1:16" ht="24.75" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:16" ht="26" x14ac:dyDescent="0.15">
       <c r="A2" s="16" t="s">
         <v>109</v>
       </c>
@@ -3294,7 +3289,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:16" ht="24.75" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:16" ht="26" x14ac:dyDescent="0.15">
       <c r="A3" s="16" t="s">
         <v>110</v>
       </c>
@@ -3341,7 +3336,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:16" ht="24.75" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:16" ht="26" x14ac:dyDescent="0.15">
       <c r="A4" s="16" t="s">
         <v>111</v>
       </c>
@@ -3388,7 +3383,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="5" spans="1:16" ht="24.75" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:16" ht="26" x14ac:dyDescent="0.15">
       <c r="A5" s="16" t="s">
         <v>112</v>
       </c>
@@ -3435,7 +3430,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="6" spans="1:16" ht="24.75" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:16" ht="26" x14ac:dyDescent="0.15">
       <c r="A6" s="16" t="s">
         <v>113</v>
       </c>
@@ -3482,7 +3477,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:16" ht="24.75" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:16" ht="26" x14ac:dyDescent="0.15">
       <c r="A7" s="16" t="s">
         <v>114</v>
       </c>
@@ -3529,7 +3524,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:16" ht="37.15" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:16" ht="39" x14ac:dyDescent="0.15">
       <c r="A8" s="16" t="s">
         <v>118</v>
       </c>
@@ -3576,7 +3571,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="9" spans="1:16" ht="24.75" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:16" ht="26" x14ac:dyDescent="0.15">
       <c r="A9" s="16" t="s">
         <v>119</v>
       </c>
@@ -3623,7 +3618,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.15">
       <c r="J10" s="28"/>
       <c r="K10" s="28"/>
       <c r="L10" s="27"/>
@@ -3631,43 +3626,43 @@
       <c r="O10" s="28"/>
       <c r="P10" s="27"/>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.15">
       <c r="B13" s="20" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.15">
       <c r="B14" s="30"/>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.15">
       <c r="B15" s="31" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="16" spans="1:16" ht="19.5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:16" ht="22" x14ac:dyDescent="0.15">
       <c r="B16" s="32" t="s">
         <v>230</v>
       </c>
     </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:2" x14ac:dyDescent="0.15">
       <c r="B17" s="20"/>
     </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:2" x14ac:dyDescent="0.15">
       <c r="B18" s="31" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="19" spans="2:2" ht="58.5" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:2" ht="66" x14ac:dyDescent="0.15">
       <c r="B19" s="32" t="s">
         <v>229</v>
       </c>
     </row>
-    <row r="21" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:2" x14ac:dyDescent="0.15">
       <c r="B21" s="31" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="22" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:2" x14ac:dyDescent="0.15">
       <c r="B22" s="32" t="s">
         <v>231</v>
       </c>
@@ -3684,24 +3679,24 @@
   <dimension ref="A1:P20"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.8203125" defaultRowHeight="12.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="10.8203125" style="33"/>
+    <col min="1" max="1" width="10.83203125" style="33"/>
     <col min="2" max="2" width="22" style="33" bestFit="1" customWidth="1"/>
-    <col min="3" max="9" width="10.8203125" style="33"/>
-    <col min="10" max="10" width="13.8203125" style="33" customWidth="1"/>
+    <col min="3" max="9" width="10.83203125" style="33"/>
+    <col min="10" max="10" width="13.83203125" style="33" customWidth="1"/>
     <col min="11" max="11" width="16" style="33" customWidth="1"/>
-    <col min="12" max="12" width="15.8203125" style="33" customWidth="1"/>
-    <col min="13" max="13" width="4.17578125" style="33" customWidth="1"/>
-    <col min="14" max="14" width="10.8203125" style="33" customWidth="1"/>
-    <col min="15" max="15" width="15.3515625" style="33" customWidth="1"/>
-    <col min="16" max="16384" width="10.8203125" style="33"/>
+    <col min="12" max="12" width="15.83203125" style="33" customWidth="1"/>
+    <col min="13" max="13" width="4.1640625" style="33" customWidth="1"/>
+    <col min="14" max="14" width="10.83203125" style="33" customWidth="1"/>
+    <col min="15" max="15" width="15.33203125" style="33" customWidth="1"/>
+    <col min="16" max="16384" width="10.83203125" style="33"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="34" t="s">
         <v>9</v>
       </c>
@@ -3749,16 +3744,19 @@
         <v>178</v>
       </c>
     </row>
-    <row r="2" spans="1:16" s="37" customFormat="1" ht="74.25" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:16" s="37" customFormat="1" ht="78" x14ac:dyDescent="0.15">
       <c r="A2" s="37" t="s">
         <v>115</v>
       </c>
-      <c r="B2" s="37" t="s">
-        <v>60</v>
+      <c r="B2" t="s">
+        <v>69</v>
       </c>
       <c r="C2" s="37" t="s">
         <v>183</v>
       </c>
+      <c r="D2" s="37" t="s">
+        <v>219</v>
+      </c>
       <c r="E2" s="37">
         <v>25</v>
       </c>
@@ -3793,16 +3791,19 @@
         <v>41</v>
       </c>
     </row>
-    <row r="3" spans="1:16" s="37" customFormat="1" ht="86.65" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:16" s="37" customFormat="1" ht="91" x14ac:dyDescent="0.15">
       <c r="A3" s="37" t="s">
         <v>116</v>
       </c>
-      <c r="B3" s="37" t="s">
-        <v>60</v>
+      <c r="B3" t="s">
+        <v>152</v>
       </c>
       <c r="C3" s="37" t="s">
         <v>183</v>
       </c>
+      <c r="D3" s="37" t="s">
+        <v>219</v>
+      </c>
       <c r="E3" s="37">
         <v>30</v>
       </c>
@@ -3837,7 +3838,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="4" spans="1:16" s="37" customFormat="1" ht="24.75" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:16" s="37" customFormat="1" ht="39" x14ac:dyDescent="0.15">
       <c r="A4" s="37" t="s">
         <v>117</v>
       </c>
@@ -3884,7 +3885,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:16" s="37" customFormat="1" ht="24.75" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:16" s="37" customFormat="1" ht="26" x14ac:dyDescent="0.15">
       <c r="A5" s="37" t="s">
         <v>120</v>
       </c>
@@ -3931,7 +3932,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:16" s="37" customFormat="1" ht="24.75" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:16" s="37" customFormat="1" ht="26" x14ac:dyDescent="0.15">
       <c r="A6" s="37" t="s">
         <v>121</v>
       </c>
@@ -3978,7 +3979,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:16" s="37" customFormat="1" ht="24.75" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:16" s="37" customFormat="1" ht="39" x14ac:dyDescent="0.15">
       <c r="A7" s="37" t="s">
         <v>122</v>
       </c>
@@ -4025,7 +4026,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="8" spans="1:16" s="37" customFormat="1" ht="24.75" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:16" s="37" customFormat="1" ht="26" x14ac:dyDescent="0.15">
       <c r="A8" s="37" t="s">
         <v>149</v>
       </c>
@@ -4072,7 +4073,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:16" s="37" customFormat="1" ht="24.75" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:16" s="37" customFormat="1" ht="26" x14ac:dyDescent="0.15">
       <c r="A9" s="37" t="s">
         <v>150</v>
       </c>
@@ -4119,17 +4120,17 @@
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:16" s="37" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="11" spans="1:16" s="37" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="12" spans="1:16" s="37" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="13" spans="1:16" s="37" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="14" spans="1:16" s="37" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="15" spans="1:16" s="37" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="16" spans="1:16" s="37" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="17" s="37" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="18" s="37" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="19" s="37" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="20" s="37" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="10" spans="1:16" s="37" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="11" spans="1:16" s="37" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="12" spans="1:16" s="37" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="13" spans="1:16" s="37" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="14" spans="1:16" s="37" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="15" spans="1:16" s="37" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="16" spans="1:16" s="37" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="17" s="37" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="18" s="37" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="19" s="37" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="20" s="37" customFormat="1" x14ac:dyDescent="0.15"/>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -4145,9 +4146,9 @@
       <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.8203125" defaultRowHeight="12.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <sheetData>
-    <row r="1" spans="1:9" ht="24.75" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" ht="26" x14ac:dyDescent="0.15">
       <c r="A1" s="4" t="s">
         <v>3</v>
       </c>
@@ -4190,9 +4191,9 @@
       <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.8203125" defaultRowHeight="12.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <sheetData>
-    <row r="1" spans="1:9" ht="24.75" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" ht="26" x14ac:dyDescent="0.15">
       <c r="A1" s="4" t="s">
         <v>3</v>
       </c>
@@ -4231,17 +4232,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:C43"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView topLeftCell="A8" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.8203125" defaultRowHeight="12.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="2" max="2" width="28.17578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="49.46875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="28.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="49.5" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A1" s="4" t="s">
         <v>108</v>
       </c>
@@ -4252,7 +4253,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" ht="32" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
         <v>109</v>
       </c>
@@ -4263,7 +4264,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="15" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" ht="16" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
         <v>110</v>
       </c>
@@ -4274,7 +4275,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="15" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" ht="16" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
         <v>111</v>
       </c>
@@ -4285,7 +4286,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" ht="32" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
         <v>112</v>
       </c>
@@ -4296,7 +4297,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="15" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" ht="16" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
         <v>113</v>
       </c>
@@ -4307,7 +4308,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="15" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" ht="16" x14ac:dyDescent="0.15">
       <c r="A7" t="s">
         <v>114</v>
       </c>
@@ -4318,7 +4319,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="45" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" ht="48" x14ac:dyDescent="0.15">
       <c r="A8" t="s">
         <v>115</v>
       </c>
@@ -4329,7 +4330,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" ht="32" x14ac:dyDescent="0.15">
       <c r="A9" t="s">
         <v>116</v>
       </c>
@@ -4340,7 +4341,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" ht="32" x14ac:dyDescent="0.15">
       <c r="A10" t="s">
         <v>117</v>
       </c>
@@ -4351,7 +4352,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" ht="32" x14ac:dyDescent="0.15">
       <c r="A11" t="s">
         <v>118</v>
       </c>
@@ -4362,7 +4363,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" ht="32" x14ac:dyDescent="0.15">
       <c r="A12" t="s">
         <v>119</v>
       </c>
@@ -4373,7 +4374,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="45" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" ht="48" x14ac:dyDescent="0.15">
       <c r="A13" t="s">
         <v>120</v>
       </c>
@@ -4384,7 +4385,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="60" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" ht="64" x14ac:dyDescent="0.15">
       <c r="A14" t="s">
         <v>121</v>
       </c>
@@ -4395,7 +4396,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" ht="32" x14ac:dyDescent="0.15">
       <c r="A15" t="s">
         <v>122</v>
       </c>
@@ -4406,7 +4407,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="15" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" ht="16" x14ac:dyDescent="0.15">
       <c r="A16" t="s">
         <v>123</v>
       </c>
@@ -4417,7 +4418,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" ht="32" x14ac:dyDescent="0.15">
       <c r="A17" t="s">
         <v>124</v>
       </c>
@@ -4428,7 +4429,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="15" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3" ht="16" x14ac:dyDescent="0.15">
       <c r="A18" t="s">
         <v>125</v>
       </c>
@@ -4439,7 +4440,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="15" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:3" ht="16" x14ac:dyDescent="0.15">
       <c r="A19" t="s">
         <v>126</v>
       </c>
@@ -4450,7 +4451,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="15" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:3" ht="16" x14ac:dyDescent="0.15">
       <c r="A20" t="s">
         <v>127</v>
       </c>
@@ -4461,7 +4462,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:3" ht="32" x14ac:dyDescent="0.15">
       <c r="A21" t="s">
         <v>128</v>
       </c>
@@ -4472,7 +4473,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:3" ht="32" x14ac:dyDescent="0.15">
       <c r="A22" t="s">
         <v>129</v>
       </c>
@@ -4483,7 +4484,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:3" ht="32" x14ac:dyDescent="0.15">
       <c r="A23" t="s">
         <v>130</v>
       </c>
@@ -4494,7 +4495,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:3" ht="32" x14ac:dyDescent="0.15">
       <c r="A24" t="s">
         <v>131</v>
       </c>
@@ -4505,7 +4506,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="45" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:3" ht="48" x14ac:dyDescent="0.15">
       <c r="A25" t="s">
         <v>132</v>
       </c>
@@ -4516,7 +4517,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:3" ht="32" x14ac:dyDescent="0.15">
       <c r="A26" t="s">
         <v>133</v>
       </c>
@@ -4527,7 +4528,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="105" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:3" ht="128" x14ac:dyDescent="0.15">
       <c r="A27" t="s">
         <v>134</v>
       </c>
@@ -4538,7 +4539,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="15" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:3" ht="16" x14ac:dyDescent="0.15">
       <c r="A28" t="s">
         <v>135</v>
       </c>
@@ -4549,7 +4550,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:3" ht="32" x14ac:dyDescent="0.15">
       <c r="A29" t="s">
         <v>136</v>
       </c>
@@ -4560,7 +4561,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="30" spans="1:3" ht="15" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:3" ht="16" x14ac:dyDescent="0.15">
       <c r="A30" t="s">
         <v>137</v>
       </c>
@@ -4571,7 +4572,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="31" spans="1:3" ht="15" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:3" ht="16" x14ac:dyDescent="0.15">
       <c r="A31" t="s">
         <v>138</v>
       </c>
@@ -4582,7 +4583,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:3" ht="32" x14ac:dyDescent="0.15">
       <c r="A32" t="s">
         <v>139</v>
       </c>
@@ -4593,7 +4594,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="33" spans="1:3" ht="15" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:3" ht="16" x14ac:dyDescent="0.15">
       <c r="A33" t="s">
         <v>140</v>
       </c>
@@ -4604,7 +4605,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="34" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:3" ht="32" x14ac:dyDescent="0.15">
       <c r="A34" t="s">
         <v>141</v>
       </c>
@@ -4615,7 +4616,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="35" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:3" ht="48" x14ac:dyDescent="0.15">
       <c r="A35" t="s">
         <v>142</v>
       </c>
@@ -4626,7 +4627,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="36" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:3" ht="32" x14ac:dyDescent="0.15">
       <c r="A36" t="s">
         <v>143</v>
       </c>
@@ -4637,7 +4638,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="37" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:3" ht="32" x14ac:dyDescent="0.15">
       <c r="A37" t="s">
         <v>144</v>
       </c>
@@ -4648,7 +4649,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="38" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:3" ht="32" x14ac:dyDescent="0.15">
       <c r="A38" t="s">
         <v>145</v>
       </c>
@@ -4659,7 +4660,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="39" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:3" ht="32" x14ac:dyDescent="0.15">
       <c r="A39" t="s">
         <v>146</v>
       </c>
@@ -4670,7 +4671,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="40" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:3" ht="32" x14ac:dyDescent="0.15">
       <c r="A40" t="s">
         <v>147</v>
       </c>
@@ -4681,7 +4682,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="41" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:3" ht="32" x14ac:dyDescent="0.15">
       <c r="A41" t="s">
         <v>148</v>
       </c>
@@ -4692,7 +4693,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="42" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:3" ht="32" x14ac:dyDescent="0.15">
       <c r="A42" t="s">
         <v>149</v>
       </c>
@@ -4703,7 +4704,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="43" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:3" ht="32" x14ac:dyDescent="0.15">
       <c r="A43" t="s">
         <v>150</v>
       </c>

</xml_diff>

<commit_message>
Implemented US28 and US32
Updated tesm report for US28 and US32

Added Sprint 3 test file to demo implemented features
</commit_message>
<xml_diff>
--- a/TeamDReport copy.xlsx
+++ b/TeamDReport copy.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10211"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/JP/OneDrive/Jonathan's Folder!/Stevens/CS_555_Agile_Methods_for_SW_Development/Project_Documents/SSW555-DriverlessCar/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Code_Modeling\Python\SSW_555\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F19390C-D01D-A94F-817B-CDF70F30ED5D}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="14400" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="14400" tabRatio="500" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Team" sheetId="1" r:id="rId1"/>
@@ -23,7 +22,7 @@
     <sheet name="Sprint4" sheetId="6" r:id="rId8"/>
     <sheet name="Stories" sheetId="11" r:id="rId9"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="330"/>
@@ -42,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="549" uniqueCount="264">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="560" uniqueCount="269">
   <si>
     <t>Date</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -867,12 +866,29 @@
   </si>
   <si>
     <t>Leaving enough time to integrate so we are not rushing to do so last minute, that way we can use the group collective to solve any problems we may have</t>
+  </si>
+  <si>
+    <t>sort_siblings
+order_siblings_by_age</t>
+  </si>
+  <si>
+    <t>18
+47</t>
+  </si>
+  <si>
+    <t>test_order_siblings_by_age</t>
+  </si>
+  <si>
+    <t>list_multiple_births</t>
+  </si>
+  <si>
+    <t>test_list_multiple_births</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="m/d"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
@@ -1016,7 +1032,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1114,6 +1130,9 @@
     </xf>
     <xf numFmtId="14" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="66">
@@ -1224,7 +1243,7 @@
             <c:numRef>
               <c:f>'Burndown README'!$B$15:$B$20</c:f>
               <c:numCache>
-                <c:formatCode>m/d/yy</c:formatCode>
+                <c:formatCode>m/d/yyyy</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
                   <c:v>41065</c:v>
@@ -1295,7 +1314,7 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:numFmt formatCode="m/d/yy" sourceLinked="1"/>
+        <c:numFmt formatCode="m/d/yyyy" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -2281,22 +2300,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
+    <sheetView zoomScale="150" workbookViewId="0">
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="7.83203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.5" customWidth="1"/>
-    <col min="4" max="5" width="20.5" customWidth="1"/>
+    <col min="1" max="1" width="7.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.6328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.453125" customWidth="1"/>
+    <col min="4" max="5" width="20.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>19</v>
       </c>
@@ -2313,7 +2332,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="2" spans="1:5" s="13" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:5" s="13" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="13" t="s">
         <v>183</v>
       </c>
@@ -2330,7 +2349,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>182</v>
       </c>
@@ -2347,7 +2366,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="13" t="s">
         <v>187</v>
       </c>
@@ -2364,7 +2383,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="13" t="s">
         <v>195</v>
       </c>
@@ -2381,7 +2400,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="D10" s="4" t="s">
         <v>31</v>
       </c>
@@ -2390,16 +2409,16 @@
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A4:D6">
+  <sortState ref="A4:D6">
     <sortCondition ref="C4:C6"/>
   </sortState>
   <phoneticPr fontId="2" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="D4" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="D3" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
-    <hyperlink ref="D2" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
-    <hyperlink ref="D5" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
-    <hyperlink ref="E10" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="D4" r:id="rId1"/>
+    <hyperlink ref="D3" r:id="rId2"/>
+    <hyperlink ref="D2" r:id="rId3"/>
+    <hyperlink ref="D5" r:id="rId4"/>
+    <hyperlink ref="E10" r:id="rId5"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -2407,24 +2426,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E33"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E30" sqref="E30"/>
+    <sheetView topLeftCell="A24" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="E31" sqref="E31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="6.83203125" style="16" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="29.1640625" style="16" customWidth="1"/>
-    <col min="3" max="3" width="34.5" style="16" customWidth="1"/>
-    <col min="4" max="4" width="6.6640625" style="16" customWidth="1"/>
-    <col min="5" max="5" width="10.33203125" style="16" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="10.83203125" style="16"/>
+    <col min="1" max="1" width="6.81640625" style="16" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="29.1796875" style="16" customWidth="1"/>
+    <col min="3" max="3" width="34.453125" style="16" customWidth="1"/>
+    <col min="4" max="4" width="6.6328125" style="16" customWidth="1"/>
+    <col min="5" max="5" width="10.36328125" style="16" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="10.81640625" style="16"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="15" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:5" s="15" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="15" t="s">
         <v>29</v>
       </c>
@@ -2441,7 +2460,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="34" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:5" ht="30" x14ac:dyDescent="0.2">
       <c r="A2" s="16" t="s">
         <v>109</v>
       </c>
@@ -2455,10 +2474,10 @@
         <v>195</v>
       </c>
       <c r="E2" s="16" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" ht="34" x14ac:dyDescent="0.15">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="30" x14ac:dyDescent="0.2">
       <c r="A3" s="16" t="s">
         <v>110</v>
       </c>
@@ -2472,10 +2491,10 @@
         <v>195</v>
       </c>
       <c r="E3" s="16" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" ht="34" x14ac:dyDescent="0.15">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="30" x14ac:dyDescent="0.2">
       <c r="A4" s="16" t="s">
         <v>111</v>
       </c>
@@ -2489,10 +2508,10 @@
         <v>183</v>
       </c>
       <c r="E4" s="16" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="51" x14ac:dyDescent="0.15">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="45" x14ac:dyDescent="0.2">
       <c r="A5" s="16" t="s">
         <v>112</v>
       </c>
@@ -2506,10 +2525,10 @@
         <v>183</v>
       </c>
       <c r="E5" s="16" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="34" x14ac:dyDescent="0.15">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="30" x14ac:dyDescent="0.2">
       <c r="A6" s="16" t="s">
         <v>113</v>
       </c>
@@ -2523,10 +2542,10 @@
         <v>187</v>
       </c>
       <c r="E6" s="16" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" ht="34" x14ac:dyDescent="0.15">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="30" x14ac:dyDescent="0.2">
       <c r="A7" s="16" t="s">
         <v>114</v>
       </c>
@@ -2540,10 +2559,10 @@
         <v>187</v>
       </c>
       <c r="E7" s="16" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="68" x14ac:dyDescent="0.15">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="60" x14ac:dyDescent="0.2">
       <c r="A8" s="16" t="s">
         <v>115</v>
       </c>
@@ -2557,10 +2576,10 @@
         <v>183</v>
       </c>
       <c r="E8" s="16" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" ht="51" x14ac:dyDescent="0.15">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="45" x14ac:dyDescent="0.2">
       <c r="A9" s="16" t="s">
         <v>116</v>
       </c>
@@ -2574,10 +2593,10 @@
         <v>183</v>
       </c>
       <c r="E9" s="16" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" ht="51" x14ac:dyDescent="0.15">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="45" x14ac:dyDescent="0.2">
       <c r="A10" s="16" t="s">
         <v>117</v>
       </c>
@@ -2591,10 +2610,10 @@
         <v>187</v>
       </c>
       <c r="E10" s="16" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" ht="51" x14ac:dyDescent="0.15">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="45" x14ac:dyDescent="0.2">
       <c r="A11" s="16" t="s">
         <v>118</v>
       </c>
@@ -2608,10 +2627,10 @@
         <v>182</v>
       </c>
       <c r="E11" s="16" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" ht="34" x14ac:dyDescent="0.15">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="30" x14ac:dyDescent="0.2">
       <c r="A12" s="16" t="s">
         <v>119</v>
       </c>
@@ -2625,10 +2644,10 @@
         <v>182</v>
       </c>
       <c r="E12" s="16" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" ht="68" x14ac:dyDescent="0.15">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="45" x14ac:dyDescent="0.2">
       <c r="A13" s="16" t="s">
         <v>120</v>
       </c>
@@ -2642,10 +2661,10 @@
         <v>187</v>
       </c>
       <c r="E13" s="16" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" ht="85" x14ac:dyDescent="0.15">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="75" x14ac:dyDescent="0.2">
       <c r="A14" s="16" t="s">
         <v>121</v>
       </c>
@@ -2659,10 +2678,10 @@
         <v>182</v>
       </c>
       <c r="E14" s="16" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" ht="34" x14ac:dyDescent="0.15">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="30" x14ac:dyDescent="0.2">
       <c r="A15" s="16" t="s">
         <v>122</v>
       </c>
@@ -2679,7 +2698,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="34" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:5" ht="30" x14ac:dyDescent="0.2">
       <c r="A16" s="16" t="s">
         <v>123</v>
       </c>
@@ -2696,7 +2715,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="34" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:5" ht="30" x14ac:dyDescent="0.2">
       <c r="A17" s="16" t="s">
         <v>124</v>
       </c>
@@ -2713,7 +2732,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="34" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:5" ht="30" x14ac:dyDescent="0.2">
       <c r="A18" s="16" t="s">
         <v>125</v>
       </c>
@@ -2730,7 +2749,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="17" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:5" ht="15" x14ac:dyDescent="0.2">
       <c r="A19" s="16" t="s">
         <v>126</v>
       </c>
@@ -2747,7 +2766,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="34" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:5" ht="30" x14ac:dyDescent="0.2">
       <c r="A20" s="16" t="s">
         <v>127</v>
       </c>
@@ -2758,7 +2777,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="34" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:5" ht="30" x14ac:dyDescent="0.2">
       <c r="A21" s="16" t="s">
         <v>128</v>
       </c>
@@ -2769,7 +2788,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="22" spans="1:5" ht="34" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:5" ht="30" x14ac:dyDescent="0.2">
       <c r="A22" s="16" t="s">
         <v>130</v>
       </c>
@@ -2780,7 +2799,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="23" spans="1:5" ht="51" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:5" ht="45" x14ac:dyDescent="0.2">
       <c r="A23" s="16" t="s">
         <v>131</v>
       </c>
@@ -2791,7 +2810,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="24" spans="1:5" ht="68" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:5" ht="45" x14ac:dyDescent="0.2">
       <c r="A24" s="16" t="s">
         <v>132</v>
       </c>
@@ -2802,7 +2821,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="25" spans="1:5" ht="51" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:5" ht="45" x14ac:dyDescent="0.2">
       <c r="A25" s="16" t="s">
         <v>133</v>
       </c>
@@ -2813,7 +2832,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="26" spans="1:5" ht="34" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:5" ht="30" x14ac:dyDescent="0.2">
       <c r="A26" s="16" t="s">
         <v>135</v>
       </c>
@@ -2824,7 +2843,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="27" spans="1:5" ht="34" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:5" ht="30" x14ac:dyDescent="0.2">
       <c r="A27" s="16" t="s">
         <v>136</v>
       </c>
@@ -2838,10 +2857,10 @@
         <v>195</v>
       </c>
       <c r="E27" s="16" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" ht="34" x14ac:dyDescent="0.15">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" ht="30" x14ac:dyDescent="0.2">
       <c r="A28" s="16" t="s">
         <v>137</v>
       </c>
@@ -2852,7 +2871,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="29" spans="1:5" ht="34" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:5" ht="30" x14ac:dyDescent="0.2">
       <c r="A29" s="16" t="s">
         <v>138</v>
       </c>
@@ -2869,7 +2888,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="30" spans="1:5" ht="34" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:5" ht="30" x14ac:dyDescent="0.2">
       <c r="A30" s="16" t="s">
         <v>139</v>
       </c>
@@ -2886,7 +2905,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="31" spans="1:5" ht="34" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:5" ht="15" x14ac:dyDescent="0.2">
       <c r="A31" s="16" t="s">
         <v>140</v>
       </c>
@@ -2900,10 +2919,10 @@
         <v>195</v>
       </c>
       <c r="E31" s="16" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" ht="34" x14ac:dyDescent="0.15">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" ht="30" x14ac:dyDescent="0.2">
       <c r="A32" s="16" t="s">
         <v>149</v>
       </c>
@@ -2920,7 +2939,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="33" spans="1:5" ht="51" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:5" ht="45" x14ac:dyDescent="0.2">
       <c r="A33" s="16" t="s">
         <v>150</v>
       </c>
@@ -2945,54 +2964,54 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G19"/>
   <sheetViews>
     <sheetView topLeftCell="A30" zoomScale="150" workbookViewId="0">
       <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.83203125" style="2"/>
-    <col min="2" max="2" width="9.5" customWidth="1"/>
-    <col min="3" max="3" width="15.83203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.33203125" customWidth="1"/>
-    <col min="5" max="5" width="6.83203125" customWidth="1"/>
-    <col min="6" max="6" width="12.5" style="7" customWidth="1"/>
+    <col min="1" max="1" width="10.81640625" style="2"/>
+    <col min="2" max="2" width="9.453125" customWidth="1"/>
+    <col min="3" max="3" width="15.81640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.36328125" customWidth="1"/>
+    <col min="5" max="5" width="6.81640625" customWidth="1"/>
+    <col min="6" max="6" width="12.453125" style="7" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="14" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
         <v>156</v>
       </c>
@@ -3015,7 +3034,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>157</v>
       </c>
@@ -3031,7 +3050,7 @@
       <c r="F15" s="11"/>
       <c r="G15" s="7"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>158</v>
       </c>
@@ -3056,7 +3075,7 @@
         <v>125.00000000000001</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
         <v>159</v>
       </c>
@@ -3081,7 +3100,7 @@
         <v>102.22222222222223</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
         <v>160</v>
       </c>
@@ -3106,7 +3125,7 @@
         <v>97.5</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
         <v>161</v>
       </c>
@@ -3139,24 +3158,24 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView zoomScale="150" workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.83203125" style="2"/>
-    <col min="2" max="2" width="16.6640625" customWidth="1"/>
-    <col min="3" max="3" width="14.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.1640625" customWidth="1"/>
-    <col min="5" max="5" width="6.83203125" customWidth="1"/>
-    <col min="6" max="6" width="12.5" style="7" customWidth="1"/>
+    <col min="1" max="1" width="10.81640625" style="2"/>
+    <col min="2" max="2" width="16.6328125" customWidth="1"/>
+    <col min="3" max="3" width="14.453125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.1796875" customWidth="1"/>
+    <col min="5" max="5" width="6.81640625" customWidth="1"/>
+    <col min="6" max="6" width="12.453125" style="7" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -3176,7 +3195,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="2">
         <v>42044</v>
       </c>
@@ -3187,7 +3206,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="2">
         <v>42058</v>
       </c>
@@ -3209,7 +3228,7 @@
         <v>44.186046511627907</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
         <v>42079</v>
       </c>
@@ -3230,12 +3249,12 @@
         <v>11.733333333333333</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
         <v>42093</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="2">
         <v>42107</v>
       </c>
@@ -3249,35 +3268,35 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P22"/>
   <sheetViews>
     <sheetView topLeftCell="A10" zoomScale="150" workbookViewId="0">
       <selection activeCell="B13" sqref="B13:B22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="9" style="16" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="24.5" style="18" customWidth="1"/>
-    <col min="3" max="3" width="7.33203125" style="16" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.6640625" style="16" customWidth="1"/>
-    <col min="5" max="5" width="8.5" style="16" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.33203125" style="16" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.6640625" style="16" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.33203125" style="16" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.453125" style="18" customWidth="1"/>
+    <col min="3" max="3" width="7.36328125" style="16" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.6328125" style="16" customWidth="1"/>
+    <col min="5" max="5" width="8.453125" style="16" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.36328125" style="16" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.6328125" style="16" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.36328125" style="16" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="11" style="26" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="20.83203125" style="29" customWidth="1"/>
-    <col min="11" max="11" width="17.83203125" style="29" customWidth="1"/>
+    <col min="10" max="10" width="20.81640625" style="29" customWidth="1"/>
+    <col min="11" max="11" width="17.81640625" style="29" customWidth="1"/>
     <col min="12" max="12" width="13" style="24" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="1.83203125" style="24" customWidth="1"/>
-    <col min="14" max="14" width="16.83203125" style="29" customWidth="1"/>
-    <col min="15" max="15" width="22.83203125" style="29" customWidth="1"/>
-    <col min="16" max="16" width="10.1640625" style="24" bestFit="1" customWidth="1"/>
-    <col min="17" max="16384" width="10.83203125" style="16"/>
+    <col min="13" max="13" width="1.81640625" style="24" customWidth="1"/>
+    <col min="14" max="14" width="16.81640625" style="29" customWidth="1"/>
+    <col min="15" max="15" width="22.81640625" style="29" customWidth="1"/>
+    <col min="16" max="16" width="10.1796875" style="24" bestFit="1" customWidth="1"/>
+    <col min="17" max="16384" width="10.81640625" style="16"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="14" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A1" s="15" t="s">
         <v>9</v>
       </c>
@@ -3324,7 +3343,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="2" spans="1:16" ht="28" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:16" ht="25.2" x14ac:dyDescent="0.2">
       <c r="A2" s="16" t="s">
         <v>109</v>
       </c>
@@ -3371,7 +3390,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:16" ht="28" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:16" ht="25.2" x14ac:dyDescent="0.2">
       <c r="A3" s="16" t="s">
         <v>110</v>
       </c>
@@ -3418,7 +3437,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:16" ht="28" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:16" ht="25.2" x14ac:dyDescent="0.2">
       <c r="A4" s="16" t="s">
         <v>111</v>
       </c>
@@ -3465,7 +3484,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="5" spans="1:16" ht="28" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:16" ht="25.2" x14ac:dyDescent="0.2">
       <c r="A5" s="16" t="s">
         <v>112</v>
       </c>
@@ -3512,7 +3531,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="6" spans="1:16" ht="28" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:16" ht="25.2" x14ac:dyDescent="0.2">
       <c r="A6" s="16" t="s">
         <v>113</v>
       </c>
@@ -3559,7 +3578,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:16" ht="28" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:16" ht="25.2" x14ac:dyDescent="0.2">
       <c r="A7" s="16" t="s">
         <v>114</v>
       </c>
@@ -3606,7 +3625,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:16" ht="42" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:16" ht="37.799999999999997" x14ac:dyDescent="0.2">
       <c r="A8" s="16" t="s">
         <v>118</v>
       </c>
@@ -3653,7 +3672,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="9" spans="1:16" ht="28" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:16" ht="25.2" x14ac:dyDescent="0.2">
       <c r="A9" s="16" t="s">
         <v>119</v>
       </c>
@@ -3700,7 +3719,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
       <c r="J10" s="28"/>
       <c r="K10" s="28"/>
       <c r="L10" s="27"/>
@@ -3708,43 +3727,43 @@
       <c r="O10" s="28"/>
       <c r="P10" s="27"/>
     </row>
-    <row r="13" spans="1:16" ht="14" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B13" s="20" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B14" s="30"/>
     </row>
-    <row r="15" spans="1:16" ht="14" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B15" s="31" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="16" spans="1:16" ht="24" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:16" ht="20.399999999999999" x14ac:dyDescent="0.2">
       <c r="B16" s="32" t="s">
         <v>230</v>
       </c>
     </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.15">
+    <row r="17" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B17" s="20"/>
     </row>
-    <row r="18" spans="2:2" ht="14" x14ac:dyDescent="0.15">
+    <row r="18" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B18" s="31" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="19" spans="2:2" ht="72" x14ac:dyDescent="0.15">
+    <row r="19" spans="2:2" ht="61.2" x14ac:dyDescent="0.2">
       <c r="B19" s="32" t="s">
         <v>229</v>
       </c>
     </row>
-    <row r="21" spans="2:2" ht="14" x14ac:dyDescent="0.15">
+    <row r="21" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B21" s="31" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="22" spans="2:2" x14ac:dyDescent="0.15">
+    <row r="22" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B22" s="32" t="s">
         <v>231</v>
       </c>
@@ -3757,28 +3776,28 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P23"/>
   <sheetViews>
-    <sheetView topLeftCell="A12" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.83203125" style="33"/>
+    <col min="1" max="1" width="10.81640625" style="33"/>
     <col min="2" max="2" width="22" style="33" bestFit="1" customWidth="1"/>
-    <col min="3" max="9" width="10.83203125" style="33"/>
-    <col min="10" max="10" width="13.83203125" style="33" customWidth="1"/>
+    <col min="3" max="9" width="10.81640625" style="33"/>
+    <col min="10" max="10" width="13.81640625" style="33" customWidth="1"/>
     <col min="11" max="11" width="16" style="33" customWidth="1"/>
-    <col min="12" max="12" width="15.83203125" style="33" customWidth="1"/>
-    <col min="13" max="13" width="4.1640625" style="33" customWidth="1"/>
-    <col min="14" max="14" width="10.83203125" style="33" customWidth="1"/>
-    <col min="15" max="15" width="15.33203125" style="33" customWidth="1"/>
-    <col min="16" max="16384" width="10.83203125" style="33"/>
+    <col min="12" max="12" width="15.81640625" style="33" customWidth="1"/>
+    <col min="13" max="13" width="4.1796875" style="33" customWidth="1"/>
+    <col min="14" max="14" width="10.81640625" style="33" customWidth="1"/>
+    <col min="15" max="15" width="15.36328125" style="33" customWidth="1"/>
+    <col min="16" max="16384" width="10.81640625" style="33"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="34" t="s">
         <v>9</v>
       </c>
@@ -3826,7 +3845,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="2" spans="1:16" s="37" customFormat="1" ht="84" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:16" s="37" customFormat="1" ht="75.599999999999994" x14ac:dyDescent="0.2">
       <c r="A2" s="37" t="s">
         <v>115</v>
       </c>
@@ -3873,7 +3892,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="3" spans="1:16" s="37" customFormat="1" ht="98" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:16" s="37" customFormat="1" ht="88.2" x14ac:dyDescent="0.2">
       <c r="A3" s="37" t="s">
         <v>116</v>
       </c>
@@ -3920,7 +3939,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="4" spans="1:16" s="37" customFormat="1" ht="42" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:16" s="37" customFormat="1" ht="25.2" x14ac:dyDescent="0.2">
       <c r="A4" s="37" t="s">
         <v>117</v>
       </c>
@@ -3967,7 +3986,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:16" s="37" customFormat="1" ht="28" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:16" s="37" customFormat="1" ht="25.2" x14ac:dyDescent="0.2">
       <c r="A5" s="37" t="s">
         <v>120</v>
       </c>
@@ -4014,7 +4033,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:16" s="37" customFormat="1" ht="28" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:16" s="37" customFormat="1" ht="25.2" x14ac:dyDescent="0.2">
       <c r="A6" s="37" t="s">
         <v>121</v>
       </c>
@@ -4061,7 +4080,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:16" s="37" customFormat="1" ht="42" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:16" s="37" customFormat="1" ht="25.2" x14ac:dyDescent="0.2">
       <c r="A7" s="37" t="s">
         <v>122</v>
       </c>
@@ -4108,7 +4127,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="8" spans="1:16" s="37" customFormat="1" ht="28" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:16" s="37" customFormat="1" ht="25.2" x14ac:dyDescent="0.2">
       <c r="A8" s="37" t="s">
         <v>149</v>
       </c>
@@ -4155,7 +4174,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:16" s="37" customFormat="1" ht="28" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:16" s="37" customFormat="1" ht="25.2" x14ac:dyDescent="0.2">
       <c r="A9" s="37" t="s">
         <v>150</v>
       </c>
@@ -4202,50 +4221,50 @@
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:16" s="37" customFormat="1" x14ac:dyDescent="0.15"/>
-    <row r="11" spans="1:16" s="37" customFormat="1" x14ac:dyDescent="0.15"/>
-    <row r="12" spans="1:16" s="37" customFormat="1" x14ac:dyDescent="0.15"/>
-    <row r="13" spans="1:16" s="37" customFormat="1" x14ac:dyDescent="0.15"/>
-    <row r="14" spans="1:16" s="37" customFormat="1" ht="14" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:16" s="37" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="11" spans="1:16" s="37" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="12" spans="1:16" s="37" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="13" spans="1:16" s="37" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="14" spans="1:16" s="37" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B14" s="20" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="15" spans="1:16" s="37" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:16" s="37" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B15" s="30"/>
     </row>
-    <row r="16" spans="1:16" s="37" customFormat="1" ht="28" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:16" s="37" customFormat="1" ht="25.2" x14ac:dyDescent="0.2">
       <c r="B16" s="31" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="17" spans="2:2" s="37" customFormat="1" ht="24" x14ac:dyDescent="0.15">
+    <row r="17" spans="2:2" s="37" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.2">
       <c r="B17" s="32" t="s">
         <v>262</v>
       </c>
     </row>
-    <row r="18" spans="2:2" s="37" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="18" spans="2:2" s="37" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B18" s="20"/>
     </row>
-    <row r="19" spans="2:2" s="37" customFormat="1" ht="28" x14ac:dyDescent="0.15">
+    <row r="19" spans="2:2" s="37" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B19" s="31" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="20" spans="2:2" s="37" customFormat="1" ht="72" x14ac:dyDescent="0.15">
+    <row r="20" spans="2:2" s="37" customFormat="1" ht="51" x14ac:dyDescent="0.2">
       <c r="B20" s="32" t="s">
         <v>263</v>
       </c>
     </row>
-    <row r="21" spans="2:2" x14ac:dyDescent="0.15">
+    <row r="21" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B21" s="18"/>
     </row>
-    <row r="22" spans="2:2" ht="14" x14ac:dyDescent="0.15">
+    <row r="22" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B22" s="31" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="23" spans="2:2" ht="36" x14ac:dyDescent="0.15">
+    <row r="23" spans="2:2" ht="20.399999999999999" x14ac:dyDescent="0.2">
       <c r="B23" s="32" t="s">
         <v>261</v>
       </c>
@@ -4258,19 +4277,24 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P9"/>
   <sheetViews>
-    <sheetView zoomScale="150" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="150" workbookViewId="0">
+      <selection activeCell="P9" sqref="P9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="23" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.81640625" style="33"/>
+    <col min="2" max="2" width="23" style="33" bestFit="1" customWidth="1"/>
+    <col min="3" max="10" width="10.81640625" style="33"/>
+    <col min="11" max="11" width="14.90625" style="33" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.81640625" style="33" bestFit="1" customWidth="1"/>
+    <col min="13" max="16384" width="10.81640625" style="33"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="34" t="s">
         <v>3</v>
       </c>
@@ -4318,140 +4342,200 @@
         <v>178</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.15">
-      <c r="A2" t="s">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A2" s="33" t="s">
         <v>123</v>
       </c>
-      <c r="B2" s="16" t="s">
+      <c r="B2" s="33" t="s">
         <v>78</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="33" t="s">
         <v>183</v>
       </c>
-      <c r="E2">
+      <c r="E2" s="33">
         <v>45</v>
       </c>
-      <c r="F2">
+      <c r="F2" s="33">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.15">
-      <c r="A3" t="s">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A3" s="33" t="s">
         <v>124</v>
       </c>
-      <c r="B3" s="16" t="s">
+      <c r="B3" s="33" t="s">
         <v>79</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="33" t="s">
         <v>187</v>
       </c>
-      <c r="E3">
+      <c r="E3" s="33">
         <v>40</v>
       </c>
-      <c r="F3">
+      <c r="F3" s="33">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.15">
-      <c r="A4" t="s">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A4" s="33" t="s">
         <v>125</v>
       </c>
-      <c r="B4" s="16" t="s">
+      <c r="B4" s="33" t="s">
         <v>172</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="33" t="s">
         <v>187</v>
       </c>
-      <c r="E4">
+      <c r="E4" s="33">
         <v>40</v>
       </c>
-      <c r="F4">
+      <c r="F4" s="33">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.15">
-      <c r="A5" t="s">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A5" s="33" t="s">
         <v>126</v>
       </c>
-      <c r="B5" s="16" t="s">
+      <c r="B5" s="33" t="s">
         <v>80</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="33" t="s">
         <v>183</v>
       </c>
-      <c r="E5">
+      <c r="E5" s="33">
         <v>45</v>
       </c>
-      <c r="F5">
+      <c r="F5" s="33">
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.15">
-      <c r="A6" t="s">
+    <row r="6" spans="1:16" ht="37.799999999999997" x14ac:dyDescent="0.2">
+      <c r="A6" s="33" t="s">
         <v>136</v>
       </c>
-      <c r="B6" s="16" t="s">
+      <c r="B6" s="33" t="s">
         <v>92</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="33" t="s">
         <v>195</v>
       </c>
-      <c r="E6">
+      <c r="D6" s="33" t="s">
+        <v>228</v>
+      </c>
+      <c r="E6" s="33">
         <v>45</v>
       </c>
-      <c r="F6">
+      <c r="F6" s="33">
         <v>3</v>
       </c>
-    </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.15">
-      <c r="A7" t="s">
+      <c r="G6" s="33">
+        <v>65</v>
+      </c>
+      <c r="H6" s="33">
+        <v>3</v>
+      </c>
+      <c r="I6" s="40">
+        <v>42080</v>
+      </c>
+      <c r="J6" s="33" t="s">
+        <v>235</v>
+      </c>
+      <c r="K6" s="33" t="s">
+        <v>264</v>
+      </c>
+      <c r="L6" s="33" t="s">
+        <v>265</v>
+      </c>
+      <c r="N6" s="33" t="s">
+        <v>237</v>
+      </c>
+      <c r="O6" s="33" t="s">
+        <v>266</v>
+      </c>
+      <c r="P6" s="33">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A7" s="33" t="s">
         <v>138</v>
       </c>
-      <c r="B7" s="16" t="s">
+      <c r="B7" s="33" t="s">
         <v>94</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="33" t="s">
         <v>182</v>
       </c>
-      <c r="E7">
+      <c r="E7" s="33">
         <v>30</v>
       </c>
-      <c r="F7">
+      <c r="F7" s="33">
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.15">
-      <c r="A8" t="s">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A8" s="33" t="s">
         <v>139</v>
       </c>
-      <c r="B8" s="16" t="s">
+      <c r="B8" s="33" t="s">
         <v>95</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" s="33" t="s">
         <v>182</v>
       </c>
-      <c r="E8">
+      <c r="E8" s="33">
         <v>30</v>
       </c>
-      <c r="F8">
+      <c r="F8" s="33">
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.15">
-      <c r="A9" t="s">
+    <row r="9" spans="1:16" ht="25.2" x14ac:dyDescent="0.2">
+      <c r="A9" s="33" t="s">
         <v>140</v>
       </c>
-      <c r="B9" s="16" t="s">
+      <c r="B9" s="33" t="s">
         <v>96</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" s="33" t="s">
         <v>195</v>
       </c>
-      <c r="E9">
+      <c r="D9" s="16" t="s">
+        <v>228</v>
+      </c>
+      <c r="E9" s="33">
         <v>15</v>
       </c>
-      <c r="F9">
+      <c r="F9" s="33">
         <v>1</v>
+      </c>
+      <c r="G9" s="33">
+        <v>53</v>
+      </c>
+      <c r="H9" s="33">
+        <v>1</v>
+      </c>
+      <c r="I9" s="40">
+        <v>42080</v>
+      </c>
+      <c r="J9" s="33" t="s">
+        <v>235</v>
+      </c>
+      <c r="K9" s="33" t="s">
+        <v>267</v>
+      </c>
+      <c r="L9" s="33">
+        <v>53</v>
+      </c>
+      <c r="N9" s="33" t="s">
+        <v>237</v>
+      </c>
+      <c r="O9" s="33" t="s">
+        <v>268</v>
+      </c>
+      <c r="P9" s="33">
+        <v>41</v>
       </c>
     </row>
   </sheetData>
@@ -4461,16 +4545,16 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I1"/>
   <sheetViews>
     <sheetView zoomScale="150" workbookViewId="0">
       <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:9" ht="28" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:9" ht="25.2" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>3</v>
       </c>
@@ -4506,20 +4590,20 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C43"/>
   <sheetViews>
     <sheetView topLeftCell="A8" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="28.1640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="49.5" style="1" customWidth="1"/>
+    <col min="2" max="2" width="28.1796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="49.453125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="4" customFormat="1" ht="14" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>108</v>
       </c>
@@ -4530,7 +4614,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>109</v>
       </c>
@@ -4541,7 +4625,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="17" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>110</v>
       </c>
@@ -4552,7 +4636,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="17" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>111</v>
       </c>
@@ -4563,7 +4647,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>112</v>
       </c>
@@ -4574,7 +4658,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="17" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>113</v>
       </c>
@@ -4585,7 +4669,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="17" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>114</v>
       </c>
@@ -4596,7 +4680,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="51" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:3" ht="45" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>115</v>
       </c>
@@ -4607,7 +4691,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>116</v>
       </c>
@@ -4618,7 +4702,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>117</v>
       </c>
@@ -4629,7 +4713,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>118</v>
       </c>
@@ -4640,7 +4724,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>119</v>
       </c>
@@ -4651,7 +4735,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="51" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:3" ht="45" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>120</v>
       </c>
@@ -4662,7 +4746,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="68" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:3" ht="45" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>121</v>
       </c>
@@ -4673,7 +4757,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>122</v>
       </c>
@@ -4684,7 +4768,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="17" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>123</v>
       </c>
@@ -4695,7 +4779,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>124</v>
       </c>
@@ -4706,7 +4790,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="17" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>125</v>
       </c>
@@ -4717,7 +4801,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="17" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>126</v>
       </c>
@@ -4728,7 +4812,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="17" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>127</v>
       </c>
@@ -4739,7 +4823,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>128</v>
       </c>
@@ -4750,7 +4834,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>129</v>
       </c>
@@ -4761,7 +4845,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>130</v>
       </c>
@@ -4772,7 +4856,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>131</v>
       </c>
@@ -4783,7 +4867,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="51" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>132</v>
       </c>
@@ -4794,7 +4878,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>133</v>
       </c>
@@ -4805,7 +4889,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="136" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:3" ht="105" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>134</v>
       </c>
@@ -4816,7 +4900,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>135</v>
       </c>
@@ -4827,7 +4911,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>136</v>
       </c>
@@ -4838,7 +4922,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="30" spans="1:3" ht="17" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>137</v>
       </c>
@@ -4849,7 +4933,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="31" spans="1:3" ht="17" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>138</v>
       </c>
@@ -4860,7 +4944,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>139</v>
       </c>
@@ -4871,7 +4955,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="33" spans="1:3" ht="17" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>140</v>
       </c>
@@ -4882,7 +4966,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="34" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>141</v>
       </c>
@@ -4893,7 +4977,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="35" spans="1:3" ht="51" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>142</v>
       </c>
@@ -4904,7 +4988,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="36" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>143</v>
       </c>
@@ -4915,7 +4999,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="37" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>144</v>
       </c>
@@ -4926,7 +5010,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="38" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>145</v>
       </c>
@@ -4937,7 +5021,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="39" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+    <row r="39" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>146</v>
       </c>
@@ -4948,7 +5032,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="40" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+    <row r="40" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>147</v>
       </c>
@@ -4959,7 +5043,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="41" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+    <row r="41" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>148</v>
       </c>
@@ -4970,7 +5054,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="42" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+    <row r="42" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>149</v>
       </c>
@@ -4981,7 +5065,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="43" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+    <row r="43" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>150</v>
       </c>

</xml_diff>

<commit_message>
Update the report and add stories in ged file
</commit_message>
<xml_diff>
--- a/TeamDReport copy.xlsx
+++ b/TeamDReport copy.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10709"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10309"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/michaelramos/SSW555-DriverlessCar/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/franklin/SSW555/SSW555-DriverlessCar/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2F21563-9A60-044B-90AA-939AAE3435FC}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8F346CF-EDB5-C843-AAC2-A334027392BD}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="23040" windowHeight="14400" tabRatio="500" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,10 +23,16 @@
     <sheet name="Sprint4" sheetId="6" r:id="rId8"/>
     <sheet name="Stories" sheetId="11" r:id="rId9"/>
   </sheets>
-  <calcPr calcId="179021"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="330"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
     </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -36,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="568" uniqueCount="273">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="576" uniqueCount="281">
   <si>
     <t>Date</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -890,6 +896,30 @@
   </si>
   <si>
     <t>test_living_marital_status_no_div_no_death, test_living_marital_status_no_div_death, test_living_marital_status_div_no_death, test_living_marital_status_div_death</t>
+  </si>
+  <si>
+    <t>siblings_not_too_many.py</t>
+  </si>
+  <si>
+    <t>siblings_not_too_many</t>
+  </si>
+  <si>
+    <t>test_siblings_not_too_many.py</t>
+  </si>
+  <si>
+    <t>test_valid_siblings_num, test_siblings_more_than_15</t>
+  </si>
+  <si>
+    <t>siblings_not_marry.py</t>
+  </si>
+  <si>
+    <t>siblings_not_marry</t>
+  </si>
+  <si>
+    <t>test_siblings_not_marry.py</t>
+  </si>
+  <si>
+    <t>test_valid, test_invalid</t>
   </si>
 </sst>
 </file>
@@ -2416,7 +2446,7 @@
       </c>
     </row>
   </sheetData>
-  <sortState ref="A4:D6">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A4:D6">
     <sortCondition ref="C4:C6"/>
   </sortState>
   <phoneticPr fontId="2" type="noConversion"/>
@@ -2467,7 +2497,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="32" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:5" ht="34" x14ac:dyDescent="0.15">
       <c r="A2" s="16" t="s">
         <v>109</v>
       </c>
@@ -2484,7 +2514,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="32" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:5" ht="34" x14ac:dyDescent="0.15">
       <c r="A3" s="16" t="s">
         <v>110</v>
       </c>
@@ -2501,7 +2531,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="32" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:5" ht="34" x14ac:dyDescent="0.15">
       <c r="A4" s="16" t="s">
         <v>111</v>
       </c>
@@ -2518,7 +2548,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="48" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:5" ht="51" x14ac:dyDescent="0.15">
       <c r="A5" s="16" t="s">
         <v>112</v>
       </c>
@@ -2535,7 +2565,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="32" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:5" ht="34" x14ac:dyDescent="0.15">
       <c r="A6" s="16" t="s">
         <v>113</v>
       </c>
@@ -2552,7 +2582,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="32" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:5" ht="34" x14ac:dyDescent="0.15">
       <c r="A7" s="16" t="s">
         <v>114</v>
       </c>
@@ -2569,7 +2599,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="64" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:5" ht="68" x14ac:dyDescent="0.15">
       <c r="A8" s="16" t="s">
         <v>115</v>
       </c>
@@ -2586,7 +2616,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="48" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:5" ht="51" x14ac:dyDescent="0.15">
       <c r="A9" s="16" t="s">
         <v>116</v>
       </c>
@@ -2603,7 +2633,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="48" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:5" ht="51" x14ac:dyDescent="0.15">
       <c r="A10" s="16" t="s">
         <v>117</v>
       </c>
@@ -2620,7 +2650,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="48" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:5" ht="51" x14ac:dyDescent="0.15">
       <c r="A11" s="16" t="s">
         <v>118</v>
       </c>
@@ -2637,7 +2667,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="32" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:5" ht="34" x14ac:dyDescent="0.15">
       <c r="A12" s="16" t="s">
         <v>119</v>
       </c>
@@ -2654,7 +2684,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="64" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:5" ht="68" x14ac:dyDescent="0.15">
       <c r="A13" s="16" t="s">
         <v>120</v>
       </c>
@@ -2671,7 +2701,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="80" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:5" ht="85" x14ac:dyDescent="0.15">
       <c r="A14" s="16" t="s">
         <v>121</v>
       </c>
@@ -2688,7 +2718,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="32" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:5" ht="34" x14ac:dyDescent="0.15">
       <c r="A15" s="16" t="s">
         <v>122</v>
       </c>
@@ -2705,7 +2735,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="32" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:5" ht="34" x14ac:dyDescent="0.15">
       <c r="A16" s="16" t="s">
         <v>123</v>
       </c>
@@ -2722,7 +2752,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="32" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:5" ht="34" x14ac:dyDescent="0.15">
       <c r="A17" s="16" t="s">
         <v>124</v>
       </c>
@@ -2739,7 +2769,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="32" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:5" ht="34" x14ac:dyDescent="0.15">
       <c r="A18" s="16" t="s">
         <v>125</v>
       </c>
@@ -2756,7 +2786,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="32" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:5" ht="34" x14ac:dyDescent="0.15">
       <c r="A19" s="16" t="s">
         <v>126</v>
       </c>
@@ -2773,7 +2803,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="32" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:5" ht="34" x14ac:dyDescent="0.15">
       <c r="A20" s="16" t="s">
         <v>127</v>
       </c>
@@ -2784,7 +2814,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="32" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:5" ht="34" x14ac:dyDescent="0.15">
       <c r="A21" s="16" t="s">
         <v>128</v>
       </c>
@@ -2795,7 +2825,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="22" spans="1:5" ht="32" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:5" ht="34" x14ac:dyDescent="0.15">
       <c r="A22" s="16" t="s">
         <v>130</v>
       </c>
@@ -2806,7 +2836,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="23" spans="1:5" ht="48" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:5" ht="51" x14ac:dyDescent="0.15">
       <c r="A23" s="16" t="s">
         <v>131</v>
       </c>
@@ -2817,7 +2847,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="24" spans="1:5" ht="64" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:5" ht="68" x14ac:dyDescent="0.15">
       <c r="A24" s="16" t="s">
         <v>132</v>
       </c>
@@ -2828,7 +2858,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="25" spans="1:5" ht="48" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:5" ht="51" x14ac:dyDescent="0.15">
       <c r="A25" s="16" t="s">
         <v>133</v>
       </c>
@@ -2839,7 +2869,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="26" spans="1:5" ht="32" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:5" ht="34" x14ac:dyDescent="0.15">
       <c r="A26" s="16" t="s">
         <v>135</v>
       </c>
@@ -2850,7 +2880,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="27" spans="1:5" ht="32" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:5" ht="34" x14ac:dyDescent="0.15">
       <c r="A27" s="16" t="s">
         <v>136</v>
       </c>
@@ -2867,7 +2897,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="28" spans="1:5" ht="32" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:5" ht="34" x14ac:dyDescent="0.15">
       <c r="A28" s="16" t="s">
         <v>137</v>
       </c>
@@ -2878,7 +2908,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="29" spans="1:5" ht="32" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:5" ht="34" x14ac:dyDescent="0.15">
       <c r="A29" s="16" t="s">
         <v>138</v>
       </c>
@@ -2895,7 +2925,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="30" spans="1:5" ht="32" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:5" ht="34" x14ac:dyDescent="0.15">
       <c r="A30" s="16" t="s">
         <v>139</v>
       </c>
@@ -2912,7 +2942,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="31" spans="1:5" ht="32" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:5" ht="34" x14ac:dyDescent="0.15">
       <c r="A31" s="16" t="s">
         <v>140</v>
       </c>
@@ -2929,7 +2959,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="32" spans="1:5" ht="32" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:5" ht="34" x14ac:dyDescent="0.15">
       <c r="A32" s="16" t="s">
         <v>149</v>
       </c>
@@ -2946,7 +2976,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="33" spans="1:5" ht="48" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:5" ht="51" x14ac:dyDescent="0.15">
       <c r="A33" s="16" t="s">
         <v>150</v>
       </c>
@@ -3303,7 +3333,7 @@
     <col min="17" max="16384" width="10.83203125" style="16"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:16" ht="14" x14ac:dyDescent="0.15">
       <c r="A1" s="15" t="s">
         <v>9</v>
       </c>
@@ -3350,7 +3380,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="2" spans="1:16" ht="26" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:16" ht="28" x14ac:dyDescent="0.15">
       <c r="A2" s="16" t="s">
         <v>109</v>
       </c>
@@ -3397,7 +3427,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:16" ht="26" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:16" ht="28" x14ac:dyDescent="0.15">
       <c r="A3" s="16" t="s">
         <v>110</v>
       </c>
@@ -3444,7 +3474,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:16" ht="26" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:16" ht="28" x14ac:dyDescent="0.15">
       <c r="A4" s="16" t="s">
         <v>111</v>
       </c>
@@ -3491,7 +3521,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="5" spans="1:16" ht="26" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:16" ht="28" x14ac:dyDescent="0.15">
       <c r="A5" s="16" t="s">
         <v>112</v>
       </c>
@@ -3538,7 +3568,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="6" spans="1:16" ht="26" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:16" ht="28" x14ac:dyDescent="0.15">
       <c r="A6" s="16" t="s">
         <v>113</v>
       </c>
@@ -3585,7 +3615,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:16" ht="26" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:16" ht="28" x14ac:dyDescent="0.15">
       <c r="A7" s="16" t="s">
         <v>114</v>
       </c>
@@ -3632,7 +3662,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:16" ht="39" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:16" ht="42" x14ac:dyDescent="0.15">
       <c r="A8" s="16" t="s">
         <v>118</v>
       </c>
@@ -3679,7 +3709,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="9" spans="1:16" ht="26" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:16" ht="28" x14ac:dyDescent="0.15">
       <c r="A9" s="16" t="s">
         <v>119</v>
       </c>
@@ -3734,7 +3764,7 @@
       <c r="O10" s="28"/>
       <c r="P10" s="27"/>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:16" ht="14" x14ac:dyDescent="0.15">
       <c r="B13" s="20" t="s">
         <v>200</v>
       </c>
@@ -3742,12 +3772,12 @@
     <row r="14" spans="1:16" x14ac:dyDescent="0.15">
       <c r="B14" s="30"/>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:16" ht="14" x14ac:dyDescent="0.15">
       <c r="B15" s="31" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="16" spans="1:16" ht="22" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:16" ht="24" x14ac:dyDescent="0.15">
       <c r="B16" s="32" t="s">
         <v>230</v>
       </c>
@@ -3755,17 +3785,17 @@
     <row r="17" spans="2:2" x14ac:dyDescent="0.15">
       <c r="B17" s="20"/>
     </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.15">
+    <row r="18" spans="2:2" ht="14" x14ac:dyDescent="0.15">
       <c r="B18" s="31" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="19" spans="2:2" ht="66" x14ac:dyDescent="0.15">
+    <row r="19" spans="2:2" ht="72" x14ac:dyDescent="0.15">
       <c r="B19" s="32" t="s">
         <v>229</v>
       </c>
     </row>
-    <row r="21" spans="2:2" x14ac:dyDescent="0.15">
+    <row r="21" spans="2:2" ht="14" x14ac:dyDescent="0.15">
       <c r="B21" s="31" t="s">
         <v>203</v>
       </c>
@@ -3852,7 +3882,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="2" spans="1:16" s="37" customFormat="1" ht="78" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:16" s="37" customFormat="1" ht="84" x14ac:dyDescent="0.15">
       <c r="A2" s="37" t="s">
         <v>115</v>
       </c>
@@ -3899,7 +3929,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="3" spans="1:16" s="37" customFormat="1" ht="91" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:16" s="37" customFormat="1" ht="98" x14ac:dyDescent="0.15">
       <c r="A3" s="37" t="s">
         <v>116</v>
       </c>
@@ -3946,7 +3976,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="4" spans="1:16" s="37" customFormat="1" ht="39" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:16" s="37" customFormat="1" ht="42" x14ac:dyDescent="0.15">
       <c r="A4" s="37" t="s">
         <v>117</v>
       </c>
@@ -3993,7 +4023,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:16" s="37" customFormat="1" ht="26" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:16" s="37" customFormat="1" ht="28" x14ac:dyDescent="0.15">
       <c r="A5" s="37" t="s">
         <v>120</v>
       </c>
@@ -4040,7 +4070,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:16" s="37" customFormat="1" ht="26" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:16" s="37" customFormat="1" ht="28" x14ac:dyDescent="0.15">
       <c r="A6" s="37" t="s">
         <v>121</v>
       </c>
@@ -4087,7 +4117,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:16" s="37" customFormat="1" ht="39" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:16" s="37" customFormat="1" ht="42" x14ac:dyDescent="0.15">
       <c r="A7" s="37" t="s">
         <v>122</v>
       </c>
@@ -4134,7 +4164,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="8" spans="1:16" s="37" customFormat="1" ht="26" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:16" s="37" customFormat="1" ht="28" x14ac:dyDescent="0.15">
       <c r="A8" s="37" t="s">
         <v>149</v>
       </c>
@@ -4181,7 +4211,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:16" s="37" customFormat="1" ht="26" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:16" s="37" customFormat="1" ht="28" x14ac:dyDescent="0.15">
       <c r="A9" s="37" t="s">
         <v>150</v>
       </c>
@@ -4232,7 +4262,7 @@
     <row r="11" spans="1:16" s="37" customFormat="1" x14ac:dyDescent="0.15"/>
     <row r="12" spans="1:16" s="37" customFormat="1" x14ac:dyDescent="0.15"/>
     <row r="13" spans="1:16" s="37" customFormat="1" x14ac:dyDescent="0.15"/>
-    <row r="14" spans="1:16" s="37" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:16" s="37" customFormat="1" ht="14" x14ac:dyDescent="0.15">
       <c r="B14" s="20" t="s">
         <v>200</v>
       </c>
@@ -4240,12 +4270,12 @@
     <row r="15" spans="1:16" s="37" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B15" s="30"/>
     </row>
-    <row r="16" spans="1:16" s="37" customFormat="1" ht="26" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:16" s="37" customFormat="1" ht="28" x14ac:dyDescent="0.15">
       <c r="B16" s="31" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="17" spans="2:2" s="37" customFormat="1" ht="22" x14ac:dyDescent="0.15">
+    <row r="17" spans="2:2" s="37" customFormat="1" ht="24" x14ac:dyDescent="0.15">
       <c r="B17" s="32" t="s">
         <v>262</v>
       </c>
@@ -4253,12 +4283,12 @@
     <row r="18" spans="2:2" s="37" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B18" s="20"/>
     </row>
-    <row r="19" spans="2:2" s="37" customFormat="1" ht="26" x14ac:dyDescent="0.15">
+    <row r="19" spans="2:2" s="37" customFormat="1" ht="28" x14ac:dyDescent="0.15">
       <c r="B19" s="31" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="20" spans="2:2" s="37" customFormat="1" ht="66" x14ac:dyDescent="0.15">
+    <row r="20" spans="2:2" s="37" customFormat="1" ht="72" x14ac:dyDescent="0.15">
       <c r="B20" s="32" t="s">
         <v>263</v>
       </c>
@@ -4266,12 +4296,12 @@
     <row r="21" spans="2:2" x14ac:dyDescent="0.15">
       <c r="B21" s="18"/>
     </row>
-    <row r="22" spans="2:2" x14ac:dyDescent="0.15">
+    <row r="22" spans="2:2" ht="14" x14ac:dyDescent="0.15">
       <c r="B22" s="31" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="23" spans="2:2" ht="33" x14ac:dyDescent="0.15">
+    <row r="23" spans="2:2" ht="36" x14ac:dyDescent="0.15">
       <c r="B23" s="32" t="s">
         <v>261</v>
       </c>
@@ -4287,8 +4317,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:P9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="150" workbookViewId="0">
-      <selection activeCell="P9" sqref="P9"/>
+    <sheetView tabSelected="1" zoomScale="90" workbookViewId="0">
+      <selection activeCell="P5" sqref="P5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -4349,7 +4379,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:16" ht="84" x14ac:dyDescent="0.15">
       <c r="A2" s="33" t="s">
         <v>123</v>
       </c>
@@ -4365,8 +4395,35 @@
       <c r="F2" s="33">
         <v>2</v>
       </c>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="G2" s="33">
+        <v>12</v>
+      </c>
+      <c r="H2" s="33">
+        <v>1</v>
+      </c>
+      <c r="I2" s="40">
+        <v>42092</v>
+      </c>
+      <c r="J2" s="33" t="s">
+        <v>273</v>
+      </c>
+      <c r="K2" s="33" t="s">
+        <v>274</v>
+      </c>
+      <c r="L2" s="33">
+        <v>15</v>
+      </c>
+      <c r="N2" s="33" t="s">
+        <v>275</v>
+      </c>
+      <c r="O2" s="33" t="s">
+        <v>276</v>
+      </c>
+      <c r="P2" s="33">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" ht="14" x14ac:dyDescent="0.15">
       <c r="A3" s="33" t="s">
         <v>124</v>
       </c>
@@ -4383,7 +4440,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:16" ht="14" x14ac:dyDescent="0.15">
       <c r="A4" s="33" t="s">
         <v>125</v>
       </c>
@@ -4400,7 +4457,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:16" ht="42" x14ac:dyDescent="0.15">
       <c r="A5" s="33" t="s">
         <v>126</v>
       </c>
@@ -4416,8 +4473,35 @@
       <c r="F5" s="33">
         <v>2</v>
       </c>
-    </row>
-    <row r="6" spans="1:16" ht="39" x14ac:dyDescent="0.15">
+      <c r="G5" s="33">
+        <v>18</v>
+      </c>
+      <c r="H5" s="33">
+        <v>2</v>
+      </c>
+      <c r="I5" s="40">
+        <v>42092</v>
+      </c>
+      <c r="J5" s="33" t="s">
+        <v>277</v>
+      </c>
+      <c r="K5" s="33" t="s">
+        <v>278</v>
+      </c>
+      <c r="L5" s="33">
+        <v>18</v>
+      </c>
+      <c r="N5" s="33" t="s">
+        <v>279</v>
+      </c>
+      <c r="O5" s="33" t="s">
+        <v>280</v>
+      </c>
+      <c r="P5" s="33">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" ht="42" x14ac:dyDescent="0.15">
       <c r="A6" s="33" t="s">
         <v>136</v>
       </c>
@@ -4464,7 +4548,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="7" spans="1:16" ht="208" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:16" ht="224" x14ac:dyDescent="0.15">
       <c r="A7" s="33" t="s">
         <v>138</v>
       </c>
@@ -4508,7 +4592,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="8" spans="1:16" ht="208" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:16" ht="224" x14ac:dyDescent="0.15">
       <c r="A8" s="33" t="s">
         <v>139</v>
       </c>
@@ -4552,7 +4636,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="9" spans="1:16" ht="39" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:16" ht="42" x14ac:dyDescent="0.15">
       <c r="A9" s="33" t="s">
         <v>140</v>
       </c>
@@ -4615,7 +4699,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <sheetData>
-    <row r="1" spans="1:9" ht="26" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:9" ht="28" x14ac:dyDescent="0.15">
       <c r="A1" s="4" t="s">
         <v>3</v>
       </c>
@@ -4664,7 +4748,7 @@
     <col min="3" max="3" width="49.5" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:3" s="4" customFormat="1" ht="14" x14ac:dyDescent="0.15">
       <c r="A1" s="4" t="s">
         <v>108</v>
       </c>
@@ -4675,7 +4759,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="32" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:3" ht="34" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
         <v>109</v>
       </c>
@@ -4686,7 +4770,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="16" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:3" ht="17" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
         <v>110</v>
       </c>
@@ -4697,7 +4781,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="16" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:3" ht="17" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
         <v>111</v>
       </c>
@@ -4708,7 +4792,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="32" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:3" ht="34" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
         <v>112</v>
       </c>
@@ -4719,7 +4803,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="16" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:3" ht="17" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
         <v>113</v>
       </c>
@@ -4730,7 +4814,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="16" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:3" ht="17" x14ac:dyDescent="0.15">
       <c r="A7" t="s">
         <v>114</v>
       </c>
@@ -4741,7 +4825,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="48" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:3" ht="51" x14ac:dyDescent="0.15">
       <c r="A8" t="s">
         <v>115</v>
       </c>
@@ -4752,7 +4836,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="32" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:3" ht="34" x14ac:dyDescent="0.15">
       <c r="A9" t="s">
         <v>116</v>
       </c>
@@ -4763,7 +4847,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="32" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:3" ht="34" x14ac:dyDescent="0.15">
       <c r="A10" t="s">
         <v>117</v>
       </c>
@@ -4774,7 +4858,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="32" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:3" ht="34" x14ac:dyDescent="0.15">
       <c r="A11" t="s">
         <v>118</v>
       </c>
@@ -4785,7 +4869,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="32" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:3" ht="34" x14ac:dyDescent="0.15">
       <c r="A12" t="s">
         <v>119</v>
       </c>
@@ -4796,7 +4880,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="48" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:3" ht="51" x14ac:dyDescent="0.15">
       <c r="A13" t="s">
         <v>120</v>
       </c>
@@ -4807,7 +4891,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="64" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:3" ht="68" x14ac:dyDescent="0.15">
       <c r="A14" t="s">
         <v>121</v>
       </c>
@@ -4818,7 +4902,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="32" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:3" ht="34" x14ac:dyDescent="0.15">
       <c r="A15" t="s">
         <v>122</v>
       </c>
@@ -4829,7 +4913,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="16" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:3" ht="17" x14ac:dyDescent="0.15">
       <c r="A16" t="s">
         <v>123</v>
       </c>
@@ -4840,7 +4924,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="32" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:3" ht="34" x14ac:dyDescent="0.15">
       <c r="A17" t="s">
         <v>124</v>
       </c>
@@ -4851,7 +4935,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="16" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:3" ht="17" x14ac:dyDescent="0.15">
       <c r="A18" t="s">
         <v>125</v>
       </c>
@@ -4862,7 +4946,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="16" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:3" ht="17" x14ac:dyDescent="0.15">
       <c r="A19" t="s">
         <v>126</v>
       </c>
@@ -4873,7 +4957,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="16" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:3" ht="17" x14ac:dyDescent="0.15">
       <c r="A20" t="s">
         <v>127</v>
       </c>
@@ -4884,7 +4968,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="32" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:3" ht="34" x14ac:dyDescent="0.15">
       <c r="A21" t="s">
         <v>128</v>
       </c>
@@ -4895,7 +4979,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="32" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:3" ht="34" x14ac:dyDescent="0.15">
       <c r="A22" t="s">
         <v>129</v>
       </c>
@@ -4906,7 +4990,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="32" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:3" ht="34" x14ac:dyDescent="0.15">
       <c r="A23" t="s">
         <v>130</v>
       </c>
@@ -4917,7 +5001,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="32" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:3" ht="34" x14ac:dyDescent="0.15">
       <c r="A24" t="s">
         <v>131</v>
       </c>
@@ -4928,7 +5012,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="48" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:3" ht="51" x14ac:dyDescent="0.15">
       <c r="A25" t="s">
         <v>132</v>
       </c>
@@ -4939,7 +5023,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="32" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:3" ht="34" x14ac:dyDescent="0.15">
       <c r="A26" t="s">
         <v>133</v>
       </c>
@@ -4950,7 +5034,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="128" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:3" ht="136" x14ac:dyDescent="0.15">
       <c r="A27" t="s">
         <v>134</v>
       </c>
@@ -4961,7 +5045,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="32" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:3" ht="34" x14ac:dyDescent="0.15">
       <c r="A28" t="s">
         <v>135</v>
       </c>
@@ -4972,7 +5056,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="32" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:3" ht="34" x14ac:dyDescent="0.15">
       <c r="A29" t="s">
         <v>136</v>
       </c>
@@ -4983,7 +5067,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="30" spans="1:3" ht="16" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:3" ht="17" x14ac:dyDescent="0.15">
       <c r="A30" t="s">
         <v>137</v>
       </c>
@@ -4994,7 +5078,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="31" spans="1:3" ht="16" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:3" ht="17" x14ac:dyDescent="0.15">
       <c r="A31" t="s">
         <v>138</v>
       </c>
@@ -5005,7 +5089,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="32" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:3" ht="34" x14ac:dyDescent="0.15">
       <c r="A32" t="s">
         <v>139</v>
       </c>
@@ -5016,7 +5100,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="33" spans="1:3" ht="16" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:3" ht="17" x14ac:dyDescent="0.15">
       <c r="A33" t="s">
         <v>140</v>
       </c>
@@ -5027,7 +5111,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="34" spans="1:3" ht="32" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:3" ht="34" x14ac:dyDescent="0.15">
       <c r="A34" t="s">
         <v>141</v>
       </c>
@@ -5038,7 +5122,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="35" spans="1:3" ht="48" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:3" ht="51" x14ac:dyDescent="0.15">
       <c r="A35" t="s">
         <v>142</v>
       </c>
@@ -5049,7 +5133,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="36" spans="1:3" ht="32" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:3" ht="34" x14ac:dyDescent="0.15">
       <c r="A36" t="s">
         <v>143</v>
       </c>
@@ -5060,7 +5144,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="37" spans="1:3" ht="32" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:3" ht="34" x14ac:dyDescent="0.15">
       <c r="A37" t="s">
         <v>144</v>
       </c>
@@ -5071,7 +5155,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="38" spans="1:3" ht="32" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:3" ht="34" x14ac:dyDescent="0.15">
       <c r="A38" t="s">
         <v>145</v>
       </c>
@@ -5082,7 +5166,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="39" spans="1:3" ht="32" x14ac:dyDescent="0.15">
+    <row r="39" spans="1:3" ht="34" x14ac:dyDescent="0.15">
       <c r="A39" t="s">
         <v>146</v>
       </c>
@@ -5093,7 +5177,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="40" spans="1:3" ht="32" x14ac:dyDescent="0.15">
+    <row r="40" spans="1:3" ht="34" x14ac:dyDescent="0.15">
       <c r="A40" t="s">
         <v>147</v>
       </c>
@@ -5104,7 +5188,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="41" spans="1:3" ht="32" x14ac:dyDescent="0.15">
+    <row r="41" spans="1:3" ht="34" x14ac:dyDescent="0.15">
       <c r="A41" t="s">
         <v>148</v>
       </c>
@@ -5115,7 +5199,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="42" spans="1:3" ht="32" x14ac:dyDescent="0.15">
+    <row r="42" spans="1:3" ht="34" x14ac:dyDescent="0.15">
       <c r="A42" t="s">
         <v>149</v>
       </c>
@@ -5126,7 +5210,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="43" spans="1:3" ht="32" x14ac:dyDescent="0.15">
+    <row r="43" spans="1:3" ht="34" x14ac:dyDescent="0.15">
       <c r="A43" t="s">
         <v>150</v>
       </c>

</xml_diff>

<commit_message>
Revert "US16 & US17"
This reverts commit a9c27d473f0f52b77f0157a0d9cff2df42d746ac.
</commit_message>
<xml_diff>
--- a/TeamDReport copy.xlsx
+++ b/TeamDReport copy.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20730"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Funbucket24\Documents\GitHub\SSW555-DriverlessCar\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Code_Modeling\Python\SSW_555\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E81BB062-2A9C-46F0-A103-367BD2946592}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="14400" tabRatio="500" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="14400" tabRatio="500" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Team" sheetId="1" r:id="rId1"/>
@@ -23,7 +22,7 @@
     <sheet name="Sprint4" sheetId="6" r:id="rId8"/>
     <sheet name="Stories" sheetId="11" r:id="rId9"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="330"/>
@@ -31,6 +30,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
       </xcalcf:calcFeatures>
     </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="570" uniqueCount="277">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="560" uniqueCount="269">
   <si>
     <t>Date</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -883,36 +883,12 @@
   </si>
   <si>
     <t>test_list_multiple_births</t>
-  </si>
-  <si>
-    <t>male_last_names.py</t>
-  </si>
-  <si>
-    <t>no_marriage_to_children.py</t>
-  </si>
-  <si>
-    <t>check_all_male_last_names</t>
-  </si>
-  <si>
-    <t>no_marriage_to_children</t>
-  </si>
-  <si>
-    <t>TestMaleLastName.py</t>
-  </si>
-  <si>
-    <t>TestMarriageToChildren.py</t>
-  </si>
-  <si>
-    <t>TestMaleNames</t>
-  </si>
-  <si>
-    <t>TestSameFamilyChildrenMarriage</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="m/d"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
@@ -2324,19 +2300,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView zoomScale="150" workbookViewId="0">
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="7.875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.5" customWidth="1"/>
-    <col min="4" max="5" width="20.5" customWidth="1"/>
+    <col min="1" max="1" width="7.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.6328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.453125" customWidth="1"/>
+    <col min="4" max="5" width="20.453125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
@@ -2438,11 +2414,11 @@
   </sortState>
   <phoneticPr fontId="2" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="D4" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="D3" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
-    <hyperlink ref="D2" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
-    <hyperlink ref="D5" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
-    <hyperlink ref="E10" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="D4" r:id="rId1"/>
+    <hyperlink ref="D3" r:id="rId2"/>
+    <hyperlink ref="D2" r:id="rId3"/>
+    <hyperlink ref="D5" r:id="rId4"/>
+    <hyperlink ref="E10" r:id="rId5"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -2450,21 +2426,21 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E33"/>
   <sheetViews>
-    <sheetView topLeftCell="A12" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView topLeftCell="A24" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="E31" sqref="E31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="6.875" style="16" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="29.125" style="16" customWidth="1"/>
-    <col min="3" max="3" width="34.5" style="16" customWidth="1"/>
-    <col min="4" max="4" width="6.625" style="16" customWidth="1"/>
-    <col min="5" max="5" width="10.375" style="16" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="10.875" style="16"/>
+    <col min="1" max="1" width="6.81640625" style="16" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="29.1796875" style="16" customWidth="1"/>
+    <col min="3" max="3" width="34.453125" style="16" customWidth="1"/>
+    <col min="4" max="4" width="6.6328125" style="16" customWidth="1"/>
+    <col min="5" max="5" width="10.36328125" style="16" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="10.81640625" style="16"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" s="15" customFormat="1" x14ac:dyDescent="0.2">
@@ -2484,7 +2460,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" ht="30" x14ac:dyDescent="0.2">
       <c r="A2" s="16" t="s">
         <v>109</v>
       </c>
@@ -2501,7 +2477,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" ht="30" x14ac:dyDescent="0.2">
       <c r="A3" s="16" t="s">
         <v>110</v>
       </c>
@@ -2518,7 +2494,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" ht="30" x14ac:dyDescent="0.2">
       <c r="A4" s="16" t="s">
         <v>111</v>
       </c>
@@ -2535,7 +2511,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="47.25" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" ht="45" x14ac:dyDescent="0.2">
       <c r="A5" s="16" t="s">
         <v>112</v>
       </c>
@@ -2552,7 +2528,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" ht="30" x14ac:dyDescent="0.2">
       <c r="A6" s="16" t="s">
         <v>113</v>
       </c>
@@ -2569,7 +2545,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" ht="30" x14ac:dyDescent="0.2">
       <c r="A7" s="16" t="s">
         <v>114</v>
       </c>
@@ -2586,7 +2562,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="63" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" ht="60" x14ac:dyDescent="0.2">
       <c r="A8" s="16" t="s">
         <v>115</v>
       </c>
@@ -2603,7 +2579,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="47.25" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" ht="45" x14ac:dyDescent="0.2">
       <c r="A9" s="16" t="s">
         <v>116</v>
       </c>
@@ -2620,7 +2596,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="47.25" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5" ht="45" x14ac:dyDescent="0.2">
       <c r="A10" s="16" t="s">
         <v>117</v>
       </c>
@@ -2637,7 +2613,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="47.25" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5" ht="45" x14ac:dyDescent="0.2">
       <c r="A11" s="16" t="s">
         <v>118</v>
       </c>
@@ -2654,7 +2630,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5" ht="30" x14ac:dyDescent="0.2">
       <c r="A12" s="16" t="s">
         <v>119</v>
       </c>
@@ -2671,7 +2647,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="63" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:5" ht="45" x14ac:dyDescent="0.2">
       <c r="A13" s="16" t="s">
         <v>120</v>
       </c>
@@ -2688,7 +2664,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="78.75" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:5" ht="75" x14ac:dyDescent="0.2">
       <c r="A14" s="16" t="s">
         <v>121</v>
       </c>
@@ -2705,7 +2681,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:5" ht="30" x14ac:dyDescent="0.2">
       <c r="A15" s="16" t="s">
         <v>122</v>
       </c>
@@ -2722,7 +2698,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:5" ht="30" x14ac:dyDescent="0.2">
       <c r="A16" s="16" t="s">
         <v>123</v>
       </c>
@@ -2739,7 +2715,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:5" ht="30" x14ac:dyDescent="0.2">
       <c r="A17" s="16" t="s">
         <v>124</v>
       </c>
@@ -2756,7 +2732,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:5" ht="30" x14ac:dyDescent="0.2">
       <c r="A18" s="16" t="s">
         <v>125</v>
       </c>
@@ -2773,7 +2749,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:5" ht="15" x14ac:dyDescent="0.2">
       <c r="A19" s="16" t="s">
         <v>126</v>
       </c>
@@ -2790,7 +2766,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:5" ht="30" x14ac:dyDescent="0.2">
       <c r="A20" s="16" t="s">
         <v>127</v>
       </c>
@@ -2801,7 +2777,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:5" ht="30" x14ac:dyDescent="0.2">
       <c r="A21" s="16" t="s">
         <v>128</v>
       </c>
@@ -2812,7 +2788,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="22" spans="1:5" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:5" ht="30" x14ac:dyDescent="0.2">
       <c r="A22" s="16" t="s">
         <v>130</v>
       </c>
@@ -2823,7 +2799,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="23" spans="1:5" ht="47.25" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:5" ht="45" x14ac:dyDescent="0.2">
       <c r="A23" s="16" t="s">
         <v>131</v>
       </c>
@@ -2834,7 +2810,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="24" spans="1:5" ht="63" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:5" ht="45" x14ac:dyDescent="0.2">
       <c r="A24" s="16" t="s">
         <v>132</v>
       </c>
@@ -2845,7 +2821,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="25" spans="1:5" ht="47.25" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:5" ht="45" x14ac:dyDescent="0.2">
       <c r="A25" s="16" t="s">
         <v>133</v>
       </c>
@@ -2856,7 +2832,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="26" spans="1:5" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:5" ht="30" x14ac:dyDescent="0.2">
       <c r="A26" s="16" t="s">
         <v>135</v>
       </c>
@@ -2867,7 +2843,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="27" spans="1:5" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:5" ht="30" x14ac:dyDescent="0.2">
       <c r="A27" s="16" t="s">
         <v>136</v>
       </c>
@@ -2884,7 +2860,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="28" spans="1:5" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:5" ht="30" x14ac:dyDescent="0.2">
       <c r="A28" s="16" t="s">
         <v>137</v>
       </c>
@@ -2895,7 +2871,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="29" spans="1:5" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:5" ht="30" x14ac:dyDescent="0.2">
       <c r="A29" s="16" t="s">
         <v>138</v>
       </c>
@@ -2912,7 +2888,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="30" spans="1:5" ht="47.25" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:5" ht="30" x14ac:dyDescent="0.2">
       <c r="A30" s="16" t="s">
         <v>139</v>
       </c>
@@ -2929,7 +2905,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="31" spans="1:5" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:5" ht="15" x14ac:dyDescent="0.2">
       <c r="A31" s="16" t="s">
         <v>140</v>
       </c>
@@ -2946,7 +2922,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="32" spans="1:5" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:5" ht="30" x14ac:dyDescent="0.2">
       <c r="A32" s="16" t="s">
         <v>149</v>
       </c>
@@ -2963,7 +2939,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="33" spans="1:5" ht="47.25" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:5" ht="45" x14ac:dyDescent="0.2">
       <c r="A33" s="16" t="s">
         <v>150</v>
       </c>
@@ -2988,21 +2964,21 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G19"/>
   <sheetViews>
     <sheetView topLeftCell="A30" zoomScale="150" workbookViewId="0">
       <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.875" style="2"/>
-    <col min="2" max="2" width="9.5" customWidth="1"/>
-    <col min="3" max="3" width="15.875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.375" customWidth="1"/>
-    <col min="5" max="5" width="6.875" customWidth="1"/>
-    <col min="6" max="6" width="12.5" style="7" customWidth="1"/>
+    <col min="1" max="1" width="10.81640625" style="2"/>
+    <col min="2" max="2" width="9.453125" customWidth="1"/>
+    <col min="3" max="3" width="15.81640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.36328125" customWidth="1"/>
+    <col min="5" max="5" width="6.81640625" customWidth="1"/>
+    <col min="6" max="6" width="12.453125" style="7" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
@@ -3182,21 +3158,21 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView zoomScale="150" workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.875" style="2"/>
-    <col min="2" max="2" width="16.625" customWidth="1"/>
-    <col min="3" max="3" width="14.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.125" customWidth="1"/>
-    <col min="5" max="5" width="6.875" customWidth="1"/>
-    <col min="6" max="6" width="12.5" style="7" customWidth="1"/>
+    <col min="1" max="1" width="10.81640625" style="2"/>
+    <col min="2" max="2" width="16.6328125" customWidth="1"/>
+    <col min="3" max="3" width="14.453125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.1796875" customWidth="1"/>
+    <col min="5" max="5" width="6.81640625" customWidth="1"/>
+    <col min="6" max="6" width="12.453125" style="7" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.2">
@@ -3292,32 +3268,32 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P22"/>
   <sheetViews>
     <sheetView topLeftCell="A10" zoomScale="150" workbookViewId="0">
       <selection activeCell="B13" sqref="B13:B22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="9" style="16" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="24.5" style="18" customWidth="1"/>
-    <col min="3" max="3" width="7.375" style="16" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.625" style="16" customWidth="1"/>
-    <col min="5" max="5" width="8.5" style="16" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.375" style="16" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.625" style="16" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.375" style="16" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.453125" style="18" customWidth="1"/>
+    <col min="3" max="3" width="7.36328125" style="16" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.6328125" style="16" customWidth="1"/>
+    <col min="5" max="5" width="8.453125" style="16" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.36328125" style="16" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.6328125" style="16" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.36328125" style="16" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="11" style="26" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="20.875" style="29" customWidth="1"/>
-    <col min="11" max="11" width="17.875" style="29" customWidth="1"/>
+    <col min="10" max="10" width="20.81640625" style="29" customWidth="1"/>
+    <col min="11" max="11" width="17.81640625" style="29" customWidth="1"/>
     <col min="12" max="12" width="13" style="24" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="1.875" style="24" customWidth="1"/>
-    <col min="14" max="14" width="16.875" style="29" customWidth="1"/>
-    <col min="15" max="15" width="22.875" style="29" customWidth="1"/>
-    <col min="16" max="16" width="10.125" style="24" bestFit="1" customWidth="1"/>
-    <col min="17" max="16384" width="10.875" style="16"/>
+    <col min="13" max="13" width="1.81640625" style="24" customWidth="1"/>
+    <col min="14" max="14" width="16.81640625" style="29" customWidth="1"/>
+    <col min="15" max="15" width="22.81640625" style="29" customWidth="1"/>
+    <col min="16" max="16" width="10.1796875" style="24" bestFit="1" customWidth="1"/>
+    <col min="17" max="16384" width="10.81640625" style="16"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.2">
@@ -3367,7 +3343,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="2" spans="1:16" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:16" ht="25.2" x14ac:dyDescent="0.2">
       <c r="A2" s="16" t="s">
         <v>109</v>
       </c>
@@ -3414,7 +3390,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:16" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:16" ht="25.2" x14ac:dyDescent="0.2">
       <c r="A3" s="16" t="s">
         <v>110</v>
       </c>
@@ -3461,7 +3437,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:16" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:16" ht="25.2" x14ac:dyDescent="0.2">
       <c r="A4" s="16" t="s">
         <v>111</v>
       </c>
@@ -3508,7 +3484,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="5" spans="1:16" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:16" ht="25.2" x14ac:dyDescent="0.2">
       <c r="A5" s="16" t="s">
         <v>112</v>
       </c>
@@ -3555,7 +3531,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="6" spans="1:16" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:16" ht="25.2" x14ac:dyDescent="0.2">
       <c r="A6" s="16" t="s">
         <v>113</v>
       </c>
@@ -3602,7 +3578,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:16" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:16" ht="25.2" x14ac:dyDescent="0.2">
       <c r="A7" s="16" t="s">
         <v>114</v>
       </c>
@@ -3649,7 +3625,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:16" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:16" ht="37.799999999999997" x14ac:dyDescent="0.2">
       <c r="A8" s="16" t="s">
         <v>118</v>
       </c>
@@ -3696,7 +3672,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="9" spans="1:16" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:16" ht="25.2" x14ac:dyDescent="0.2">
       <c r="A9" s="16" t="s">
         <v>119</v>
       </c>
@@ -3764,7 +3740,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="16" spans="1:16" ht="21" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:16" ht="20.399999999999999" x14ac:dyDescent="0.2">
       <c r="B16" s="32" t="s">
         <v>230</v>
       </c>
@@ -3777,7 +3753,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="19" spans="2:2" ht="73.5" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:2" ht="61.2" x14ac:dyDescent="0.2">
       <c r="B19" s="32" t="s">
         <v>229</v>
       </c>
@@ -3800,25 +3776,25 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P23"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.875" style="33"/>
+    <col min="1" max="1" width="10.81640625" style="33"/>
     <col min="2" max="2" width="22" style="33" bestFit="1" customWidth="1"/>
-    <col min="3" max="9" width="10.875" style="33"/>
-    <col min="10" max="10" width="13.875" style="33" customWidth="1"/>
+    <col min="3" max="9" width="10.81640625" style="33"/>
+    <col min="10" max="10" width="13.81640625" style="33" customWidth="1"/>
     <col min="11" max="11" width="16" style="33" customWidth="1"/>
-    <col min="12" max="12" width="15.875" style="33" customWidth="1"/>
-    <col min="13" max="13" width="4.125" style="33" customWidth="1"/>
-    <col min="14" max="14" width="10.875" style="33" customWidth="1"/>
-    <col min="15" max="15" width="15.375" style="33" customWidth="1"/>
-    <col min="16" max="16384" width="10.875" style="33"/>
+    <col min="12" max="12" width="15.81640625" style="33" customWidth="1"/>
+    <col min="13" max="13" width="4.1796875" style="33" customWidth="1"/>
+    <col min="14" max="14" width="10.81640625" style="33" customWidth="1"/>
+    <col min="15" max="15" width="15.36328125" style="33" customWidth="1"/>
+    <col min="16" max="16384" width="10.81640625" style="33"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -3869,7 +3845,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="2" spans="1:16" s="37" customFormat="1" ht="76.5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:16" s="37" customFormat="1" ht="75.599999999999994" x14ac:dyDescent="0.2">
       <c r="A2" s="37" t="s">
         <v>115</v>
       </c>
@@ -3916,7 +3892,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="3" spans="1:16" s="37" customFormat="1" ht="89.25" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:16" s="37" customFormat="1" ht="88.2" x14ac:dyDescent="0.2">
       <c r="A3" s="37" t="s">
         <v>116</v>
       </c>
@@ -3963,7 +3939,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="4" spans="1:16" s="37" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:16" s="37" customFormat="1" ht="25.2" x14ac:dyDescent="0.2">
       <c r="A4" s="37" t="s">
         <v>117</v>
       </c>
@@ -4010,7 +3986,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:16" s="37" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:16" s="37" customFormat="1" ht="25.2" x14ac:dyDescent="0.2">
       <c r="A5" s="37" t="s">
         <v>120</v>
       </c>
@@ -4057,7 +4033,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:16" s="37" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:16" s="37" customFormat="1" ht="25.2" x14ac:dyDescent="0.2">
       <c r="A6" s="37" t="s">
         <v>121</v>
       </c>
@@ -4104,7 +4080,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:16" s="37" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:16" s="37" customFormat="1" ht="25.2" x14ac:dyDescent="0.2">
       <c r="A7" s="37" t="s">
         <v>122</v>
       </c>
@@ -4151,7 +4127,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="8" spans="1:16" s="37" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:16" s="37" customFormat="1" ht="25.2" x14ac:dyDescent="0.2">
       <c r="A8" s="37" t="s">
         <v>149</v>
       </c>
@@ -4198,7 +4174,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:16" s="37" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:16" s="37" customFormat="1" ht="25.2" x14ac:dyDescent="0.2">
       <c r="A9" s="37" t="s">
         <v>150</v>
       </c>
@@ -4257,12 +4233,12 @@
     <row r="15" spans="1:16" s="37" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B15" s="30"/>
     </row>
-    <row r="16" spans="1:16" s="37" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:16" s="37" customFormat="1" ht="25.2" x14ac:dyDescent="0.2">
       <c r="B16" s="31" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="17" spans="2:2" s="37" customFormat="1" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:2" s="37" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.2">
       <c r="B17" s="32" t="s">
         <v>262</v>
       </c>
@@ -4275,7 +4251,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="20" spans="2:2" s="37" customFormat="1" ht="63" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:2" s="37" customFormat="1" ht="51" x14ac:dyDescent="0.2">
       <c r="B20" s="32" t="s">
         <v>263</v>
       </c>
@@ -4288,7 +4264,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="23" spans="2:2" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:2" ht="20.399999999999999" x14ac:dyDescent="0.2">
       <c r="B23" s="32" t="s">
         <v>261</v>
       </c>
@@ -4301,21 +4277,21 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="150" workbookViewId="0">
-      <selection activeCell="P4" sqref="P4"/>
+    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="150" workbookViewId="0">
+      <selection activeCell="P9" sqref="P9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.875" style="33"/>
+    <col min="1" max="1" width="10.81640625" style="33"/>
     <col min="2" max="2" width="23" style="33" bestFit="1" customWidth="1"/>
-    <col min="3" max="10" width="10.875" style="33"/>
-    <col min="11" max="11" width="14.875" style="33" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.875" style="33" bestFit="1" customWidth="1"/>
-    <col min="13" max="16384" width="10.875" style="33"/>
+    <col min="3" max="10" width="10.81640625" style="33"/>
+    <col min="11" max="11" width="14.90625" style="33" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.81640625" style="33" bestFit="1" customWidth="1"/>
+    <col min="13" max="16384" width="10.81640625" style="33"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -4383,7 +4359,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:16" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A3" s="33" t="s">
         <v>124</v>
       </c>
@@ -4393,44 +4369,14 @@
       <c r="C3" s="33" t="s">
         <v>187</v>
       </c>
-      <c r="D3" s="33" t="s">
-        <v>228</v>
-      </c>
       <c r="E3" s="33">
         <v>40</v>
       </c>
       <c r="F3" s="33">
         <v>2</v>
       </c>
-      <c r="G3" s="33">
-        <v>60</v>
-      </c>
-      <c r="H3" s="33">
-        <v>4</v>
-      </c>
-      <c r="I3" s="40">
-        <v>42092</v>
-      </c>
-      <c r="J3" s="33" t="s">
-        <v>269</v>
-      </c>
-      <c r="K3" s="33" t="s">
-        <v>271</v>
-      </c>
-      <c r="L3" s="33">
-        <v>34</v>
-      </c>
-      <c r="N3" s="33" t="s">
-        <v>273</v>
-      </c>
-      <c r="O3" s="33" t="s">
-        <v>275</v>
-      </c>
-      <c r="P3" s="33">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="4" spans="1:16" ht="38.25" x14ac:dyDescent="0.2">
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A4" s="33" t="s">
         <v>125</v>
       </c>
@@ -4440,41 +4386,11 @@
       <c r="C4" s="33" t="s">
         <v>187</v>
       </c>
-      <c r="D4" s="33" t="s">
-        <v>228</v>
-      </c>
       <c r="E4" s="33">
         <v>40</v>
       </c>
       <c r="F4" s="33">
         <v>2</v>
-      </c>
-      <c r="G4" s="33">
-        <v>70</v>
-      </c>
-      <c r="H4" s="33">
-        <v>4</v>
-      </c>
-      <c r="I4" s="40">
-        <v>42092</v>
-      </c>
-      <c r="J4" s="33" t="s">
-        <v>270</v>
-      </c>
-      <c r="K4" s="33" t="s">
-        <v>272</v>
-      </c>
-      <c r="L4" s="33">
-        <v>25</v>
-      </c>
-      <c r="N4" s="33" t="s">
-        <v>274</v>
-      </c>
-      <c r="O4" s="33" t="s">
-        <v>276</v>
-      </c>
-      <c r="P4" s="33">
-        <v>42</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.2">
@@ -4494,7 +4410,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:16" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:16" ht="37.799999999999997" x14ac:dyDescent="0.2">
       <c r="A6" s="33" t="s">
         <v>136</v>
       </c>
@@ -4575,7 +4491,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:16" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:16" ht="25.2" x14ac:dyDescent="0.2">
       <c r="A9" s="33" t="s">
         <v>140</v>
       </c>
@@ -4629,16 +4545,16 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I1"/>
   <sheetViews>
     <sheetView zoomScale="150" workbookViewId="0">
       <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" ht="25.2" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>3</v>
       </c>
@@ -4674,17 +4590,17 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C43"/>
   <sheetViews>
     <sheetView topLeftCell="A8" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="28.125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="49.5" style="1" customWidth="1"/>
+    <col min="2" max="2" width="28.1796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="49.453125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.2">
@@ -4698,7 +4614,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>109</v>
       </c>
@@ -4709,7 +4625,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>110</v>
       </c>
@@ -4720,7 +4636,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>111</v>
       </c>
@@ -4731,7 +4647,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>112</v>
       </c>
@@ -4742,7 +4658,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>113</v>
       </c>
@@ -4753,7 +4669,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>114</v>
       </c>
@@ -4764,7 +4680,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="47.25" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3" ht="45" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>115</v>
       </c>
@@ -4775,7 +4691,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>116</v>
       </c>
@@ -4786,7 +4702,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>117</v>
       </c>
@@ -4797,7 +4713,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>118</v>
       </c>
@@ -4808,7 +4724,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>119</v>
       </c>
@@ -4819,7 +4735,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="47.25" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:3" ht="45" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>120</v>
       </c>
@@ -4830,7 +4746,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="63" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:3" ht="45" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>121</v>
       </c>
@@ -4841,7 +4757,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>122</v>
       </c>
@@ -4852,7 +4768,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>123</v>
       </c>
@@ -4863,7 +4779,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>124</v>
       </c>
@@ -4874,7 +4790,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>125</v>
       </c>
@@ -4885,7 +4801,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>126</v>
       </c>
@@ -4896,7 +4812,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>127</v>
       </c>
@@ -4907,7 +4823,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>128</v>
       </c>
@@ -4918,7 +4834,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>129</v>
       </c>
@@ -4929,7 +4845,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>130</v>
       </c>
@@ -4940,7 +4856,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>131</v>
       </c>
@@ -4951,7 +4867,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="47.25" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>132</v>
       </c>
@@ -4962,7 +4878,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>133</v>
       </c>
@@ -4973,7 +4889,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="126" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:3" ht="105" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>134</v>
       </c>
@@ -4984,7 +4900,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>135</v>
       </c>
@@ -4995,7 +4911,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>136</v>
       </c>
@@ -5006,7 +4922,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="30" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>137</v>
       </c>
@@ -5017,7 +4933,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="31" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>138</v>
       </c>
@@ -5028,7 +4944,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>139</v>
       </c>
@@ -5039,7 +4955,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="33" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>140</v>
       </c>
@@ -5050,7 +4966,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="34" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>141</v>
       </c>
@@ -5061,7 +4977,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="35" spans="1:3" ht="47.25" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>142</v>
       </c>
@@ -5072,7 +4988,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="36" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>143</v>
       </c>
@@ -5083,7 +4999,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="37" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>144</v>
       </c>
@@ -5094,7 +5010,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="38" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>145</v>
       </c>
@@ -5105,7 +5021,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="39" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>146</v>
       </c>
@@ -5116,7 +5032,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="40" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>147</v>
       </c>
@@ -5127,7 +5043,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="41" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>148</v>
       </c>
@@ -5138,7 +5054,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="42" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>149</v>
       </c>
@@ -5149,7 +5065,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="43" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>150</v>
       </c>

</xml_diff>

<commit_message>
Update team report and main script
Updated burndown chart and console output of main script
</commit_message>
<xml_diff>
--- a/TeamDReport copy.xlsx
+++ b/TeamDReport copy.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10211"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Funbucket24\Documents\GitHub\SSW555-DriverlessCar\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/JP/OneDrive/Jonathan's Folder!/Stevens/CS_555_Agile_Methods_for_SW_Development/Project_Documents/SSW555-DriverlessCar/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{542E80AE-453D-4D1B-BBB2-F51105A6934F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D96D92C9-520D-9444-B1FD-2363034EA705}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8295" tabRatio="500" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="14400" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Team" sheetId="1" r:id="rId1"/>
@@ -31,6 +31,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
       </xcalcf:calcFeatures>
     </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
@@ -872,71 +873,71 @@
 order_siblings_by_age</t>
   </si>
   <si>
+    <t>test_order_siblings_by_age</t>
+  </si>
+  <si>
+    <t>list_multiple_births</t>
+  </si>
+  <si>
+    <t>test_list_multiple_births</t>
+  </si>
+  <si>
+    <t>LivingMaritalStatus.py</t>
+  </si>
+  <si>
+    <t>list_living_married</t>
+  </si>
+  <si>
+    <t>TestLivingMaritalStatus.py</t>
+  </si>
+  <si>
+    <t>test_living_marital_status_no_div_no_death, test_living_marital_status_no_div_death, test_living_marital_status_div_no_death, test_living_marital_status_div_death</t>
+  </si>
+  <si>
+    <t>siblings_not_too_many.py</t>
+  </si>
+  <si>
+    <t>siblings_not_too_many</t>
+  </si>
+  <si>
+    <t>test_siblings_not_too_many.py</t>
+  </si>
+  <si>
+    <t>test_valid_siblings_num, test_siblings_more_than_15</t>
+  </si>
+  <si>
+    <t>siblings_not_marry.py</t>
+  </si>
+  <si>
+    <t>siblings_not_marry</t>
+  </si>
+  <si>
+    <t>test_siblings_not_marry.py</t>
+  </si>
+  <si>
+    <t>test_valid, test_invalid</t>
+  </si>
+  <si>
+    <t>male_last_names.py</t>
+  </si>
+  <si>
+    <t>no_marriage_to_children.py</t>
+  </si>
+  <si>
+    <t>TestSameFamilyChildrenMarriage.py</t>
+  </si>
+  <si>
+    <t>TestMaleNames.py</t>
+  </si>
+  <si>
+    <t>TestMaleNames</t>
+  </si>
+  <si>
+    <t>TestMarriageToChildren</t>
+  </si>
+  <si>
     <t>18
-47</t>
-  </si>
-  <si>
-    <t>test_order_siblings_by_age</t>
-  </si>
-  <si>
-    <t>list_multiple_births</t>
-  </si>
-  <si>
-    <t>test_list_multiple_births</t>
-  </si>
-  <si>
-    <t>LivingMaritalStatus.py</t>
-  </si>
-  <si>
-    <t>list_living_married</t>
-  </si>
-  <si>
-    <t>TestLivingMaritalStatus.py</t>
-  </si>
-  <si>
-    <t>test_living_marital_status_no_div_no_death, test_living_marital_status_no_div_death, test_living_marital_status_div_no_death, test_living_marital_status_div_death</t>
-  </si>
-  <si>
-    <t>siblings_not_too_many.py</t>
-  </si>
-  <si>
-    <t>siblings_not_too_many</t>
-  </si>
-  <si>
-    <t>test_siblings_not_too_many.py</t>
-  </si>
-  <si>
-    <t>test_valid_siblings_num, test_siblings_more_than_15</t>
-  </si>
-  <si>
-    <t>siblings_not_marry.py</t>
-  </si>
-  <si>
-    <t>siblings_not_marry</t>
-  </si>
-  <si>
-    <t>test_siblings_not_marry.py</t>
-  </si>
-  <si>
-    <t>test_valid, test_invalid</t>
-  </si>
-  <si>
-    <t>male_last_names.py</t>
-  </si>
-  <si>
-    <t>no_marriage_to_children.py</t>
-  </si>
-  <si>
-    <t>TestSameFamilyChildrenMarriage.py</t>
-  </si>
-  <si>
-    <t>TestMaleNames.py</t>
-  </si>
-  <si>
-    <t>TestMaleNames</t>
-  </si>
-  <si>
-    <t>TestMarriageToChildren</t>
+43</t>
   </si>
 </sst>
 </file>
@@ -1297,7 +1298,7 @@
             <c:numRef>
               <c:f>'Burndown README'!$B$15:$B$20</c:f>
               <c:numCache>
-                <c:formatCode>m/d/yyyy</c:formatCode>
+                <c:formatCode>m/d/yy</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
                   <c:v>41065</c:v>
@@ -1368,7 +1369,7 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:numFmt formatCode="m/d/yyyy" sourceLinked="1"/>
+        <c:numFmt formatCode="m/d/yy" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1468,6 +1469,9 @@
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2357,19 +2361,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView zoomScale="150" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="7.875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="8.5" customWidth="1"/>
     <col min="4" max="5" width="20.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A1" s="4" t="s">
         <v>19</v>
       </c>
@@ -2386,7 +2390,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="2" spans="1:5" s="13" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" s="13" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A2" s="13" t="s">
         <v>183</v>
       </c>
@@ -2403,7 +2407,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
         <v>182</v>
       </c>
@@ -2420,7 +2424,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A4" s="13" t="s">
         <v>187</v>
       </c>
@@ -2437,7 +2441,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A5" s="13" t="s">
         <v>195</v>
       </c>
@@ -2454,7 +2458,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.15">
       <c r="D10" s="4" t="s">
         <v>31</v>
       </c>
@@ -2463,7 +2467,7 @@
       </c>
     </row>
   </sheetData>
-  <sortState ref="A4:D6">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A4:D6">
     <sortCondition ref="C4:C6"/>
   </sortState>
   <phoneticPr fontId="2" type="noConversion"/>
@@ -2483,21 +2487,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E33"/>
   <sheetViews>
-    <sheetView topLeftCell="A24" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E31" sqref="E31"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="6.875" style="16" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="29.125" style="16" customWidth="1"/>
+    <col min="1" max="1" width="6.83203125" style="16" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="29.1640625" style="16" customWidth="1"/>
     <col min="3" max="3" width="34.5" style="16" customWidth="1"/>
-    <col min="4" max="4" width="6.625" style="16" customWidth="1"/>
-    <col min="5" max="5" width="10.375" style="16" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="10.875" style="16"/>
+    <col min="4" max="4" width="6.6640625" style="16" customWidth="1"/>
+    <col min="5" max="5" width="10.33203125" style="16" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="10.83203125" style="16"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="15" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" s="15" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A1" s="15" t="s">
         <v>29</v>
       </c>
@@ -2514,7 +2518,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" ht="34" x14ac:dyDescent="0.15">
       <c r="A2" s="16" t="s">
         <v>109</v>
       </c>
@@ -2531,7 +2535,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" ht="34" x14ac:dyDescent="0.15">
       <c r="A3" s="16" t="s">
         <v>110</v>
       </c>
@@ -2548,7 +2552,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" ht="34" x14ac:dyDescent="0.15">
       <c r="A4" s="16" t="s">
         <v>111</v>
       </c>
@@ -2565,7 +2569,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="47.25" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" ht="51" x14ac:dyDescent="0.15">
       <c r="A5" s="16" t="s">
         <v>112</v>
       </c>
@@ -2582,7 +2586,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" ht="34" x14ac:dyDescent="0.15">
       <c r="A6" s="16" t="s">
         <v>113</v>
       </c>
@@ -2599,7 +2603,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" ht="34" x14ac:dyDescent="0.15">
       <c r="A7" s="16" t="s">
         <v>114</v>
       </c>
@@ -2616,7 +2620,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="63" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" ht="68" x14ac:dyDescent="0.15">
       <c r="A8" s="16" t="s">
         <v>115</v>
       </c>
@@ -2633,7 +2637,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="47.25" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" ht="51" x14ac:dyDescent="0.15">
       <c r="A9" s="16" t="s">
         <v>116</v>
       </c>
@@ -2650,7 +2654,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="47.25" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5" ht="51" x14ac:dyDescent="0.15">
       <c r="A10" s="16" t="s">
         <v>117</v>
       </c>
@@ -2667,7 +2671,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="47.25" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5" ht="51" x14ac:dyDescent="0.15">
       <c r="A11" s="16" t="s">
         <v>118</v>
       </c>
@@ -2684,7 +2688,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5" ht="34" x14ac:dyDescent="0.15">
       <c r="A12" s="16" t="s">
         <v>119</v>
       </c>
@@ -2701,7 +2705,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="63" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:5" ht="68" x14ac:dyDescent="0.15">
       <c r="A13" s="16" t="s">
         <v>120</v>
       </c>
@@ -2718,7 +2722,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="78.75" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:5" ht="85" x14ac:dyDescent="0.15">
       <c r="A14" s="16" t="s">
         <v>121</v>
       </c>
@@ -2735,7 +2739,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:5" ht="34" x14ac:dyDescent="0.15">
       <c r="A15" s="16" t="s">
         <v>122</v>
       </c>
@@ -2752,7 +2756,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:5" ht="34" x14ac:dyDescent="0.15">
       <c r="A16" s="16" t="s">
         <v>123</v>
       </c>
@@ -2766,10 +2770,10 @@
         <v>183</v>
       </c>
       <c r="E16" s="16" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" ht="31.5" x14ac:dyDescent="0.2">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="34" x14ac:dyDescent="0.15">
       <c r="A17" s="16" t="s">
         <v>124</v>
       </c>
@@ -2783,10 +2787,10 @@
         <v>187</v>
       </c>
       <c r="E17" s="16" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" ht="31.5" x14ac:dyDescent="0.2">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="34" x14ac:dyDescent="0.15">
       <c r="A18" s="16" t="s">
         <v>125</v>
       </c>
@@ -2800,10 +2804,10 @@
         <v>187</v>
       </c>
       <c r="E18" s="16" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" ht="31.5" x14ac:dyDescent="0.2">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="34" x14ac:dyDescent="0.15">
       <c r="A19" s="16" t="s">
         <v>126</v>
       </c>
@@ -2817,10 +2821,10 @@
         <v>183</v>
       </c>
       <c r="E19" s="16" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" ht="31.5" x14ac:dyDescent="0.2">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="34" x14ac:dyDescent="0.15">
       <c r="A20" s="16" t="s">
         <v>127</v>
       </c>
@@ -2831,7 +2835,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:5" ht="34" x14ac:dyDescent="0.15">
       <c r="A21" s="16" t="s">
         <v>128</v>
       </c>
@@ -2842,7 +2846,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="22" spans="1:5" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:5" ht="34" x14ac:dyDescent="0.15">
       <c r="A22" s="16" t="s">
         <v>130</v>
       </c>
@@ -2853,7 +2857,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="23" spans="1:5" ht="47.25" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:5" ht="51" x14ac:dyDescent="0.15">
       <c r="A23" s="16" t="s">
         <v>131</v>
       </c>
@@ -2864,7 +2868,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="24" spans="1:5" ht="63" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:5" ht="68" x14ac:dyDescent="0.15">
       <c r="A24" s="16" t="s">
         <v>132</v>
       </c>
@@ -2875,7 +2879,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="25" spans="1:5" ht="47.25" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:5" ht="51" x14ac:dyDescent="0.15">
       <c r="A25" s="16" t="s">
         <v>133</v>
       </c>
@@ -2886,7 +2890,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="26" spans="1:5" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:5" ht="34" x14ac:dyDescent="0.15">
       <c r="A26" s="16" t="s">
         <v>135</v>
       </c>
@@ -2897,7 +2901,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="27" spans="1:5" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:5" ht="34" x14ac:dyDescent="0.15">
       <c r="A27" s="16" t="s">
         <v>136</v>
       </c>
@@ -2914,7 +2918,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="28" spans="1:5" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:5" ht="34" x14ac:dyDescent="0.15">
       <c r="A28" s="16" t="s">
         <v>137</v>
       </c>
@@ -2925,7 +2929,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="29" spans="1:5" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:5" ht="34" x14ac:dyDescent="0.15">
       <c r="A29" s="16" t="s">
         <v>138</v>
       </c>
@@ -2939,10 +2943,10 @@
         <v>182</v>
       </c>
       <c r="E29" s="16" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" ht="47.25" x14ac:dyDescent="0.2">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" ht="51" x14ac:dyDescent="0.15">
       <c r="A30" s="16" t="s">
         <v>139</v>
       </c>
@@ -2956,10 +2960,10 @@
         <v>182</v>
       </c>
       <c r="E30" s="16" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" ht="31.5" x14ac:dyDescent="0.2">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" ht="34" x14ac:dyDescent="0.15">
       <c r="A31" s="16" t="s">
         <v>140</v>
       </c>
@@ -2976,7 +2980,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="32" spans="1:5" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:5" ht="34" x14ac:dyDescent="0.15">
       <c r="A32" s="16" t="s">
         <v>149</v>
       </c>
@@ -2993,7 +2997,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="33" spans="1:5" ht="47.25" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:5" ht="51" x14ac:dyDescent="0.15">
       <c r="A33" s="16" t="s">
         <v>150</v>
       </c>
@@ -3021,51 +3025,51 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:G19"/>
   <sheetViews>
-    <sheetView topLeftCell="A30" zoomScale="150" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+    <sheetView topLeftCell="A7" zoomScale="150" workbookViewId="0">
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="10.875" style="2"/>
+    <col min="1" max="1" width="10.83203125" style="2"/>
     <col min="2" max="2" width="9.5" customWidth="1"/>
-    <col min="3" max="3" width="15.875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.375" customWidth="1"/>
-    <col min="5" max="5" width="6.875" customWidth="1"/>
+    <col min="3" max="3" width="15.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.33203125" customWidth="1"/>
+    <col min="5" max="5" width="6.83203125" customWidth="1"/>
     <col min="6" max="6" width="12.5" style="7" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A1" s="2" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A2" s="2" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A3" s="2" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A5" s="2" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A6" s="2" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A8" s="2" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="14" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A14" s="4" t="s">
         <v>156</v>
       </c>
@@ -3088,7 +3092,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A15" t="s">
         <v>157</v>
       </c>
@@ -3104,7 +3108,7 @@
       <c r="F15" s="11"/>
       <c r="G15" s="7"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A16" t="s">
         <v>158</v>
       </c>
@@ -3129,7 +3133,7 @@
         <v>125.00000000000001</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A17" s="2" t="s">
         <v>159</v>
       </c>
@@ -3154,7 +3158,7 @@
         <v>102.22222222222223</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A18" s="2" t="s">
         <v>160</v>
       </c>
@@ -3179,7 +3183,7 @@
         <v>97.5</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A19" s="2" t="s">
         <v>161</v>
       </c>
@@ -3216,20 +3220,20 @@
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView zoomScale="150" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="10.875" style="2"/>
-    <col min="2" max="2" width="16.625" customWidth="1"/>
+    <col min="1" max="1" width="10.83203125" style="2"/>
+    <col min="2" max="2" width="16.6640625" customWidth="1"/>
     <col min="3" max="3" width="14.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.125" customWidth="1"/>
-    <col min="5" max="5" width="6.875" customWidth="1"/>
+    <col min="4" max="4" width="7.1640625" customWidth="1"/>
+    <col min="5" max="5" width="6.83203125" customWidth="1"/>
     <col min="6" max="6" width="12.5" style="7" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -3249,7 +3253,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A2" s="2">
         <v>42044</v>
       </c>
@@ -3260,7 +3264,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A3" s="2">
         <v>42058</v>
       </c>
@@ -3282,7 +3286,7 @@
         <v>44.186046511627907</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A4" s="2">
         <v>42079</v>
       </c>
@@ -3303,12 +3307,28 @@
         <v>11.733333333333333</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A5" s="2">
         <v>42093</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B5">
+        <v>8</v>
+      </c>
+      <c r="C5">
+        <v>8</v>
+      </c>
+      <c r="D5">
+        <v>309</v>
+      </c>
+      <c r="E5">
+        <v>17</v>
+      </c>
+      <c r="F5" s="7">
+        <f>(D5-D4)/(E5)</f>
+        <v>-3.3529411764705883</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A6" s="2">
         <v>42107</v>
       </c>
@@ -3329,28 +3349,28 @@
       <selection activeCell="B13" sqref="B13:B22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="9" style="16" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="24.5" style="18" customWidth="1"/>
-    <col min="3" max="3" width="7.375" style="16" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.625" style="16" customWidth="1"/>
+    <col min="3" max="3" width="7.33203125" style="16" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.6640625" style="16" customWidth="1"/>
     <col min="5" max="5" width="8.5" style="16" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.375" style="16" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.625" style="16" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.375" style="16" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.33203125" style="16" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.6640625" style="16" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.33203125" style="16" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="11" style="26" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="20.875" style="29" customWidth="1"/>
-    <col min="11" max="11" width="17.875" style="29" customWidth="1"/>
+    <col min="10" max="10" width="20.83203125" style="29" customWidth="1"/>
+    <col min="11" max="11" width="17.83203125" style="29" customWidth="1"/>
     <col min="12" max="12" width="13" style="24" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="1.875" style="24" customWidth="1"/>
-    <col min="14" max="14" width="16.875" style="29" customWidth="1"/>
-    <col min="15" max="15" width="22.875" style="29" customWidth="1"/>
-    <col min="16" max="16" width="10.125" style="24" bestFit="1" customWidth="1"/>
-    <col min="17" max="16384" width="10.875" style="16"/>
+    <col min="13" max="13" width="1.83203125" style="24" customWidth="1"/>
+    <col min="14" max="14" width="16.83203125" style="29" customWidth="1"/>
+    <col min="15" max="15" width="22.83203125" style="29" customWidth="1"/>
+    <col min="16" max="16" width="10.1640625" style="24" bestFit="1" customWidth="1"/>
+    <col min="17" max="16384" width="10.83203125" style="16"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:16" ht="14" x14ac:dyDescent="0.15">
       <c r="A1" s="15" t="s">
         <v>9</v>
       </c>
@@ -3397,7 +3417,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="2" spans="1:16" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:16" ht="28" x14ac:dyDescent="0.15">
       <c r="A2" s="16" t="s">
         <v>109</v>
       </c>
@@ -3444,7 +3464,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:16" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:16" ht="28" x14ac:dyDescent="0.15">
       <c r="A3" s="16" t="s">
         <v>110</v>
       </c>
@@ -3491,7 +3511,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:16" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:16" ht="28" x14ac:dyDescent="0.15">
       <c r="A4" s="16" t="s">
         <v>111</v>
       </c>
@@ -3538,7 +3558,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="5" spans="1:16" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:16" ht="28" x14ac:dyDescent="0.15">
       <c r="A5" s="16" t="s">
         <v>112</v>
       </c>
@@ -3585,7 +3605,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="6" spans="1:16" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:16" ht="28" x14ac:dyDescent="0.15">
       <c r="A6" s="16" t="s">
         <v>113</v>
       </c>
@@ -3632,7 +3652,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:16" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:16" ht="28" x14ac:dyDescent="0.15">
       <c r="A7" s="16" t="s">
         <v>114</v>
       </c>
@@ -3679,7 +3699,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:16" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:16" ht="42" x14ac:dyDescent="0.15">
       <c r="A8" s="16" t="s">
         <v>118</v>
       </c>
@@ -3726,7 +3746,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="9" spans="1:16" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:16" ht="28" x14ac:dyDescent="0.15">
       <c r="A9" s="16" t="s">
         <v>119</v>
       </c>
@@ -3773,7 +3793,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.15">
       <c r="J10" s="28"/>
       <c r="K10" s="28"/>
       <c r="L10" s="27"/>
@@ -3781,43 +3801,43 @@
       <c r="O10" s="28"/>
       <c r="P10" s="27"/>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:16" ht="14" x14ac:dyDescent="0.15">
       <c r="B13" s="20" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.15">
       <c r="B14" s="30"/>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:16" ht="14" x14ac:dyDescent="0.15">
       <c r="B15" s="31" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="16" spans="1:16" ht="21" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:16" ht="24" x14ac:dyDescent="0.15">
       <c r="B16" s="32" t="s">
         <v>230</v>
       </c>
     </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:2" x14ac:dyDescent="0.15">
       <c r="B17" s="20"/>
     </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:2" ht="14" x14ac:dyDescent="0.15">
       <c r="B18" s="31" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="19" spans="2:2" ht="73.5" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:2" ht="72" x14ac:dyDescent="0.15">
       <c r="B19" s="32" t="s">
         <v>229</v>
       </c>
     </row>
-    <row r="21" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:2" ht="14" x14ac:dyDescent="0.15">
       <c r="B21" s="31" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="22" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:2" x14ac:dyDescent="0.15">
       <c r="B22" s="32" t="s">
         <v>231</v>
       </c>
@@ -3834,24 +3854,24 @@
   <dimension ref="A1:P23"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="10.875" style="33"/>
+    <col min="1" max="1" width="10.83203125" style="33"/>
     <col min="2" max="2" width="22" style="33" bestFit="1" customWidth="1"/>
-    <col min="3" max="9" width="10.875" style="33"/>
-    <col min="10" max="10" width="13.875" style="33" customWidth="1"/>
+    <col min="3" max="9" width="10.83203125" style="33"/>
+    <col min="10" max="10" width="13.83203125" style="33" customWidth="1"/>
     <col min="11" max="11" width="16" style="33" customWidth="1"/>
-    <col min="12" max="12" width="15.875" style="33" customWidth="1"/>
-    <col min="13" max="13" width="4.125" style="33" customWidth="1"/>
-    <col min="14" max="14" width="10.875" style="33" customWidth="1"/>
-    <col min="15" max="15" width="15.375" style="33" customWidth="1"/>
-    <col min="16" max="16384" width="10.875" style="33"/>
+    <col min="12" max="12" width="15.83203125" style="33" customWidth="1"/>
+    <col min="13" max="13" width="4.1640625" style="33" customWidth="1"/>
+    <col min="14" max="14" width="10.83203125" style="33" customWidth="1"/>
+    <col min="15" max="15" width="15.33203125" style="33" customWidth="1"/>
+    <col min="16" max="16384" width="10.83203125" style="33"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="34" t="s">
         <v>9</v>
       </c>
@@ -3899,11 +3919,11 @@
         <v>178</v>
       </c>
     </row>
-    <row r="2" spans="1:16" s="37" customFormat="1" ht="76.5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:16" s="37" customFormat="1" ht="84" x14ac:dyDescent="0.15">
       <c r="A2" s="37" t="s">
         <v>115</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="16" t="s">
         <v>69</v>
       </c>
       <c r="C2" s="37" t="s">
@@ -3946,11 +3966,11 @@
         <v>41</v>
       </c>
     </row>
-    <row r="3" spans="1:16" s="37" customFormat="1" ht="89.25" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:16" s="37" customFormat="1" ht="98" x14ac:dyDescent="0.15">
       <c r="A3" s="37" t="s">
         <v>116</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="16" t="s">
         <v>152</v>
       </c>
       <c r="C3" s="37" t="s">
@@ -3993,7 +4013,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="4" spans="1:16" s="37" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:16" s="37" customFormat="1" ht="42" x14ac:dyDescent="0.15">
       <c r="A4" s="37" t="s">
         <v>117</v>
       </c>
@@ -4040,7 +4060,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:16" s="37" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:16" s="37" customFormat="1" ht="28" x14ac:dyDescent="0.15">
       <c r="A5" s="37" t="s">
         <v>120</v>
       </c>
@@ -4087,7 +4107,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:16" s="37" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:16" s="37" customFormat="1" ht="28" x14ac:dyDescent="0.15">
       <c r="A6" s="37" t="s">
         <v>121</v>
       </c>
@@ -4134,7 +4154,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:16" s="37" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:16" s="37" customFormat="1" ht="42" x14ac:dyDescent="0.15">
       <c r="A7" s="37" t="s">
         <v>122</v>
       </c>
@@ -4181,7 +4201,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="8" spans="1:16" s="37" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:16" s="37" customFormat="1" ht="28" x14ac:dyDescent="0.15">
       <c r="A8" s="37" t="s">
         <v>149</v>
       </c>
@@ -4228,7 +4248,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:16" s="37" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:16" s="37" customFormat="1" ht="28" x14ac:dyDescent="0.15">
       <c r="A9" s="37" t="s">
         <v>150</v>
       </c>
@@ -4275,50 +4295,50 @@
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:16" s="37" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="11" spans="1:16" s="37" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="12" spans="1:16" s="37" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="13" spans="1:16" s="37" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="14" spans="1:16" s="37" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:16" s="37" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="11" spans="1:16" s="37" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="12" spans="1:16" s="37" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="13" spans="1:16" s="37" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="14" spans="1:16" s="37" customFormat="1" ht="14" x14ac:dyDescent="0.15">
       <c r="B14" s="20" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="15" spans="1:16" s="37" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:16" s="37" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B15" s="30"/>
     </row>
-    <row r="16" spans="1:16" s="37" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:16" s="37" customFormat="1" ht="28" x14ac:dyDescent="0.15">
       <c r="B16" s="31" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="17" spans="2:2" s="37" customFormat="1" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:2" s="37" customFormat="1" ht="24" x14ac:dyDescent="0.15">
       <c r="B17" s="32" t="s">
         <v>262</v>
       </c>
     </row>
-    <row r="18" spans="2:2" s="37" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:2" s="37" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B18" s="20"/>
     </row>
-    <row r="19" spans="2:2" s="37" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:2" s="37" customFormat="1" ht="28" x14ac:dyDescent="0.15">
       <c r="B19" s="31" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="20" spans="2:2" s="37" customFormat="1" ht="63" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:2" s="37" customFormat="1" ht="72" x14ac:dyDescent="0.15">
       <c r="B20" s="32" t="s">
         <v>263</v>
       </c>
     </row>
-    <row r="21" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:2" x14ac:dyDescent="0.15">
       <c r="B21" s="18"/>
     </row>
-    <row r="22" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:2" ht="14" x14ac:dyDescent="0.15">
       <c r="B22" s="31" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="23" spans="2:2" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:2" ht="36" x14ac:dyDescent="0.15">
       <c r="B23" s="32" t="s">
         <v>261</v>
       </c>
@@ -4334,21 +4354,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:P9"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" workbookViewId="0">
-      <selection activeCell="O4" sqref="O4"/>
+    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2:G9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="10.875" style="33"/>
+    <col min="1" max="1" width="10.83203125" style="33"/>
     <col min="2" max="2" width="23" style="33" bestFit="1" customWidth="1"/>
-    <col min="3" max="10" width="10.875" style="33"/>
-    <col min="11" max="11" width="14.875" style="33" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.875" style="33" bestFit="1" customWidth="1"/>
-    <col min="13" max="16384" width="10.875" style="33"/>
+    <col min="3" max="10" width="10.83203125" style="33"/>
+    <col min="11" max="11" width="14.83203125" style="33" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.83203125" style="33" bestFit="1" customWidth="1"/>
+    <col min="13" max="16384" width="10.83203125" style="33"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="34" t="s">
         <v>3</v>
       </c>
@@ -4396,7 +4416,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="2" spans="1:16" ht="63.75" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:16" ht="84" x14ac:dyDescent="0.15">
       <c r="A2" s="33" t="s">
         <v>123</v>
       </c>
@@ -4422,25 +4442,25 @@
         <v>42092</v>
       </c>
       <c r="J2" s="33" t="s">
+        <v>272</v>
+      </c>
+      <c r="K2" s="33" t="s">
         <v>273</v>
-      </c>
-      <c r="K2" s="33" t="s">
-        <v>274</v>
       </c>
       <c r="L2" s="33">
         <v>15</v>
       </c>
       <c r="N2" s="33" t="s">
+        <v>274</v>
+      </c>
+      <c r="O2" s="33" t="s">
         <v>275</v>
-      </c>
-      <c r="O2" s="33" t="s">
-        <v>276</v>
       </c>
       <c r="P2" s="33">
         <v>42</v>
       </c>
     </row>
-    <row r="3" spans="1:16" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:16" ht="28" x14ac:dyDescent="0.15">
       <c r="A3" s="33" t="s">
         <v>124</v>
       </c>
@@ -4466,25 +4486,25 @@
         <v>42092</v>
       </c>
       <c r="J3" s="33" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="K3" s="33" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="L3" s="33">
         <v>33</v>
       </c>
       <c r="N3" s="33" t="s">
+        <v>283</v>
+      </c>
+      <c r="O3" s="33" t="s">
         <v>284</v>
-      </c>
-      <c r="O3" s="33" t="s">
-        <v>285</v>
       </c>
       <c r="P3" s="33">
         <v>38</v>
       </c>
     </row>
-    <row r="4" spans="1:16" ht="51" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:16" ht="56" x14ac:dyDescent="0.15">
       <c r="A4" s="33" t="s">
         <v>125</v>
       </c>
@@ -4510,25 +4530,25 @@
         <v>42093</v>
       </c>
       <c r="J4" s="33" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="K4" s="33" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="L4" s="33">
         <v>24</v>
       </c>
       <c r="N4" s="33" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="O4" s="33" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="P4" s="33">
         <v>43</v>
       </c>
     </row>
-    <row r="5" spans="1:16" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:16" ht="42" x14ac:dyDescent="0.15">
       <c r="A5" s="33" t="s">
         <v>126</v>
       </c>
@@ -4554,25 +4574,25 @@
         <v>42092</v>
       </c>
       <c r="J5" s="33" t="s">
+        <v>276</v>
+      </c>
+      <c r="K5" s="33" t="s">
         <v>277</v>
-      </c>
-      <c r="K5" s="33" t="s">
-        <v>278</v>
       </c>
       <c r="L5" s="33">
         <v>18</v>
       </c>
       <c r="N5" s="33" t="s">
+        <v>278</v>
+      </c>
+      <c r="O5" s="33" t="s">
         <v>279</v>
-      </c>
-      <c r="O5" s="33" t="s">
-        <v>280</v>
       </c>
       <c r="P5" s="33">
         <v>264</v>
       </c>
     </row>
-    <row r="6" spans="1:16" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:16" ht="42" x14ac:dyDescent="0.15">
       <c r="A6" s="33" t="s">
         <v>136</v>
       </c>
@@ -4607,19 +4627,19 @@
         <v>264</v>
       </c>
       <c r="L6" s="33" t="s">
-        <v>265</v>
+        <v>286</v>
       </c>
       <c r="N6" s="33" t="s">
         <v>237</v>
       </c>
       <c r="O6" s="33" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="P6" s="33">
         <v>46</v>
       </c>
     </row>
-    <row r="7" spans="1:16" ht="204" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:16" ht="224" x14ac:dyDescent="0.15">
       <c r="A7" s="33" t="s">
         <v>138</v>
       </c>
@@ -4645,25 +4665,25 @@
         <v>42092</v>
       </c>
       <c r="J7" s="37" t="s">
+        <v>268</v>
+      </c>
+      <c r="K7" s="37" t="s">
         <v>269</v>
-      </c>
-      <c r="K7" s="37" t="s">
-        <v>270</v>
       </c>
       <c r="L7" s="33">
         <v>48</v>
       </c>
       <c r="N7" s="37" t="s">
+        <v>270</v>
+      </c>
+      <c r="O7" s="37" t="s">
         <v>271</v>
-      </c>
-      <c r="O7" s="37" t="s">
-        <v>272</v>
       </c>
       <c r="P7" s="33">
         <v>79</v>
       </c>
     </row>
-    <row r="8" spans="1:16" ht="204" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:16" ht="224" x14ac:dyDescent="0.15">
       <c r="A8" s="33" t="s">
         <v>139</v>
       </c>
@@ -4689,25 +4709,25 @@
         <v>42092</v>
       </c>
       <c r="J8" s="37" t="s">
+        <v>268</v>
+      </c>
+      <c r="K8" s="37" t="s">
         <v>269</v>
-      </c>
-      <c r="K8" s="37" t="s">
-        <v>270</v>
       </c>
       <c r="L8" s="33">
         <v>48</v>
       </c>
       <c r="N8" s="37" t="s">
+        <v>270</v>
+      </c>
+      <c r="O8" s="37" t="s">
         <v>271</v>
-      </c>
-      <c r="O8" s="37" t="s">
-        <v>272</v>
       </c>
       <c r="P8" s="33">
         <v>79</v>
       </c>
     </row>
-    <row r="9" spans="1:16" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:16" ht="42" x14ac:dyDescent="0.15">
       <c r="A9" s="33" t="s">
         <v>140</v>
       </c>
@@ -4739,7 +4759,7 @@
         <v>235</v>
       </c>
       <c r="K9" s="33" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="L9" s="33">
         <v>53</v>
@@ -4748,7 +4768,7 @@
         <v>237</v>
       </c>
       <c r="O9" s="33" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="P9" s="33">
         <v>41</v>
@@ -4768,9 +4788,9 @@
       <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <sheetData>
-    <row r="1" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" ht="28" x14ac:dyDescent="0.15">
       <c r="A1" s="4" t="s">
         <v>3</v>
       </c>
@@ -4813,13 +4833,13 @@
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="2" max="2" width="28.125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.1640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="49.5" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" s="4" customFormat="1" ht="14" x14ac:dyDescent="0.15">
       <c r="A1" s="4" t="s">
         <v>108</v>
       </c>
@@ -4830,7 +4850,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" ht="34" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
         <v>109</v>
       </c>
@@ -4841,7 +4861,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" ht="17" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
         <v>110</v>
       </c>
@@ -4852,7 +4872,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" ht="17" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
         <v>111</v>
       </c>
@@ -4863,7 +4883,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" ht="34" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
         <v>112</v>
       </c>
@@ -4874,7 +4894,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" ht="17" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
         <v>113</v>
       </c>
@@ -4885,7 +4905,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" ht="17" x14ac:dyDescent="0.15">
       <c r="A7" t="s">
         <v>114</v>
       </c>
@@ -4896,7 +4916,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="47.25" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3" ht="51" x14ac:dyDescent="0.15">
       <c r="A8" t="s">
         <v>115</v>
       </c>
@@ -4907,7 +4927,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3" ht="34" x14ac:dyDescent="0.15">
       <c r="A9" t="s">
         <v>116</v>
       </c>
@@ -4918,7 +4938,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3" ht="34" x14ac:dyDescent="0.15">
       <c r="A10" t="s">
         <v>117</v>
       </c>
@@ -4929,7 +4949,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:3" ht="34" x14ac:dyDescent="0.15">
       <c r="A11" t="s">
         <v>118</v>
       </c>
@@ -4940,7 +4960,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:3" ht="34" x14ac:dyDescent="0.15">
       <c r="A12" t="s">
         <v>119</v>
       </c>
@@ -4951,7 +4971,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="47.25" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:3" ht="51" x14ac:dyDescent="0.15">
       <c r="A13" t="s">
         <v>120</v>
       </c>
@@ -4962,7 +4982,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="63" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:3" ht="68" x14ac:dyDescent="0.15">
       <c r="A14" t="s">
         <v>121</v>
       </c>
@@ -4973,7 +4993,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:3" ht="34" x14ac:dyDescent="0.15">
       <c r="A15" t="s">
         <v>122</v>
       </c>
@@ -4984,7 +5004,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:3" ht="17" x14ac:dyDescent="0.15">
       <c r="A16" t="s">
         <v>123</v>
       </c>
@@ -4995,7 +5015,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:3" ht="34" x14ac:dyDescent="0.15">
       <c r="A17" t="s">
         <v>124</v>
       </c>
@@ -5006,7 +5026,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:3" ht="17" x14ac:dyDescent="0.15">
       <c r="A18" t="s">
         <v>125</v>
       </c>
@@ -5017,7 +5037,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:3" ht="17" x14ac:dyDescent="0.15">
       <c r="A19" t="s">
         <v>126</v>
       </c>
@@ -5028,7 +5048,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:3" ht="17" x14ac:dyDescent="0.15">
       <c r="A20" t="s">
         <v>127</v>
       </c>
@@ -5039,7 +5059,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:3" ht="34" x14ac:dyDescent="0.15">
       <c r="A21" t="s">
         <v>128</v>
       </c>
@@ -5050,7 +5070,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:3" ht="34" x14ac:dyDescent="0.15">
       <c r="A22" t="s">
         <v>129</v>
       </c>
@@ -5061,7 +5081,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:3" ht="34" x14ac:dyDescent="0.15">
       <c r="A23" t="s">
         <v>130</v>
       </c>
@@ -5072,7 +5092,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:3" ht="34" x14ac:dyDescent="0.15">
       <c r="A24" t="s">
         <v>131</v>
       </c>
@@ -5083,7 +5103,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="47.25" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:3" ht="51" x14ac:dyDescent="0.15">
       <c r="A25" t="s">
         <v>132</v>
       </c>
@@ -5094,7 +5114,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:3" ht="34" x14ac:dyDescent="0.15">
       <c r="A26" t="s">
         <v>133</v>
       </c>
@@ -5105,7 +5125,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="126" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:3" ht="136" x14ac:dyDescent="0.15">
       <c r="A27" t="s">
         <v>134</v>
       </c>
@@ -5116,7 +5136,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:3" ht="17" x14ac:dyDescent="0.15">
       <c r="A28" t="s">
         <v>135</v>
       </c>
@@ -5127,7 +5147,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:3" ht="34" x14ac:dyDescent="0.15">
       <c r="A29" t="s">
         <v>136</v>
       </c>
@@ -5138,7 +5158,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="30" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:3" ht="17" x14ac:dyDescent="0.15">
       <c r="A30" t="s">
         <v>137</v>
       </c>
@@ -5149,7 +5169,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="31" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:3" ht="17" x14ac:dyDescent="0.15">
       <c r="A31" t="s">
         <v>138</v>
       </c>
@@ -5160,7 +5180,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:3" ht="34" x14ac:dyDescent="0.15">
       <c r="A32" t="s">
         <v>139</v>
       </c>
@@ -5171,7 +5191,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="33" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:3" ht="17" x14ac:dyDescent="0.15">
       <c r="A33" t="s">
         <v>140</v>
       </c>
@@ -5182,7 +5202,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="34" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:3" ht="34" x14ac:dyDescent="0.15">
       <c r="A34" t="s">
         <v>141</v>
       </c>
@@ -5193,7 +5213,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="35" spans="1:3" ht="47.25" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:3" ht="51" x14ac:dyDescent="0.15">
       <c r="A35" t="s">
         <v>142</v>
       </c>
@@ -5204,7 +5224,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="36" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:3" ht="34" x14ac:dyDescent="0.15">
       <c r="A36" t="s">
         <v>143</v>
       </c>
@@ -5215,7 +5235,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="37" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:3" ht="34" x14ac:dyDescent="0.15">
       <c r="A37" t="s">
         <v>144</v>
       </c>
@@ -5226,7 +5246,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="38" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:3" ht="34" x14ac:dyDescent="0.15">
       <c r="A38" t="s">
         <v>145</v>
       </c>
@@ -5237,7 +5257,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="39" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:3" ht="34" x14ac:dyDescent="0.15">
       <c r="A39" t="s">
         <v>146</v>
       </c>
@@ -5248,7 +5268,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="40" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:3" ht="34" x14ac:dyDescent="0.15">
       <c r="A40" t="s">
         <v>147</v>
       </c>
@@ -5259,7 +5279,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="41" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:3" ht="34" x14ac:dyDescent="0.15">
       <c r="A41" t="s">
         <v>148</v>
       </c>
@@ -5270,7 +5290,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="42" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:3" ht="34" x14ac:dyDescent="0.15">
       <c r="A42" t="s">
         <v>149</v>
       </c>
@@ -5281,7 +5301,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="43" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:3" ht="34" x14ac:dyDescent="0.15">
       <c r="A43" t="s">
         <v>150</v>
       </c>

</xml_diff>

<commit_message>
Implementing US 25 and US 29
- Updated main script to include error for US 22 (unique IDs)
- Updated TestMain to include new unit tests
- Added implementation and unit tests  for US25
- Added implementation and unit tests for US29
- Updated team report
</commit_message>
<xml_diff>
--- a/TeamDReport copy.xlsx
+++ b/TeamDReport copy.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/JP/OneDrive/Jonathan's Folder!/Stevens/CS_555_Agile_Methods_for_SW_Development/Project_Documents/SSW555-DriverlessCar/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBC56346-0AAE-2146-8F33-AE60F349788C}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26F12634-1F64-CA4B-AC4B-9978A0EEF9AD}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="23040" windowHeight="13940" tabRatio="500" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="14400" tabRatio="500" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Team" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="649" uniqueCount="293">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="659" uniqueCount="300">
   <si>
     <t>Date</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -956,6 +956,27 @@
   </si>
   <si>
     <t>Stories that look simple to implement are actually turning out to be complex</t>
+  </si>
+  <si>
+    <t>DeseasedIndividuals.py</t>
+  </si>
+  <si>
+    <t>list_deseased_individuals</t>
+  </si>
+  <si>
+    <t>test_list_deseased</t>
+  </si>
+  <si>
+    <t>TestDeseasedIndividauls,py</t>
+  </si>
+  <si>
+    <t>FamilyValidation.oy</t>
+  </si>
+  <si>
+    <t>check_same_name</t>
+  </si>
+  <si>
+    <t>test_same_name_XXX</t>
   </si>
 </sst>
 </file>
@@ -2532,8 +2553,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E33"/>
   <sheetViews>
-    <sheetView topLeftCell="A27" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A28" sqref="A28:B28"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -2577,7 +2598,7 @@
         <v>195</v>
       </c>
       <c r="E2" s="15" t="s">
-        <v>228</v>
+        <v>287</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="34" x14ac:dyDescent="0.15">
@@ -2594,7 +2615,7 @@
         <v>195</v>
       </c>
       <c r="E3" s="15" t="s">
-        <v>228</v>
+        <v>287</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="34" x14ac:dyDescent="0.15">
@@ -2611,7 +2632,7 @@
         <v>183</v>
       </c>
       <c r="E4" s="15" t="s">
-        <v>228</v>
+        <v>287</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="51" x14ac:dyDescent="0.15">
@@ -2628,7 +2649,7 @@
         <v>183</v>
       </c>
       <c r="E5" s="15" t="s">
-        <v>228</v>
+        <v>287</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="34" x14ac:dyDescent="0.15">
@@ -2645,7 +2666,7 @@
         <v>187</v>
       </c>
       <c r="E6" s="15" t="s">
-        <v>228</v>
+        <v>287</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="34" x14ac:dyDescent="0.15">
@@ -2662,7 +2683,7 @@
         <v>187</v>
       </c>
       <c r="E7" s="15" t="s">
-        <v>228</v>
+        <v>287</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="68" x14ac:dyDescent="0.15">
@@ -2679,7 +2700,7 @@
         <v>183</v>
       </c>
       <c r="E8" s="15" t="s">
-        <v>228</v>
+        <v>287</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="51" x14ac:dyDescent="0.15">
@@ -2696,7 +2717,7 @@
         <v>183</v>
       </c>
       <c r="E9" s="15" t="s">
-        <v>228</v>
+        <v>287</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="51" x14ac:dyDescent="0.15">
@@ -2713,7 +2734,7 @@
         <v>187</v>
       </c>
       <c r="E10" s="15" t="s">
-        <v>228</v>
+        <v>287</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="51" x14ac:dyDescent="0.15">
@@ -2730,7 +2751,7 @@
         <v>182</v>
       </c>
       <c r="E11" s="15" t="s">
-        <v>228</v>
+        <v>287</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="34" x14ac:dyDescent="0.15">
@@ -2747,7 +2768,7 @@
         <v>182</v>
       </c>
       <c r="E12" s="15" t="s">
-        <v>228</v>
+        <v>287</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="68" x14ac:dyDescent="0.15">
@@ -2764,7 +2785,7 @@
         <v>187</v>
       </c>
       <c r="E13" s="15" t="s">
-        <v>228</v>
+        <v>287</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="85" x14ac:dyDescent="0.15">
@@ -2781,7 +2802,7 @@
         <v>182</v>
       </c>
       <c r="E14" s="15" t="s">
-        <v>228</v>
+        <v>287</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="34" x14ac:dyDescent="0.15">
@@ -2798,7 +2819,7 @@
         <v>195</v>
       </c>
       <c r="E15" s="15" t="s">
-        <v>228</v>
+        <v>287</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="34" x14ac:dyDescent="0.15">
@@ -2815,7 +2836,7 @@
         <v>183</v>
       </c>
       <c r="E16" s="15" t="s">
-        <v>228</v>
+        <v>287</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="34" x14ac:dyDescent="0.15">
@@ -2832,7 +2853,7 @@
         <v>187</v>
       </c>
       <c r="E17" s="15" t="s">
-        <v>228</v>
+        <v>287</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="34" x14ac:dyDescent="0.15">
@@ -2849,10 +2870,10 @@
         <v>187</v>
       </c>
       <c r="E18" s="15" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" ht="17" x14ac:dyDescent="0.15">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="34" x14ac:dyDescent="0.15">
       <c r="A19" s="15" t="s">
         <v>126</v>
       </c>
@@ -2866,7 +2887,7 @@
         <v>183</v>
       </c>
       <c r="E19" s="15" t="s">
-        <v>228</v>
+        <v>287</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="34" x14ac:dyDescent="0.15">
@@ -2968,7 +2989,7 @@
         <v>195</v>
       </c>
       <c r="E25" s="15" t="s">
-        <v>161</v>
+        <v>287</v>
       </c>
     </row>
     <row r="26" spans="1:5" ht="34" x14ac:dyDescent="0.15">
@@ -3002,7 +3023,7 @@
         <v>195</v>
       </c>
       <c r="E27" s="15" t="s">
-        <v>228</v>
+        <v>287</v>
       </c>
     </row>
     <row r="28" spans="1:5" ht="34" x14ac:dyDescent="0.15">
@@ -3019,7 +3040,7 @@
         <v>195</v>
       </c>
       <c r="E28" s="15" t="s">
-        <v>161</v>
+        <v>287</v>
       </c>
     </row>
     <row r="29" spans="1:5" ht="34" x14ac:dyDescent="0.15">
@@ -3036,7 +3057,7 @@
         <v>182</v>
       </c>
       <c r="E29" s="15" t="s">
-        <v>228</v>
+        <v>287</v>
       </c>
     </row>
     <row r="30" spans="1:5" ht="34" x14ac:dyDescent="0.15">
@@ -3053,7 +3074,7 @@
         <v>182</v>
       </c>
       <c r="E30" s="15" t="s">
-        <v>228</v>
+        <v>287</v>
       </c>
     </row>
     <row r="31" spans="1:5" ht="34" x14ac:dyDescent="0.15">
@@ -3070,7 +3091,7 @@
         <v>195</v>
       </c>
       <c r="E31" s="15" t="s">
-        <v>228</v>
+        <v>287</v>
       </c>
     </row>
     <row r="32" spans="1:5" ht="34" x14ac:dyDescent="0.15">
@@ -3087,7 +3108,7 @@
         <v>182</v>
       </c>
       <c r="E32" s="15" t="s">
-        <v>228</v>
+        <v>287</v>
       </c>
     </row>
     <row r="33" spans="1:5" ht="51" x14ac:dyDescent="0.15">
@@ -3104,7 +3125,7 @@
         <v>195</v>
       </c>
       <c r="E33" s="15" t="s">
-        <v>228</v>
+        <v>287</v>
       </c>
     </row>
   </sheetData>
@@ -4447,7 +4468,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:P22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+    <sheetView topLeftCell="A8" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
@@ -4939,8 +4960,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:P9"/>
   <sheetViews>
-    <sheetView zoomScale="150" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+    <sheetView tabSelected="1" topLeftCell="L1" zoomScale="150" workbookViewId="0">
+      <selection activeCell="P8" sqref="P8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="21.33203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -4958,7 +4979,7 @@
     <col min="11" max="11" width="16.5" style="32" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="13" style="32" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="21.33203125" style="32"/>
-    <col min="14" max="14" width="9.1640625" style="32" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="18.1640625" style="32" customWidth="1"/>
     <col min="15" max="15" width="14" style="32" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="10.1640625" style="32" bestFit="1" customWidth="1"/>
     <col min="17" max="16384" width="21.33203125" style="32"/>
@@ -5110,11 +5131,41 @@
       <c r="C7" s="32" t="s">
         <v>195</v>
       </c>
+      <c r="D7" s="32" t="s">
+        <v>228</v>
+      </c>
       <c r="E7" s="32">
         <v>50</v>
       </c>
       <c r="F7" s="32">
         <v>2</v>
+      </c>
+      <c r="G7" s="32">
+        <v>45</v>
+      </c>
+      <c r="H7" s="32">
+        <v>1</v>
+      </c>
+      <c r="I7" s="39">
+        <v>42094</v>
+      </c>
+      <c r="J7" s="32" t="s">
+        <v>297</v>
+      </c>
+      <c r="K7" s="32" t="s">
+        <v>298</v>
+      </c>
+      <c r="L7" s="32">
+        <v>37</v>
+      </c>
+      <c r="N7" s="32" t="s">
+        <v>237</v>
+      </c>
+      <c r="O7" s="32" t="s">
+        <v>299</v>
+      </c>
+      <c r="P7" s="32">
+        <v>58</v>
       </c>
     </row>
     <row r="8" spans="1:16" ht="14" x14ac:dyDescent="0.15">
@@ -5137,7 +5188,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="9" spans="1:16" ht="14" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:16" ht="28" x14ac:dyDescent="0.15">
       <c r="A9" s="15" t="s">
         <v>137</v>
       </c>
@@ -5147,11 +5198,41 @@
       <c r="C9" s="32" t="s">
         <v>195</v>
       </c>
+      <c r="D9" s="32" t="s">
+        <v>228</v>
+      </c>
       <c r="E9" s="32">
         <v>45</v>
       </c>
       <c r="F9" s="32">
         <v>2</v>
+      </c>
+      <c r="G9" s="32">
+        <v>28</v>
+      </c>
+      <c r="H9" s="32">
+        <v>1</v>
+      </c>
+      <c r="I9" s="39">
+        <v>42094</v>
+      </c>
+      <c r="J9" s="32" t="s">
+        <v>293</v>
+      </c>
+      <c r="K9" s="32" t="s">
+        <v>294</v>
+      </c>
+      <c r="L9" s="32">
+        <v>20</v>
+      </c>
+      <c r="N9" s="32" t="s">
+        <v>296</v>
+      </c>
+      <c r="O9" s="32" t="s">
+        <v>295</v>
+      </c>
+      <c r="P9" s="32">
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add stories of US23, US24 to the ged file and update the report
</commit_message>
<xml_diff>
--- a/TeamDReport copy.xlsx
+++ b/TeamDReport copy.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10709"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10309"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/michaelramos/SSW555-DriverlessCar/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/franklin/SSW555/SSW555-DriverlessCar/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE3A47C3-17CF-804B-B46C-4838EEC70915}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6F54F46-DAFC-7E46-BB0D-7CBBE176F40E}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="23040" windowHeight="14400" tabRatio="500" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2660" yWindow="500" windowWidth="23040" windowHeight="14400" tabRatio="500" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Team" sheetId="1" r:id="rId1"/>
@@ -23,10 +23,17 @@
     <sheet name="Sprint4" sheetId="6" r:id="rId8"/>
     <sheet name="Stories" sheetId="11" r:id="rId9"/>
   </sheets>
-  <calcPr calcId="179021"/>
+  <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="330"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
     </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -36,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="659" uniqueCount="300">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="667" uniqueCount="308">
   <si>
     <t>Date</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -971,6 +978,30 @@
   </si>
   <si>
     <t>test_same_name_XXX</t>
+  </si>
+  <si>
+    <t>unique_name_birth.py</t>
+  </si>
+  <si>
+    <t>unique_name_and_birth</t>
+  </si>
+  <si>
+    <t>unique_family_spouses_marriage_date.py</t>
+  </si>
+  <si>
+    <t>unique_family_spouse_marriage_date</t>
+  </si>
+  <si>
+    <t>test_unique_name_birth.py</t>
+  </si>
+  <si>
+    <t>test_valid_unique_name_and_birth, test_unique_name_and_birth_invalid_name, test_unique_name_and_birth_invalid_birth</t>
+  </si>
+  <si>
+    <t>test_unique_family_spouses_marriage_date.py</t>
+  </si>
+  <si>
+    <t>test_valid_spouses_and_marriage_date, test_unique_family_spouses_name, test_unique_family_marriage_date</t>
   </si>
 </sst>
 </file>
@@ -2527,7 +2558,7 @@
       </c>
     </row>
   </sheetData>
-  <sortState ref="A4:D6">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A4:D6">
     <sortCondition ref="C4:C6"/>
   </sortState>
   <phoneticPr fontId="2" type="noConversion"/>
@@ -2578,7 +2609,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="32" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:5" ht="34" x14ac:dyDescent="0.15">
       <c r="A2" s="15" t="s">
         <v>109</v>
       </c>
@@ -2595,7 +2626,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="32" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:5" ht="34" x14ac:dyDescent="0.15">
       <c r="A3" s="15" t="s">
         <v>110</v>
       </c>
@@ -2612,7 +2643,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="32" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:5" ht="34" x14ac:dyDescent="0.15">
       <c r="A4" s="15" t="s">
         <v>111</v>
       </c>
@@ -2629,7 +2660,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="48" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:5" ht="51" x14ac:dyDescent="0.15">
       <c r="A5" s="15" t="s">
         <v>112</v>
       </c>
@@ -2646,7 +2677,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="32" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:5" ht="34" x14ac:dyDescent="0.15">
       <c r="A6" s="15" t="s">
         <v>113</v>
       </c>
@@ -2663,7 +2694,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="32" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:5" ht="34" x14ac:dyDescent="0.15">
       <c r="A7" s="15" t="s">
         <v>114</v>
       </c>
@@ -2680,7 +2711,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="64" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:5" ht="68" x14ac:dyDescent="0.15">
       <c r="A8" s="15" t="s">
         <v>115</v>
       </c>
@@ -2697,7 +2728,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="48" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:5" ht="51" x14ac:dyDescent="0.15">
       <c r="A9" s="15" t="s">
         <v>116</v>
       </c>
@@ -2714,7 +2745,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="48" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:5" ht="51" x14ac:dyDescent="0.15">
       <c r="A10" s="15" t="s">
         <v>117</v>
       </c>
@@ -2731,7 +2762,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="48" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:5" ht="51" x14ac:dyDescent="0.15">
       <c r="A11" s="15" t="s">
         <v>118</v>
       </c>
@@ -2748,7 +2779,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="32" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:5" ht="34" x14ac:dyDescent="0.15">
       <c r="A12" s="15" t="s">
         <v>119</v>
       </c>
@@ -2765,7 +2796,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="64" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:5" ht="68" x14ac:dyDescent="0.15">
       <c r="A13" s="15" t="s">
         <v>120</v>
       </c>
@@ -2782,7 +2813,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="80" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:5" ht="85" x14ac:dyDescent="0.15">
       <c r="A14" s="15" t="s">
         <v>121</v>
       </c>
@@ -2799,7 +2830,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="32" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:5" ht="34" x14ac:dyDescent="0.15">
       <c r="A15" s="15" t="s">
         <v>122</v>
       </c>
@@ -2816,7 +2847,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="32" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:5" ht="34" x14ac:dyDescent="0.15">
       <c r="A16" s="15" t="s">
         <v>123</v>
       </c>
@@ -2833,7 +2864,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="32" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:5" ht="34" x14ac:dyDescent="0.15">
       <c r="A17" s="15" t="s">
         <v>124</v>
       </c>
@@ -2850,7 +2881,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="32" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:5" ht="34" x14ac:dyDescent="0.15">
       <c r="A18" s="15" t="s">
         <v>125</v>
       </c>
@@ -2867,7 +2898,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="16" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:5" ht="17" x14ac:dyDescent="0.15">
       <c r="A19" s="15" t="s">
         <v>126</v>
       </c>
@@ -2884,7 +2915,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="32" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:5" ht="34" x14ac:dyDescent="0.15">
       <c r="A20" s="15" t="s">
         <v>127</v>
       </c>
@@ -2901,7 +2932,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="32" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:5" ht="34" x14ac:dyDescent="0.15">
       <c r="A21" s="15" t="s">
         <v>128</v>
       </c>
@@ -2918,7 +2949,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="22" spans="1:5" ht="32" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:5" ht="34" x14ac:dyDescent="0.15">
       <c r="A22" s="15" t="s">
         <v>130</v>
       </c>
@@ -2935,7 +2966,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="23" spans="1:5" ht="48" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:5" ht="51" x14ac:dyDescent="0.15">
       <c r="A23" s="15" t="s">
         <v>131</v>
       </c>
@@ -2952,7 +2983,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="24" spans="1:5" ht="64" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:5" ht="68" x14ac:dyDescent="0.15">
       <c r="A24" s="15" t="s">
         <v>132</v>
       </c>
@@ -2969,7 +3000,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="25" spans="1:5" ht="48" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:5" ht="51" x14ac:dyDescent="0.15">
       <c r="A25" s="15" t="s">
         <v>133</v>
       </c>
@@ -2986,7 +3017,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="26" spans="1:5" ht="32" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:5" ht="34" x14ac:dyDescent="0.15">
       <c r="A26" s="15" t="s">
         <v>135</v>
       </c>
@@ -3003,7 +3034,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="27" spans="1:5" ht="32" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:5" ht="34" x14ac:dyDescent="0.15">
       <c r="A27" s="15" t="s">
         <v>136</v>
       </c>
@@ -3020,7 +3051,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="28" spans="1:5" ht="32" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:5" ht="34" x14ac:dyDescent="0.15">
       <c r="A28" s="15" t="s">
         <v>137</v>
       </c>
@@ -3037,7 +3068,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="29" spans="1:5" ht="32" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:5" ht="34" x14ac:dyDescent="0.15">
       <c r="A29" s="15" t="s">
         <v>138</v>
       </c>
@@ -3054,7 +3085,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="30" spans="1:5" ht="32" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:5" ht="34" x14ac:dyDescent="0.15">
       <c r="A30" s="15" t="s">
         <v>139</v>
       </c>
@@ -3071,7 +3102,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="31" spans="1:5" ht="32" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:5" ht="34" x14ac:dyDescent="0.15">
       <c r="A31" s="15" t="s">
         <v>140</v>
       </c>
@@ -3088,7 +3119,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="32" spans="1:5" ht="32" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:5" ht="34" x14ac:dyDescent="0.15">
       <c r="A32" s="15" t="s">
         <v>149</v>
       </c>
@@ -3105,7 +3136,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="33" spans="1:5" ht="48" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:5" ht="51" x14ac:dyDescent="0.15">
       <c r="A33" s="15" t="s">
         <v>150</v>
       </c>
@@ -3478,7 +3509,7 @@
     <col min="17" max="16384" width="10.83203125" style="15"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:16" ht="14" x14ac:dyDescent="0.15">
       <c r="A1" s="14" t="s">
         <v>9</v>
       </c>
@@ -3525,7 +3556,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="2" spans="1:16" ht="26" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:16" ht="28" x14ac:dyDescent="0.15">
       <c r="A2" s="15" t="s">
         <v>109</v>
       </c>
@@ -3572,7 +3603,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:16" ht="26" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:16" ht="28" x14ac:dyDescent="0.15">
       <c r="A3" s="15" t="s">
         <v>110</v>
       </c>
@@ -3619,7 +3650,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:16" ht="26" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:16" ht="28" x14ac:dyDescent="0.15">
       <c r="A4" s="15" t="s">
         <v>111</v>
       </c>
@@ -3666,7 +3697,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="5" spans="1:16" ht="26" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:16" ht="28" x14ac:dyDescent="0.15">
       <c r="A5" s="15" t="s">
         <v>112</v>
       </c>
@@ -3713,7 +3744,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="6" spans="1:16" ht="26" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:16" ht="28" x14ac:dyDescent="0.15">
       <c r="A6" s="15" t="s">
         <v>113</v>
       </c>
@@ -3760,7 +3791,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:16" ht="26" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:16" ht="28" x14ac:dyDescent="0.15">
       <c r="A7" s="15" t="s">
         <v>114</v>
       </c>
@@ -3807,7 +3838,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:16" ht="39" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:16" ht="42" x14ac:dyDescent="0.15">
       <c r="A8" s="15" t="s">
         <v>118</v>
       </c>
@@ -3854,7 +3885,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="9" spans="1:16" ht="26" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:16" ht="28" x14ac:dyDescent="0.15">
       <c r="A9" s="15" t="s">
         <v>119</v>
       </c>
@@ -3909,7 +3940,7 @@
       <c r="O10" s="27"/>
       <c r="P10" s="26"/>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:16" ht="14" x14ac:dyDescent="0.15">
       <c r="B13" s="19" t="s">
         <v>200</v>
       </c>
@@ -3917,12 +3948,12 @@
     <row r="14" spans="1:16" x14ac:dyDescent="0.15">
       <c r="B14" s="29"/>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:16" ht="14" x14ac:dyDescent="0.15">
       <c r="B15" s="30" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="16" spans="1:16" ht="22" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:16" ht="24" x14ac:dyDescent="0.15">
       <c r="B16" s="31" t="s">
         <v>230</v>
       </c>
@@ -3930,17 +3961,17 @@
     <row r="17" spans="2:2" x14ac:dyDescent="0.15">
       <c r="B17" s="19"/>
     </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.15">
+    <row r="18" spans="2:2" ht="14" x14ac:dyDescent="0.15">
       <c r="B18" s="30" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="19" spans="2:2" ht="66" x14ac:dyDescent="0.15">
+    <row r="19" spans="2:2" ht="72" x14ac:dyDescent="0.15">
       <c r="B19" s="31" t="s">
         <v>229</v>
       </c>
     </row>
-    <row r="21" spans="2:2" x14ac:dyDescent="0.15">
+    <row r="21" spans="2:2" ht="14" x14ac:dyDescent="0.15">
       <c r="B21" s="30" t="s">
         <v>203</v>
       </c>
@@ -4027,7 +4058,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="2" spans="1:16" s="36" customFormat="1" ht="78" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:16" s="36" customFormat="1" ht="84" x14ac:dyDescent="0.15">
       <c r="A2" s="36" t="s">
         <v>115</v>
       </c>
@@ -4074,7 +4105,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="3" spans="1:16" s="36" customFormat="1" ht="91" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:16" s="36" customFormat="1" ht="98" x14ac:dyDescent="0.15">
       <c r="A3" s="36" t="s">
         <v>116</v>
       </c>
@@ -4121,7 +4152,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="4" spans="1:16" s="36" customFormat="1" ht="39" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:16" s="36" customFormat="1" ht="42" x14ac:dyDescent="0.15">
       <c r="A4" s="36" t="s">
         <v>117</v>
       </c>
@@ -4168,7 +4199,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:16" s="36" customFormat="1" ht="26" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:16" s="36" customFormat="1" ht="28" x14ac:dyDescent="0.15">
       <c r="A5" s="36" t="s">
         <v>120</v>
       </c>
@@ -4215,7 +4246,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:16" s="36" customFormat="1" ht="26" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:16" s="36" customFormat="1" ht="28" x14ac:dyDescent="0.15">
       <c r="A6" s="36" t="s">
         <v>121</v>
       </c>
@@ -4262,7 +4293,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:16" s="36" customFormat="1" ht="39" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:16" s="36" customFormat="1" ht="42" x14ac:dyDescent="0.15">
       <c r="A7" s="36" t="s">
         <v>122</v>
       </c>
@@ -4309,7 +4340,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="8" spans="1:16" s="36" customFormat="1" ht="26" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:16" s="36" customFormat="1" ht="28" x14ac:dyDescent="0.15">
       <c r="A8" s="36" t="s">
         <v>149</v>
       </c>
@@ -4356,7 +4387,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:16" s="36" customFormat="1" ht="26" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:16" s="36" customFormat="1" ht="28" x14ac:dyDescent="0.15">
       <c r="A9" s="36" t="s">
         <v>150</v>
       </c>
@@ -4407,7 +4438,7 @@
     <row r="11" spans="1:16" s="36" customFormat="1" x14ac:dyDescent="0.15"/>
     <row r="12" spans="1:16" s="36" customFormat="1" x14ac:dyDescent="0.15"/>
     <row r="13" spans="1:16" s="36" customFormat="1" x14ac:dyDescent="0.15"/>
-    <row r="14" spans="1:16" s="36" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:16" s="36" customFormat="1" ht="14" x14ac:dyDescent="0.15">
       <c r="B14" s="19" t="s">
         <v>200</v>
       </c>
@@ -4415,12 +4446,12 @@
     <row r="15" spans="1:16" s="36" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B15" s="29"/>
     </row>
-    <row r="16" spans="1:16" s="36" customFormat="1" ht="26" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:16" s="36" customFormat="1" ht="28" x14ac:dyDescent="0.15">
       <c r="B16" s="30" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="17" spans="2:2" s="36" customFormat="1" ht="22" x14ac:dyDescent="0.15">
+    <row r="17" spans="2:2" s="36" customFormat="1" ht="24" x14ac:dyDescent="0.15">
       <c r="B17" s="31" t="s">
         <v>262</v>
       </c>
@@ -4428,12 +4459,12 @@
     <row r="18" spans="2:2" s="36" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B18" s="19"/>
     </row>
-    <row r="19" spans="2:2" s="36" customFormat="1" ht="26" x14ac:dyDescent="0.15">
+    <row r="19" spans="2:2" s="36" customFormat="1" ht="28" x14ac:dyDescent="0.15">
       <c r="B19" s="30" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="20" spans="2:2" s="36" customFormat="1" ht="66" x14ac:dyDescent="0.15">
+    <row r="20" spans="2:2" s="36" customFormat="1" ht="72" x14ac:dyDescent="0.15">
       <c r="B20" s="31" t="s">
         <v>263</v>
       </c>
@@ -4441,12 +4472,12 @@
     <row r="21" spans="2:2" x14ac:dyDescent="0.15">
       <c r="B21" s="17"/>
     </row>
-    <row r="22" spans="2:2" x14ac:dyDescent="0.15">
+    <row r="22" spans="2:2" ht="14" x14ac:dyDescent="0.15">
       <c r="B22" s="30" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="23" spans="2:2" ht="33" x14ac:dyDescent="0.15">
+    <row r="23" spans="2:2" ht="36" x14ac:dyDescent="0.15">
       <c r="B23" s="31" t="s">
         <v>261</v>
       </c>
@@ -4524,7 +4555,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="2" spans="1:16" ht="78" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:16" ht="84" x14ac:dyDescent="0.15">
       <c r="A2" s="32" t="s">
         <v>123</v>
       </c>
@@ -4571,7 +4602,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="3" spans="1:16" ht="26" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:16" ht="28" x14ac:dyDescent="0.15">
       <c r="A3" s="32" t="s">
         <v>124</v>
       </c>
@@ -4618,7 +4649,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="4" spans="1:16" ht="52" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:16" ht="56" x14ac:dyDescent="0.15">
       <c r="A4" s="32" t="s">
         <v>125</v>
       </c>
@@ -4665,7 +4696,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="5" spans="1:16" ht="39" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:16" ht="42" x14ac:dyDescent="0.15">
       <c r="A5" s="32" t="s">
         <v>126</v>
       </c>
@@ -4712,7 +4743,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="6" spans="1:16" ht="39" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:16" ht="42" x14ac:dyDescent="0.15">
       <c r="A6" s="32" t="s">
         <v>136</v>
       </c>
@@ -4759,7 +4790,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="7" spans="1:16" ht="208" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:16" ht="224" x14ac:dyDescent="0.15">
       <c r="A7" s="32" t="s">
         <v>138</v>
       </c>
@@ -4806,7 +4837,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="8" spans="1:16" ht="208" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:16" ht="224" x14ac:dyDescent="0.15">
       <c r="A8" s="32" t="s">
         <v>139</v>
       </c>
@@ -4853,7 +4884,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="9" spans="1:16" ht="39" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:16" ht="42" x14ac:dyDescent="0.15">
       <c r="A9" s="32" t="s">
         <v>140</v>
       </c>
@@ -4913,7 +4944,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="16" spans="1:16" ht="48" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:16" ht="52" x14ac:dyDescent="0.15">
       <c r="B16" s="42" t="s">
         <v>290</v>
       </c>
@@ -4926,7 +4957,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="19" spans="2:2" ht="60" x14ac:dyDescent="0.15">
+    <row r="19" spans="2:2" ht="65" x14ac:dyDescent="0.15">
       <c r="B19" s="42" t="s">
         <v>291</v>
       </c>
@@ -4939,7 +4970,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="22" spans="2:2" ht="36" x14ac:dyDescent="0.15">
+    <row r="22" spans="2:2" ht="39" x14ac:dyDescent="0.15">
       <c r="B22" s="42" t="s">
         <v>292</v>
       </c>
@@ -4954,8 +4985,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:P9"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+    <sheetView tabSelected="1" topLeftCell="B6" zoomScale="150" workbookViewId="0">
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="21.33203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -5027,7 +5058,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="2" spans="1:16" ht="26" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:16" ht="28" x14ac:dyDescent="0.15">
       <c r="A2" s="32" t="s">
         <v>127</v>
       </c>
@@ -5044,7 +5075,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:16" ht="14" x14ac:dyDescent="0.15">
       <c r="A3" s="32" t="s">
         <v>128</v>
       </c>
@@ -5061,7 +5092,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:16" ht="14" x14ac:dyDescent="0.15">
       <c r="A4" s="32" t="s">
         <v>130</v>
       </c>
@@ -5082,7 +5113,7 @@
       </c>
       <c r="I4" s="39"/>
     </row>
-    <row r="5" spans="1:16" ht="26" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:16" ht="126" x14ac:dyDescent="0.15">
       <c r="A5" s="32" t="s">
         <v>131</v>
       </c>
@@ -5098,8 +5129,35 @@
       <c r="F5" s="32">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:16" ht="26" x14ac:dyDescent="0.15">
+      <c r="G5" s="32">
+        <v>22</v>
+      </c>
+      <c r="H5" s="32">
+        <v>1</v>
+      </c>
+      <c r="I5" s="39">
+        <v>42096</v>
+      </c>
+      <c r="J5" s="32" t="s">
+        <v>300</v>
+      </c>
+      <c r="K5" s="36" t="s">
+        <v>301</v>
+      </c>
+      <c r="L5" s="32">
+        <v>20</v>
+      </c>
+      <c r="N5" s="36" t="s">
+        <v>304</v>
+      </c>
+      <c r="O5" s="36" t="s">
+        <v>305</v>
+      </c>
+      <c r="P5" s="32">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" ht="126" x14ac:dyDescent="0.15">
       <c r="A6" s="32" t="s">
         <v>132</v>
       </c>
@@ -5115,8 +5173,35 @@
       <c r="F6" s="32">
         <v>2</v>
       </c>
-    </row>
-    <row r="7" spans="1:16" ht="26" x14ac:dyDescent="0.15">
+      <c r="G6" s="32">
+        <v>32</v>
+      </c>
+      <c r="H6" s="32">
+        <v>1</v>
+      </c>
+      <c r="I6" s="39">
+        <v>42096</v>
+      </c>
+      <c r="J6" s="36" t="s">
+        <v>302</v>
+      </c>
+      <c r="K6" s="36" t="s">
+        <v>303</v>
+      </c>
+      <c r="L6" s="32">
+        <v>29</v>
+      </c>
+      <c r="N6" s="36" t="s">
+        <v>306</v>
+      </c>
+      <c r="O6" s="36" t="s">
+        <v>307</v>
+      </c>
+      <c r="P6" s="32">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" ht="28" x14ac:dyDescent="0.15">
       <c r="A7" s="32" t="s">
         <v>133</v>
       </c>
@@ -5163,7 +5248,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:16" ht="14" x14ac:dyDescent="0.15">
       <c r="A8" s="32" t="s">
         <v>135</v>
       </c>
@@ -5183,7 +5268,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="9" spans="1:16" ht="26" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:16" ht="28" x14ac:dyDescent="0.15">
       <c r="A9" s="15" t="s">
         <v>137</v>
       </c>
@@ -5250,7 +5335,7 @@
     <col min="3" max="3" width="49.5" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:3" s="4" customFormat="1" ht="14" x14ac:dyDescent="0.15">
       <c r="A1" s="4" t="s">
         <v>108</v>
       </c>
@@ -5261,7 +5346,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="32" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:3" ht="34" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
         <v>109</v>
       </c>
@@ -5272,7 +5357,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="16" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:3" ht="17" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
         <v>110</v>
       </c>
@@ -5283,7 +5368,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="16" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:3" ht="17" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
         <v>111</v>
       </c>
@@ -5294,7 +5379,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="32" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:3" ht="34" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
         <v>112</v>
       </c>
@@ -5305,7 +5390,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="16" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:3" ht="17" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
         <v>113</v>
       </c>
@@ -5316,7 +5401,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="16" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:3" ht="17" x14ac:dyDescent="0.15">
       <c r="A7" t="s">
         <v>114</v>
       </c>
@@ -5327,7 +5412,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="48" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:3" ht="51" x14ac:dyDescent="0.15">
       <c r="A8" t="s">
         <v>115</v>
       </c>
@@ -5338,7 +5423,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="32" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:3" ht="34" x14ac:dyDescent="0.15">
       <c r="A9" t="s">
         <v>116</v>
       </c>
@@ -5349,7 +5434,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="32" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:3" ht="34" x14ac:dyDescent="0.15">
       <c r="A10" t="s">
         <v>117</v>
       </c>
@@ -5360,7 +5445,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="32" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:3" ht="34" x14ac:dyDescent="0.15">
       <c r="A11" t="s">
         <v>118</v>
       </c>
@@ -5371,7 +5456,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="32" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:3" ht="34" x14ac:dyDescent="0.15">
       <c r="A12" t="s">
         <v>119</v>
       </c>
@@ -5382,7 +5467,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="48" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:3" ht="51" x14ac:dyDescent="0.15">
       <c r="A13" t="s">
         <v>120</v>
       </c>
@@ -5393,7 +5478,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="64" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:3" ht="68" x14ac:dyDescent="0.15">
       <c r="A14" t="s">
         <v>121</v>
       </c>
@@ -5404,7 +5489,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="32" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:3" ht="34" x14ac:dyDescent="0.15">
       <c r="A15" t="s">
         <v>122</v>
       </c>
@@ -5415,7 +5500,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="16" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:3" ht="17" x14ac:dyDescent="0.15">
       <c r="A16" t="s">
         <v>123</v>
       </c>
@@ -5426,7 +5511,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="32" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:3" ht="34" x14ac:dyDescent="0.15">
       <c r="A17" t="s">
         <v>124</v>
       </c>
@@ -5437,7 +5522,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="16" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:3" ht="17" x14ac:dyDescent="0.15">
       <c r="A18" t="s">
         <v>125</v>
       </c>
@@ -5448,7 +5533,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="16" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:3" ht="17" x14ac:dyDescent="0.15">
       <c r="A19" t="s">
         <v>126</v>
       </c>
@@ -5459,7 +5544,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="16" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:3" ht="17" x14ac:dyDescent="0.15">
       <c r="A20" t="s">
         <v>127</v>
       </c>
@@ -5470,7 +5555,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="32" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:3" ht="34" x14ac:dyDescent="0.15">
       <c r="A21" t="s">
         <v>128</v>
       </c>
@@ -5481,7 +5566,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="32" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:3" ht="34" x14ac:dyDescent="0.15">
       <c r="A22" t="s">
         <v>129</v>
       </c>
@@ -5492,7 +5577,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="32" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:3" ht="34" x14ac:dyDescent="0.15">
       <c r="A23" t="s">
         <v>130</v>
       </c>
@@ -5503,7 +5588,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="32" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:3" ht="34" x14ac:dyDescent="0.15">
       <c r="A24" t="s">
         <v>131</v>
       </c>
@@ -5514,7 +5599,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="48" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:3" ht="51" x14ac:dyDescent="0.15">
       <c r="A25" t="s">
         <v>132</v>
       </c>
@@ -5525,7 +5610,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="32" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:3" ht="34" x14ac:dyDescent="0.15">
       <c r="A26" t="s">
         <v>133</v>
       </c>
@@ -5536,7 +5621,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="128" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:3" ht="136" x14ac:dyDescent="0.15">
       <c r="A27" t="s">
         <v>134</v>
       </c>
@@ -5547,7 +5632,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="32" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:3" ht="17" x14ac:dyDescent="0.15">
       <c r="A28" t="s">
         <v>135</v>
       </c>
@@ -5558,7 +5643,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="32" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:3" ht="34" x14ac:dyDescent="0.15">
       <c r="A29" t="s">
         <v>136</v>
       </c>
@@ -5569,7 +5654,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="30" spans="1:3" ht="16" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:3" ht="17" x14ac:dyDescent="0.15">
       <c r="A30" t="s">
         <v>137</v>
       </c>
@@ -5580,7 +5665,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="31" spans="1:3" ht="16" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:3" ht="17" x14ac:dyDescent="0.15">
       <c r="A31" t="s">
         <v>138</v>
       </c>
@@ -5591,7 +5676,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="32" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:3" ht="34" x14ac:dyDescent="0.15">
       <c r="A32" t="s">
         <v>139</v>
       </c>
@@ -5602,7 +5687,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="33" spans="1:3" ht="16" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:3" ht="17" x14ac:dyDescent="0.15">
       <c r="A33" t="s">
         <v>140</v>
       </c>
@@ -5613,7 +5698,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="34" spans="1:3" ht="32" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:3" ht="34" x14ac:dyDescent="0.15">
       <c r="A34" t="s">
         <v>141</v>
       </c>
@@ -5624,7 +5709,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="35" spans="1:3" ht="48" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:3" ht="51" x14ac:dyDescent="0.15">
       <c r="A35" t="s">
         <v>142</v>
       </c>
@@ -5635,7 +5720,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="36" spans="1:3" ht="32" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:3" ht="34" x14ac:dyDescent="0.15">
       <c r="A36" t="s">
         <v>143</v>
       </c>
@@ -5646,7 +5731,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="37" spans="1:3" ht="32" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:3" ht="34" x14ac:dyDescent="0.15">
       <c r="A37" t="s">
         <v>144</v>
       </c>
@@ -5657,7 +5742,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="38" spans="1:3" ht="32" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:3" ht="34" x14ac:dyDescent="0.15">
       <c r="A38" t="s">
         <v>145</v>
       </c>
@@ -5668,7 +5753,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="39" spans="1:3" ht="32" x14ac:dyDescent="0.15">
+    <row r="39" spans="1:3" ht="34" x14ac:dyDescent="0.15">
       <c r="A39" t="s">
         <v>146</v>
       </c>
@@ -5679,7 +5764,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="40" spans="1:3" ht="32" x14ac:dyDescent="0.15">
+    <row r="40" spans="1:3" ht="34" x14ac:dyDescent="0.15">
       <c r="A40" t="s">
         <v>147</v>
       </c>
@@ -5690,7 +5775,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="41" spans="1:3" ht="32" x14ac:dyDescent="0.15">
+    <row r="41" spans="1:3" ht="34" x14ac:dyDescent="0.15">
       <c r="A41" t="s">
         <v>148</v>
       </c>
@@ -5701,7 +5786,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="42" spans="1:3" ht="32" x14ac:dyDescent="0.15">
+    <row r="42" spans="1:3" ht="34" x14ac:dyDescent="0.15">
       <c r="A42" t="s">
         <v>149</v>
       </c>
@@ -5712,7 +5797,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="43" spans="1:3" ht="32" x14ac:dyDescent="0.15">
+    <row r="43" spans="1:3" ht="34" x14ac:dyDescent="0.15">
       <c r="A43" t="s">
         <v>150</v>
       </c>

</xml_diff>

<commit_message>
Revert "Merge branch 'master' of https://github.com/EricLin24/SSW555-DriverlessCar"
This reverts commit 112628938f5be3419f698e811d87e9e7048f815b, reversing
changes made to 7cc5978e59ee65751dd8d4f5cffb9e610361d00c.
</commit_message>
<xml_diff>
--- a/TeamDReport copy.xlsx
+++ b/TeamDReport copy.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10309"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20730"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/franklin/SSW555/SSW555-DriverlessCar/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Funbucket24\Documents\GitHub\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{244EACD8-0D17-A34E-BA9E-F0E0BE48DAF7}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{D7A2F1E4-39D7-4456-BEE1-BCBDF390EEC2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="12220" tabRatio="500" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" tabRatio="500" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Team" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,6 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
       </xcalcf:calcFeatures>
     </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
@@ -42,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="679" uniqueCount="312">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="669" uniqueCount="304">
   <si>
     <t>Date</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -989,30 +988,6 @@
   </si>
   <si>
     <t>TestCousinMarrages</t>
-  </si>
-  <si>
-    <t>unique_name_birth.py</t>
-  </si>
-  <si>
-    <t>unique_name_and_birth</t>
-  </si>
-  <si>
-    <t>test_unique_name_birth.py</t>
-  </si>
-  <si>
-    <t>test_valid_unique_name_and_birth, test_unique_name_and_birth_invalid_name, test_unique_name_and_birth_invalid_birth</t>
-  </si>
-  <si>
-    <t>unique_family_spouses_marriage_date.py</t>
-  </si>
-  <si>
-    <t>unique_family_spouse_marriage_date</t>
-  </si>
-  <si>
-    <t>test_unique_family_spouses_marriage_date.py</t>
-  </si>
-  <si>
-    <t>test_valid_spouses_and_marriage_date, test_unique_family_spouses_name, test_unique_family_marriage_date</t>
   </si>
 </sst>
 </file>
@@ -1400,7 +1375,7 @@
             <c:numRef>
               <c:f>'Burndown README'!$B$15:$B$20</c:f>
               <c:numCache>
-                <c:formatCode>m/d/yy</c:formatCode>
+                <c:formatCode>m/d/yyyy</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
                   <c:v>41065</c:v>
@@ -1471,7 +1446,7 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:numFmt formatCode="m/d/yy" sourceLinked="1"/>
+        <c:numFmt formatCode="m/d/yyyy" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -2467,15 +2442,15 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="7.83203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="8.5" customWidth="1"/>
     <col min="4" max="5" width="20.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>19</v>
       </c>
@@ -2492,7 +2467,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="2" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="12" t="s">
         <v>183</v>
       </c>
@@ -2509,7 +2484,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>182</v>
       </c>
@@ -2526,7 +2501,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="12" t="s">
         <v>187</v>
       </c>
@@ -2543,7 +2518,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="12" t="s">
         <v>195</v>
       </c>
@@ -2560,7 +2535,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="D10" s="4" t="s">
         <v>31</v>
       </c>
@@ -2569,7 +2544,7 @@
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A4:D6">
+  <sortState ref="A4:D6">
     <sortCondition ref="C4:C6"/>
   </sortState>
   <phoneticPr fontId="2" type="noConversion"/>
@@ -2589,21 +2564,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E33"/>
   <sheetViews>
-    <sheetView topLeftCell="A17" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="6.83203125" style="15" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="29.1640625" style="15" customWidth="1"/>
+    <col min="1" max="1" width="6.875" style="15" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="29.125" style="15" customWidth="1"/>
     <col min="3" max="3" width="34.5" style="15" customWidth="1"/>
-    <col min="4" max="4" width="6.6640625" style="15" customWidth="1"/>
-    <col min="5" max="5" width="10.33203125" style="15" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="10.83203125" style="15"/>
+    <col min="4" max="4" width="6.625" style="15" customWidth="1"/>
+    <col min="5" max="5" width="10.375" style="15" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="10.875" style="15"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="14" t="s">
         <v>29</v>
       </c>
@@ -2620,7 +2595,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="34" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:5" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A2" s="15" t="s">
         <v>109</v>
       </c>
@@ -2637,7 +2612,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="34" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:5" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A3" s="15" t="s">
         <v>110</v>
       </c>
@@ -2654,7 +2629,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="34" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:5" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A4" s="15" t="s">
         <v>111</v>
       </c>
@@ -2671,7 +2646,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="51" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:5" ht="47.25" x14ac:dyDescent="0.2">
       <c r="A5" s="15" t="s">
         <v>112</v>
       </c>
@@ -2688,7 +2663,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="34" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:5" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A6" s="15" t="s">
         <v>113</v>
       </c>
@@ -2705,7 +2680,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="34" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:5" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A7" s="15" t="s">
         <v>114</v>
       </c>
@@ -2722,7 +2697,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="68" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:5" ht="63" x14ac:dyDescent="0.2">
       <c r="A8" s="15" t="s">
         <v>115</v>
       </c>
@@ -2739,7 +2714,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="51" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:5" ht="47.25" x14ac:dyDescent="0.2">
       <c r="A9" s="15" t="s">
         <v>116</v>
       </c>
@@ -2756,7 +2731,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="51" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:5" ht="47.25" x14ac:dyDescent="0.2">
       <c r="A10" s="15" t="s">
         <v>117</v>
       </c>
@@ -2773,7 +2748,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="51" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:5" ht="47.25" x14ac:dyDescent="0.2">
       <c r="A11" s="15" t="s">
         <v>118</v>
       </c>
@@ -2790,7 +2765,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="34" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:5" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A12" s="15" t="s">
         <v>119</v>
       </c>
@@ -2807,7 +2782,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="68" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:5" ht="63" x14ac:dyDescent="0.2">
       <c r="A13" s="15" t="s">
         <v>120</v>
       </c>
@@ -2824,7 +2799,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="85" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:5" ht="78.75" x14ac:dyDescent="0.2">
       <c r="A14" s="15" t="s">
         <v>121</v>
       </c>
@@ -2841,7 +2816,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="34" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:5" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A15" s="15" t="s">
         <v>122</v>
       </c>
@@ -2858,7 +2833,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="34" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:5" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A16" s="15" t="s">
         <v>123</v>
       </c>
@@ -2875,7 +2850,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="34" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:5" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A17" s="15" t="s">
         <v>124</v>
       </c>
@@ -2892,7 +2867,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="34" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:5" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A18" s="15" t="s">
         <v>125</v>
       </c>
@@ -2909,7 +2884,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="17" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:5" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A19" s="15" t="s">
         <v>126</v>
       </c>
@@ -2926,7 +2901,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="34" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:5" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A20" s="15" t="s">
         <v>127</v>
       </c>
@@ -2943,7 +2918,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="34" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:5" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A21" s="15" t="s">
         <v>128</v>
       </c>
@@ -2960,7 +2935,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="22" spans="1:5" ht="34" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:5" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A22" s="15" t="s">
         <v>130</v>
       </c>
@@ -2977,7 +2952,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="23" spans="1:5" ht="51" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:5" ht="47.25" x14ac:dyDescent="0.2">
       <c r="A23" s="15" t="s">
         <v>131</v>
       </c>
@@ -2994,7 +2969,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="24" spans="1:5" ht="68" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:5" ht="63" x14ac:dyDescent="0.2">
       <c r="A24" s="15" t="s">
         <v>132</v>
       </c>
@@ -3011,7 +2986,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="25" spans="1:5" ht="51" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:5" ht="47.25" x14ac:dyDescent="0.2">
       <c r="A25" s="15" t="s">
         <v>133</v>
       </c>
@@ -3028,7 +3003,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="26" spans="1:5" ht="34" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:5" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A26" s="15" t="s">
         <v>135</v>
       </c>
@@ -3045,7 +3020,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="27" spans="1:5" ht="34" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:5" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A27" s="15" t="s">
         <v>136</v>
       </c>
@@ -3062,7 +3037,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="28" spans="1:5" ht="34" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:5" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A28" s="15" t="s">
         <v>137</v>
       </c>
@@ -3079,7 +3054,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="29" spans="1:5" ht="34" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:5" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A29" s="15" t="s">
         <v>138</v>
       </c>
@@ -3096,7 +3071,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="30" spans="1:5" ht="34" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:5" ht="47.25" x14ac:dyDescent="0.2">
       <c r="A30" s="15" t="s">
         <v>139</v>
       </c>
@@ -3113,7 +3088,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="31" spans="1:5" ht="34" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:5" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A31" s="15" t="s">
         <v>140</v>
       </c>
@@ -3130,7 +3105,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="32" spans="1:5" ht="34" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:5" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A32" s="15" t="s">
         <v>149</v>
       </c>
@@ -3147,7 +3122,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="33" spans="1:5" ht="51" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:5" ht="47.25" x14ac:dyDescent="0.2">
       <c r="A33" s="15" t="s">
         <v>150</v>
       </c>
@@ -3179,47 +3154,47 @@
       <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.83203125" style="2"/>
+    <col min="1" max="1" width="10.875" style="2"/>
     <col min="2" max="2" width="9.5" customWidth="1"/>
-    <col min="3" max="3" width="15.83203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.33203125" customWidth="1"/>
-    <col min="5" max="5" width="6.83203125" customWidth="1"/>
+    <col min="3" max="3" width="15.875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.375" customWidth="1"/>
+    <col min="5" max="5" width="6.875" customWidth="1"/>
     <col min="6" max="6" width="12.5" style="7" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="14" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
         <v>156</v>
       </c>
@@ -3242,7 +3217,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>157</v>
       </c>
@@ -3258,7 +3233,7 @@
       <c r="F15" s="10"/>
       <c r="G15" s="7"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>158</v>
       </c>
@@ -3283,7 +3258,7 @@
         <v>125.00000000000001</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
         <v>159</v>
       </c>
@@ -3308,7 +3283,7 @@
         <v>102.22222222222223</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
         <v>160</v>
       </c>
@@ -3333,7 +3308,7 @@
         <v>97.5</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
         <v>161</v>
       </c>
@@ -3373,17 +3348,17 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.83203125" style="2"/>
-    <col min="2" max="2" width="16.6640625" customWidth="1"/>
+    <col min="1" max="1" width="10.875" style="2"/>
+    <col min="2" max="2" width="16.625" customWidth="1"/>
     <col min="3" max="3" width="14.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.1640625" customWidth="1"/>
-    <col min="5" max="5" width="6.83203125" customWidth="1"/>
+    <col min="4" max="4" width="7.125" customWidth="1"/>
+    <col min="5" max="5" width="6.875" customWidth="1"/>
     <col min="6" max="6" width="12.5" style="7" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -3403,7 +3378,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="2">
         <v>42044</v>
       </c>
@@ -3414,7 +3389,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="2">
         <v>42058</v>
       </c>
@@ -3436,7 +3411,7 @@
         <v>44.186046511627907</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
         <v>42079</v>
       </c>
@@ -3457,7 +3432,7 @@
         <v>11.733333333333333</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
         <v>42093</v>
       </c>
@@ -3478,7 +3453,7 @@
         <v>18.176470588235293</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="2">
         <v>42107</v>
       </c>
@@ -3499,28 +3474,28 @@
       <selection activeCell="B13" sqref="B13:B22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="9" style="15" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="24.5" style="17" customWidth="1"/>
-    <col min="3" max="3" width="7.33203125" style="15" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.6640625" style="15" customWidth="1"/>
+    <col min="3" max="3" width="7.375" style="15" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.625" style="15" customWidth="1"/>
     <col min="5" max="5" width="8.5" style="15" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.33203125" style="15" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.6640625" style="15" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.33203125" style="15" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.375" style="15" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.625" style="15" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.375" style="15" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="11" style="25" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="20.83203125" style="28" customWidth="1"/>
-    <col min="11" max="11" width="17.83203125" style="28" customWidth="1"/>
+    <col min="10" max="10" width="20.875" style="28" customWidth="1"/>
+    <col min="11" max="11" width="17.875" style="28" customWidth="1"/>
     <col min="12" max="12" width="13" style="23" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="1.83203125" style="23" customWidth="1"/>
-    <col min="14" max="14" width="16.83203125" style="28" customWidth="1"/>
-    <col min="15" max="15" width="22.83203125" style="28" customWidth="1"/>
-    <col min="16" max="16" width="10.1640625" style="23" bestFit="1" customWidth="1"/>
-    <col min="17" max="16384" width="10.83203125" style="15"/>
+    <col min="13" max="13" width="1.875" style="23" customWidth="1"/>
+    <col min="14" max="14" width="16.875" style="28" customWidth="1"/>
+    <col min="15" max="15" width="22.875" style="28" customWidth="1"/>
+    <col min="16" max="16" width="10.125" style="23" bestFit="1" customWidth="1"/>
+    <col min="17" max="16384" width="10.875" style="15"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="14" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A1" s="14" t="s">
         <v>9</v>
       </c>
@@ -3567,7 +3542,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="2" spans="1:16" ht="28" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:16" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A2" s="15" t="s">
         <v>109</v>
       </c>
@@ -3614,7 +3589,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:16" ht="28" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:16" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A3" s="15" t="s">
         <v>110</v>
       </c>
@@ -3661,7 +3636,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:16" ht="28" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:16" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A4" s="15" t="s">
         <v>111</v>
       </c>
@@ -3708,7 +3683,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="5" spans="1:16" ht="28" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:16" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A5" s="15" t="s">
         <v>112</v>
       </c>
@@ -3755,7 +3730,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="6" spans="1:16" ht="28" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:16" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A6" s="15" t="s">
         <v>113</v>
       </c>
@@ -3802,7 +3777,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:16" ht="28" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:16" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A7" s="15" t="s">
         <v>114</v>
       </c>
@@ -3849,7 +3824,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:16" ht="42" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:16" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A8" s="15" t="s">
         <v>118</v>
       </c>
@@ -3896,7 +3871,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="9" spans="1:16" ht="28" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:16" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A9" s="15" t="s">
         <v>119</v>
       </c>
@@ -3943,7 +3918,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
       <c r="J10" s="27"/>
       <c r="K10" s="27"/>
       <c r="L10" s="26"/>
@@ -3951,43 +3926,43 @@
       <c r="O10" s="27"/>
       <c r="P10" s="26"/>
     </row>
-    <row r="13" spans="1:16" ht="14" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B13" s="19" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B14" s="29"/>
     </row>
-    <row r="15" spans="1:16" ht="14" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B15" s="30" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="16" spans="1:16" ht="24" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:16" ht="21" x14ac:dyDescent="0.2">
       <c r="B16" s="31" t="s">
         <v>230</v>
       </c>
     </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.15">
+    <row r="17" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B17" s="19"/>
     </row>
-    <row r="18" spans="2:2" ht="14" x14ac:dyDescent="0.15">
+    <row r="18" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B18" s="30" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="19" spans="2:2" ht="72" x14ac:dyDescent="0.15">
+    <row r="19" spans="2:2" ht="73.5" x14ac:dyDescent="0.2">
       <c r="B19" s="31" t="s">
         <v>229</v>
       </c>
     </row>
-    <row r="21" spans="2:2" ht="14" x14ac:dyDescent="0.15">
+    <row r="21" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B21" s="30" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="22" spans="2:2" x14ac:dyDescent="0.15">
+    <row r="22" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B22" s="31" t="s">
         <v>231</v>
       </c>
@@ -4007,21 +3982,21 @@
       <selection activeCell="L2" sqref="L2:L9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.83203125" style="32"/>
+    <col min="1" max="1" width="10.875" style="32"/>
     <col min="2" max="2" width="22" style="32" bestFit="1" customWidth="1"/>
-    <col min="3" max="9" width="10.83203125" style="32"/>
-    <col min="10" max="10" width="13.83203125" style="32" customWidth="1"/>
+    <col min="3" max="9" width="10.875" style="32"/>
+    <col min="10" max="10" width="13.875" style="32" customWidth="1"/>
     <col min="11" max="11" width="16" style="32" customWidth="1"/>
-    <col min="12" max="12" width="15.83203125" style="32" customWidth="1"/>
-    <col min="13" max="13" width="4.1640625" style="32" customWidth="1"/>
-    <col min="14" max="14" width="10.83203125" style="32" customWidth="1"/>
-    <col min="15" max="15" width="15.33203125" style="32" customWidth="1"/>
-    <col min="16" max="16384" width="10.83203125" style="32"/>
+    <col min="12" max="12" width="15.875" style="32" customWidth="1"/>
+    <col min="13" max="13" width="4.125" style="32" customWidth="1"/>
+    <col min="14" max="14" width="10.875" style="32" customWidth="1"/>
+    <col min="15" max="15" width="15.375" style="32" customWidth="1"/>
+    <col min="16" max="16384" width="10.875" style="32"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="33" t="s">
         <v>9</v>
       </c>
@@ -4069,7 +4044,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="2" spans="1:16" s="36" customFormat="1" ht="84" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:16" s="36" customFormat="1" ht="76.5" x14ac:dyDescent="0.2">
       <c r="A2" s="36" t="s">
         <v>115</v>
       </c>
@@ -4116,7 +4091,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="3" spans="1:16" s="36" customFormat="1" ht="98" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:16" s="36" customFormat="1" ht="89.25" x14ac:dyDescent="0.2">
       <c r="A3" s="36" t="s">
         <v>116</v>
       </c>
@@ -4163,7 +4138,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="4" spans="1:16" s="36" customFormat="1" ht="42" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:16" s="36" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A4" s="36" t="s">
         <v>117</v>
       </c>
@@ -4210,7 +4185,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:16" s="36" customFormat="1" ht="28" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:16" s="36" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A5" s="36" t="s">
         <v>120</v>
       </c>
@@ -4257,7 +4232,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:16" s="36" customFormat="1" ht="28" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:16" s="36" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A6" s="36" t="s">
         <v>121</v>
       </c>
@@ -4304,7 +4279,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:16" s="36" customFormat="1" ht="42" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:16" s="36" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A7" s="36" t="s">
         <v>122</v>
       </c>
@@ -4351,7 +4326,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="8" spans="1:16" s="36" customFormat="1" ht="28" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:16" s="36" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A8" s="36" t="s">
         <v>149</v>
       </c>
@@ -4398,7 +4373,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:16" s="36" customFormat="1" ht="28" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:16" s="36" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A9" s="36" t="s">
         <v>150</v>
       </c>
@@ -4445,50 +4420,50 @@
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:16" s="36" customFormat="1" x14ac:dyDescent="0.15"/>
-    <row r="11" spans="1:16" s="36" customFormat="1" x14ac:dyDescent="0.15"/>
-    <row r="12" spans="1:16" s="36" customFormat="1" x14ac:dyDescent="0.15"/>
-    <row r="13" spans="1:16" s="36" customFormat="1" x14ac:dyDescent="0.15"/>
-    <row r="14" spans="1:16" s="36" customFormat="1" ht="14" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:16" s="36" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="11" spans="1:16" s="36" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="12" spans="1:16" s="36" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="13" spans="1:16" s="36" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="14" spans="1:16" s="36" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B14" s="19" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="15" spans="1:16" s="36" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:16" s="36" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B15" s="29"/>
     </row>
-    <row r="16" spans="1:16" s="36" customFormat="1" ht="28" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:16" s="36" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="B16" s="30" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="17" spans="2:2" s="36" customFormat="1" ht="24" x14ac:dyDescent="0.15">
+    <row r="17" spans="2:2" s="36" customFormat="1" ht="31.5" x14ac:dyDescent="0.2">
       <c r="B17" s="31" t="s">
         <v>262</v>
       </c>
     </row>
-    <row r="18" spans="2:2" s="36" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="18" spans="2:2" s="36" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B18" s="19"/>
     </row>
-    <row r="19" spans="2:2" s="36" customFormat="1" ht="28" x14ac:dyDescent="0.15">
+    <row r="19" spans="2:2" s="36" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B19" s="30" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="20" spans="2:2" s="36" customFormat="1" ht="72" x14ac:dyDescent="0.15">
+    <row r="20" spans="2:2" s="36" customFormat="1" ht="63" x14ac:dyDescent="0.2">
       <c r="B20" s="31" t="s">
         <v>263</v>
       </c>
     </row>
-    <row r="21" spans="2:2" x14ac:dyDescent="0.15">
+    <row r="21" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B21" s="17"/>
     </row>
-    <row r="22" spans="2:2" ht="14" x14ac:dyDescent="0.15">
+    <row r="22" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B22" s="30" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="23" spans="2:2" ht="36" x14ac:dyDescent="0.15">
+    <row r="23" spans="2:2" ht="31.5" x14ac:dyDescent="0.2">
       <c r="B23" s="31" t="s">
         <v>261</v>
       </c>
@@ -4508,17 +4483,17 @@
       <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.83203125" style="32"/>
+    <col min="1" max="1" width="10.875" style="32"/>
     <col min="2" max="2" width="23" style="32" bestFit="1" customWidth="1"/>
-    <col min="3" max="10" width="10.83203125" style="32"/>
-    <col min="11" max="11" width="14.83203125" style="32" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.83203125" style="32" bestFit="1" customWidth="1"/>
-    <col min="13" max="16384" width="10.83203125" style="32"/>
+    <col min="3" max="10" width="10.875" style="32"/>
+    <col min="11" max="11" width="14.875" style="32" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.875" style="32" bestFit="1" customWidth="1"/>
+    <col min="13" max="16384" width="10.875" style="32"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="33" t="s">
         <v>3</v>
       </c>
@@ -4566,7 +4541,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="2" spans="1:16" ht="84" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:16" ht="63.75" x14ac:dyDescent="0.2">
       <c r="A2" s="32" t="s">
         <v>123</v>
       </c>
@@ -4613,7 +4588,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="3" spans="1:16" ht="28" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:16" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A3" s="32" t="s">
         <v>124</v>
       </c>
@@ -4660,7 +4635,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="4" spans="1:16" ht="56" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:16" ht="51" x14ac:dyDescent="0.2">
       <c r="A4" s="32" t="s">
         <v>125</v>
       </c>
@@ -4707,7 +4682,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="5" spans="1:16" ht="42" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:16" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A5" s="32" t="s">
         <v>126</v>
       </c>
@@ -4754,7 +4729,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="6" spans="1:16" ht="42" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:16" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A6" s="32" t="s">
         <v>136</v>
       </c>
@@ -4801,7 +4776,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="7" spans="1:16" ht="224" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:16" ht="204" x14ac:dyDescent="0.2">
       <c r="A7" s="32" t="s">
         <v>138</v>
       </c>
@@ -4848,7 +4823,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="8" spans="1:16" ht="224" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:16" ht="204" x14ac:dyDescent="0.2">
       <c r="A8" s="32" t="s">
         <v>139</v>
       </c>
@@ -4895,7 +4870,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="9" spans="1:16" ht="42" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:16" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A9" s="32" t="s">
         <v>140</v>
       </c>
@@ -4942,46 +4917,46 @@
         <v>41</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B13" s="41" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B14" s="42"/>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B15" s="43" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="16" spans="1:16" ht="52" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:16" ht="45" x14ac:dyDescent="0.2">
       <c r="B16" s="42" t="s">
         <v>290</v>
       </c>
     </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.15">
+    <row r="17" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B17" s="41"/>
     </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.15">
+    <row r="18" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B18" s="43" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="19" spans="2:2" ht="65" x14ac:dyDescent="0.15">
+    <row r="19" spans="2:2" ht="67.5" x14ac:dyDescent="0.2">
       <c r="B19" s="42" t="s">
         <v>291</v>
       </c>
     </row>
-    <row r="20" spans="2:2" x14ac:dyDescent="0.15">
+    <row r="20" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B20" s="42"/>
     </row>
-    <row r="21" spans="2:2" x14ac:dyDescent="0.15">
+    <row r="21" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B21" s="43" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="22" spans="2:2" ht="39" x14ac:dyDescent="0.15">
+    <row r="22" spans="2:2" ht="33.75" x14ac:dyDescent="0.2">
       <c r="B22" s="42" t="s">
         <v>292</v>
       </c>
@@ -4997,31 +4972,31 @@
   <dimension ref="A1:P9"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
-      <selection activeCell="Q6" sqref="Q6"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="21.33203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="21.375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="9" style="32" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="21" style="32" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="7.5" style="32" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="19.5" style="32" customWidth="1"/>
     <col min="5" max="5" width="8.5" style="32" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.33203125" style="32" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.6640625" style="32" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.375" style="32" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.625" style="32" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="9.5" style="32" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.33203125" style="32" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.375" style="32" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="11.5" style="32" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="16.5" style="32" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="13" style="32" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="21.33203125" style="32"/>
-    <col min="14" max="14" width="18.1640625" style="32" customWidth="1"/>
+    <col min="13" max="13" width="21.375" style="32"/>
+    <col min="14" max="14" width="18.125" style="32" customWidth="1"/>
     <col min="15" max="15" width="14" style="32" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="10.1640625" style="32" bestFit="1" customWidth="1"/>
-    <col min="17" max="16384" width="21.33203125" style="32"/>
+    <col min="16" max="16" width="10.125" style="32" bestFit="1" customWidth="1"/>
+    <col min="17" max="16384" width="21.375" style="32"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="33" t="s">
         <v>3</v>
       </c>
@@ -5069,7 +5044,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="2" spans="1:16" ht="42" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:16" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A2" s="32" t="s">
         <v>127</v>
       </c>
@@ -5116,7 +5091,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:16" ht="42" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:16" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A3" s="32" t="s">
         <v>128</v>
       </c>
@@ -5163,7 +5138,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:16" ht="14" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A4" s="32" t="s">
         <v>130</v>
       </c>
@@ -5183,7 +5158,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="5" spans="1:16" ht="126" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:16" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A5" s="32" t="s">
         <v>131</v>
       </c>
@@ -5193,44 +5168,14 @@
       <c r="C5" s="32" t="s">
         <v>183</v>
       </c>
-      <c r="D5" s="36" t="s">
-        <v>287</v>
-      </c>
       <c r="E5" s="32">
         <v>25</v>
       </c>
       <c r="F5" s="32">
         <v>1</v>
       </c>
-      <c r="G5" s="32">
-        <v>22</v>
-      </c>
-      <c r="H5" s="32">
-        <v>1</v>
-      </c>
-      <c r="I5" s="39">
-        <v>42096</v>
-      </c>
-      <c r="J5" s="36" t="s">
-        <v>304</v>
-      </c>
-      <c r="K5" s="36" t="s">
-        <v>305</v>
-      </c>
-      <c r="L5" s="32">
-        <v>18</v>
-      </c>
-      <c r="N5" s="36" t="s">
-        <v>306</v>
-      </c>
-      <c r="O5" s="36" t="s">
-        <v>307</v>
-      </c>
-      <c r="P5" s="32">
-        <v>439</v>
-      </c>
-    </row>
-    <row r="6" spans="1:16" ht="126" x14ac:dyDescent="0.15">
+    </row>
+    <row r="6" spans="1:16" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A6" s="32" t="s">
         <v>132</v>
       </c>
@@ -5240,44 +5185,14 @@
       <c r="C6" s="32" t="s">
         <v>183</v>
       </c>
-      <c r="D6" s="36" t="s">
-        <v>287</v>
-      </c>
       <c r="E6" s="32">
         <v>35</v>
       </c>
       <c r="F6" s="32">
         <v>2</v>
       </c>
-      <c r="G6" s="32">
-        <v>32</v>
-      </c>
-      <c r="H6" s="32">
-        <v>1</v>
-      </c>
-      <c r="I6" s="39">
-        <v>42096</v>
-      </c>
-      <c r="J6" s="36" t="s">
-        <v>308</v>
-      </c>
-      <c r="K6" s="36" t="s">
-        <v>309</v>
-      </c>
-      <c r="L6" s="32">
-        <v>29</v>
-      </c>
-      <c r="N6" s="36" t="s">
-        <v>310</v>
-      </c>
-      <c r="O6" s="36" t="s">
-        <v>311</v>
-      </c>
-      <c r="P6" s="32">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="7" spans="1:16" ht="28" x14ac:dyDescent="0.15">
+    </row>
+    <row r="7" spans="1:16" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A7" s="32" t="s">
         <v>133</v>
       </c>
@@ -5324,7 +5239,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="8" spans="1:16" ht="14" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A8" s="32" t="s">
         <v>135</v>
       </c>
@@ -5344,7 +5259,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="9" spans="1:16" ht="28" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:16" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A9" s="15" t="s">
         <v>137</v>
       </c>
@@ -5406,13 +5321,13 @@
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="28.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="49.5" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="4" customFormat="1" ht="14" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>108</v>
       </c>
@@ -5423,7 +5338,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>109</v>
       </c>
@@ -5434,7 +5349,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="17" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>110</v>
       </c>
@@ -5445,7 +5360,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="17" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>111</v>
       </c>
@@ -5456,7 +5371,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>112</v>
       </c>
@@ -5467,7 +5382,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="17" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>113</v>
       </c>
@@ -5478,7 +5393,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="17" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>114</v>
       </c>
@@ -5489,7 +5404,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="51" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:3" ht="47.25" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>115</v>
       </c>
@@ -5500,7 +5415,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>116</v>
       </c>
@@ -5511,7 +5426,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>117</v>
       </c>
@@ -5522,7 +5437,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>118</v>
       </c>
@@ -5533,7 +5448,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>119</v>
       </c>
@@ -5544,7 +5459,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="51" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:3" ht="47.25" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>120</v>
       </c>
@@ -5555,7 +5470,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="68" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:3" ht="63" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>121</v>
       </c>
@@ -5566,7 +5481,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>122</v>
       </c>
@@ -5577,7 +5492,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="17" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>123</v>
       </c>
@@ -5588,7 +5503,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>124</v>
       </c>
@@ -5599,7 +5514,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="17" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>125</v>
       </c>
@@ -5610,7 +5525,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="17" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>126</v>
       </c>
@@ -5621,7 +5536,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="17" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>127</v>
       </c>
@@ -5632,7 +5547,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>128</v>
       </c>
@@ -5643,7 +5558,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>129</v>
       </c>
@@ -5654,7 +5569,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>130</v>
       </c>
@@ -5665,7 +5580,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>131</v>
       </c>
@@ -5676,7 +5591,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="51" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:3" ht="47.25" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>132</v>
       </c>
@@ -5687,7 +5602,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>133</v>
       </c>
@@ -5698,7 +5613,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="136" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:3" ht="126" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>134</v>
       </c>
@@ -5709,7 +5624,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>135</v>
       </c>
@@ -5720,7 +5635,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>136</v>
       </c>
@@ -5731,7 +5646,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="30" spans="1:3" ht="17" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>137</v>
       </c>
@@ -5742,7 +5657,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="31" spans="1:3" ht="17" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>138</v>
       </c>
@@ -5753,7 +5668,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>139</v>
       </c>
@@ -5764,7 +5679,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="33" spans="1:3" ht="17" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>140</v>
       </c>
@@ -5775,7 +5690,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="34" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>141</v>
       </c>
@@ -5786,7 +5701,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="35" spans="1:3" ht="51" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:3" ht="47.25" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>142</v>
       </c>
@@ -5797,7 +5712,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="36" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>143</v>
       </c>
@@ -5808,7 +5723,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="37" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>144</v>
       </c>
@@ -5819,7 +5734,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="38" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>145</v>
       </c>
@@ -5830,7 +5745,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="39" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+    <row r="39" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>146</v>
       </c>
@@ -5841,7 +5756,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="40" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+    <row r="40" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>147</v>
       </c>
@@ -5852,7 +5767,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="41" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+    <row r="41" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>148</v>
       </c>
@@ -5863,7 +5778,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="42" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+    <row r="42" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>149</v>
       </c>
@@ -5874,7 +5789,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="43" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+    <row r="43" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>150</v>
       </c>

</xml_diff>